<commit_message>
Changes to be committed: 	modified:   Libro1.xlsx 	modified:   prueba.html 	new file:   prueba2.html 	modified:   styless/css.css 	deleted:    tatus
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>LA FRIA</t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>TOTAL DE FALLAS</t>
-  </si>
-  <si>
-    <t>MARZO</t>
   </si>
   <si>
     <t>Marzo %</t>
@@ -151,7 +148,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,12 +158,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF4EF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFAFD7FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -218,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -229,10 +220,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -274,28 +261,25 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$B$2</c:f>
+              <c:f>Hoja1!$C$1:$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Marzo %</c:v>
+                  <c:v>TOTAL DE FALLAS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$A$3:$A$38</c:f>
+              <c:f>Hoja1!$A$2:$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
@@ -411,78 +395,78 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$3:$B$38</c:f>
+              <c:f>Hoja1!$C$2:$C$37</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>0.73</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.12</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.05</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.15</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.05</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.73</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.02</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.02</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.02</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.22</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.05</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.02</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.12</c:v>
-                </c:pt>
-                <c:pt idx="26" formatCode="0%">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.05</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.05</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.05</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -495,349 +479,11 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="121504512"/>
-        <c:axId val="121521280"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="121504512"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121521280"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="121521280"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121504512"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-VE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja1!$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>TOTAL DE FALLAS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6">
-                <a:lumMod val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Hoja1!$A$3:$A$38</c:f>
-              <c:strCache>
-                <c:ptCount val="36"/>
-                <c:pt idx="0">
-                  <c:v>LA FRIA</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>BARINAS</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>PRTO. ORDAZ</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>MARACAY</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>BARCELONA</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>CIUDAD BOLIVAR</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>VALENCIA</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>PRTO. CABELLO</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>PTO. FIJO</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>LARA</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>HOSP. MLTR. SAN CRISTOBAL</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>SAN CRISTOBAL</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>MARACAIBO</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>ZULIA</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>MNRO. DE LA DEFENSA</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>ACADEMIA MILITAR</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>CANES</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>C.G GNB</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>GUARICO</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>PORTUGUESA</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>APURE</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>MIRANDA</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>MONAGAS</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>DTA. AMACURO</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>NVA. ESPARTA</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>SUCRE</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>TRUJILLO</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>MERIDA</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>YARACUY</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>COJEDES</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>AMAZONAS</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>ALTOS MIRANDINOS</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>HOSP. MLTR. DR. CARLOS AREVALO</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>RAMO VERDE</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>CARUPANO</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>CIRCULO MILITAR</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja1!$C$3:$C$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="38"/>
-                <c:pt idx="0">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="142515584"/>
-        <c:axId val="153552768"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="142515584"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153552768"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="153552768"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142515584"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
+        <c:firstSliceAng val="0"/>
+        <c:holeSize val="50"/>
+      </c:doughnutChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -860,20 +506,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>53975</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="3 Gráfico"/>
+        <xdr:cNvPr id="2" name="1 Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -883,36 +529,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>152398</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="4 Gráfico"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1211,7 +827,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,147 +836,151 @@
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.73</v>
+      </c>
+      <c r="C2" s="4">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="B3" s="5">
-        <v>0.73</v>
+        <v>0.12</v>
       </c>
       <c r="C3" s="4">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="5">
-        <v>0.12</v>
-      </c>
-      <c r="C4" s="4">
-        <v>5</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="C5" s="4">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B6" s="5">
-        <v>0.15</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C6" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="C7" s="4">
         <v>2</v>
-      </c>
-      <c r="B7" s="5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C7" s="4">
-        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" s="5">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="C8" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="C9" s="4">
         <v>4</v>
-      </c>
-      <c r="B9" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="C9" s="4">
-        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="C10" s="4">
-        <v>4</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="C12" s="4">
-        <v>2</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.73</v>
+      </c>
+      <c r="C13" s="4">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B14" s="5">
-        <v>0.73</v>
+        <v>0.02</v>
       </c>
       <c r="C14" s="4">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B15" s="5">
         <v>0.02</v>
@@ -1371,221 +991,213 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="5">
-        <v>0.02</v>
-      </c>
-      <c r="C16" s="4">
-        <v>1</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="B17" s="5"/>
       <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="B18" s="5"/>
       <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="B19" s="5"/>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" s="5">
-        <v>0.02</v>
+        <v>0.22</v>
       </c>
       <c r="C21" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22" s="5">
-        <v>0.22</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C22" s="4">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C23" s="4">
-        <v>3</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="C24" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B25" s="5">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="C25" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="5">
-        <v>0.02</v>
-      </c>
-      <c r="C26" s="4">
-        <v>1</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="4"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="B27" s="5">
+        <v>0.12</v>
+      </c>
+      <c r="C27" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B28" s="5">
-        <v>0.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C28" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" s="6">
-        <v>7.0000000000000007E-2</v>
+        <v>26</v>
+      </c>
+      <c r="B29" s="5">
+        <v>0.05</v>
       </c>
       <c r="C29" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B30" s="5">
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C30" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B31" s="5">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="C31" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="C32" s="4">
-        <v>2</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="4"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="B33" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="C33" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="C34" s="4">
-        <v>2</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="B35" s="5"/>
       <c r="C35" s="4"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="B36" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="C36" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="C37" s="4">
-        <v>4</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="4"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
+      <c r="C38">
+        <f>SUM(C2:C37)</f>
+        <v>128</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Changes to be committed: 	modified:   Libro1.xlsx 	modified:   index.html 	deleted:    prueba2.html 	new file:   prueba3.html 	deleted:    ~$Libro1.xlsx
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -468,6 +468,9 @@
                 <c:pt idx="34">
                   <c:v>4</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -484,6 +487,615 @@
         <c:firstSliceAng val="0"/>
         <c:holeSize val="50"/>
       </c:doughnutChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-VE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Marzo %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$2:$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>LA FRIA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BARINAS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>PRTO. ORDAZ</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MARACAY</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BARCELONA</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CIUDAD BOLIVAR</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>VALENCIA</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>PRTO. CABELLO</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>PTO. FIJO</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>LARA</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>HOSP. MLTR. SAN CRISTOBAL</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>SAN CRISTOBAL</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>MARACAIBO</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>ZULIA</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>MNRO. DE LA DEFENSA</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>ACADEMIA MILITAR</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>CANES</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>C.G GNB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>GUARICO</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>PORTUGUESA</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>APURE</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>MIRANDA</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>MONAGAS</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>DTA. AMACURO</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>NVA. ESPARTA</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>SUCRE</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>TRUJILLO</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>MERIDA</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>YARACUY</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>COJEDES</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>AMAZONAS</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>ALTOS MIRANDINOS</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>HOSP. MLTR. DR. CARLOS AREVALO</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>RAMO VERDE</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>CARUPANO</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>CIRCULO MILITAR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$2:$B$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="5099520"/>
+        <c:axId val="5101056"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="5099520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="5101056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="5101056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="5099520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-VE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TOTAL DE FALLAS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$2:$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>LA FRIA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BARINAS</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>PRTO. ORDAZ</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MARACAY</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BARCELONA</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CIUDAD BOLIVAR</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>VALENCIA</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>PRTO. CABELLO</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>PTO. FIJO</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>LARA</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>HOSP. MLTR. SAN CRISTOBAL</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>SAN CRISTOBAL</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>MARACAIBO</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>ZULIA</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>MNRO. DE LA DEFENSA</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>ACADEMIA MILITAR</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>CANES</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>C.G GNB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>GUARICO</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>PORTUGUESA</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>APURE</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>MIRANDA</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>MONAGAS</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>DTA. AMACURO</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>NVA. ESPARTA</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>SUCRE</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>TRUJILLO</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>MERIDA</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>YARACUY</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>COJEDES</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>AMAZONAS</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>ALTOS MIRANDINOS</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>HOSP. MLTR. DR. CARLOS AREVALO</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>RAMO VERDE</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>CARUPANO</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>CIRCULO MILITAR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$C$2:$C$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>133</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="6674304"/>
+        <c:axId val="6675840"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="6674304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="6675840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="6675840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="6674304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -529,6 +1141,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="5 Gráfico"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95248</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="6 Gráfico"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1189,12 +1865,14 @@
         <v>34</v>
       </c>
       <c r="B37" s="5"/>
-      <c r="C37" s="4"/>
+      <c r="C37" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C38">
         <f>SUM(C2:C37)</f>
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to be committed: 	modified:   Libro1.xlsx 	modified:   index.html 	modified:   meses/abril.html 	modified:   meses/enero.html 	modified:   src/charts3.js
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="340">
   <si>
     <t>LA FRIA</t>
   </si>
@@ -997,6 +997,45 @@
   </si>
   <si>
     <t>10:08</t>
+  </si>
+  <si>
+    <t>10:09</t>
+  </si>
+  <si>
+    <t>BANFA-9896</t>
+  </si>
+  <si>
+    <t>1208</t>
+  </si>
+  <si>
+    <t>031</t>
+  </si>
+  <si>
+    <t>BANFA-9897</t>
+  </si>
+  <si>
+    <t>1209</t>
+  </si>
+  <si>
+    <t>ZODI LARA</t>
+  </si>
+  <si>
+    <t>10:11</t>
+  </si>
+  <si>
+    <t>032</t>
+  </si>
+  <si>
+    <t>BANFA-9898</t>
+  </si>
+  <si>
+    <t>1210</t>
+  </si>
+  <si>
+    <t>BANFA-9899</t>
+  </si>
+  <si>
+    <t>1211</t>
   </si>
 </sst>
 </file>
@@ -1678,7 +1717,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -2084,6 +2123,17 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -10958,7 +11008,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -10968,6 +11017,7 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8704">
     <cellStyle name="20% - Énfasis1 1" xfId="3"/>
@@ -20197,11 +20247,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="182617216"/>
-        <c:axId val="182618752"/>
+        <c:axId val="193213568"/>
+        <c:axId val="193215104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="182617216"/>
+        <c:axId val="193213568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20210,7 +20260,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182618752"/>
+        <c:crossAx val="193215104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20218,7 +20268,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182618752"/>
+        <c:axId val="193215104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20229,7 +20279,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182617216"/>
+        <c:crossAx val="193213568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20506,11 +20556,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="183118464"/>
-        <c:axId val="183120256"/>
+        <c:axId val="193260160"/>
+        <c:axId val="195625344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="183118464"/>
+        <c:axId val="193260160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20519,7 +20569,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183120256"/>
+        <c:crossAx val="195625344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20527,7 +20577,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="183120256"/>
+        <c:axId val="195625344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20538,7 +20588,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183118464"/>
+        <c:crossAx val="193260160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21329,10 +21379,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N200"/>
+  <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -21739,8 +21789,8 @@
         <v>7</v>
       </c>
       <c r="N11" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "LARA")</f>
-        <v>0</v>
+        <f>COUNTIFS(A131:A204,A201,D131:D204, D204)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75">
@@ -22099,8 +22149,8 @@
         <v>18</v>
       </c>
       <c r="N21" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, D91)</f>
-        <v>1</v>
+        <f>COUNTIFS(A131:A202,A200,D131:D202, D201)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75">
@@ -22459,8 +22509,8 @@
         <v>28</v>
       </c>
       <c r="N31" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "COJEDES")</f>
-        <v>0</v>
+        <f>COUNTIFS(A131:A204,A202,D131:D204, D203)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75">
@@ -22707,9 +22757,9 @@
       <c r="I38" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="N38">
+      <c r="N38" s="59">
         <f>SUM(N2:N37)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="31.5">
@@ -22972,8 +23022,6 @@
       <c r="I47" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="M47" s="3"/>
-      <c r="N47" s="1"/>
     </row>
     <row r="48" spans="1:14" ht="15.75">
       <c r="A48" s="13" t="s">
@@ -23003,10 +23051,8 @@
       <c r="I48" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="M48" s="56"/>
-      <c r="N48" s="56"/>
     </row>
-    <row r="49" spans="1:14" ht="15.75">
+    <row r="49" spans="1:9" ht="15.75">
       <c r="A49" s="13" t="s">
         <v>227</v>
       </c>
@@ -23034,10 +23080,8 @@
       <c r="I49" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="M49" s="56"/>
-      <c r="N49" s="56"/>
     </row>
-    <row r="50" spans="1:14" ht="15.75">
+    <row r="50" spans="1:9" ht="15.75">
       <c r="A50" s="13" t="s">
         <v>228</v>
       </c>
@@ -23061,10 +23105,8 @@
       </c>
       <c r="H50" s="22"/>
       <c r="I50" s="16"/>
-      <c r="M50" s="56"/>
-      <c r="N50" s="56"/>
     </row>
-    <row r="51" spans="1:14" ht="15.75">
+    <row r="51" spans="1:9" ht="15.75">
       <c r="A51" s="13" t="s">
         <v>228</v>
       </c>
@@ -23092,10 +23134,8 @@
       <c r="I51" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="M51" s="56"/>
-      <c r="N51" s="56"/>
     </row>
-    <row r="52" spans="1:14" ht="31.5">
+    <row r="52" spans="1:9" ht="31.5">
       <c r="A52" s="13" t="s">
         <v>228</v>
       </c>
@@ -23123,10 +23163,8 @@
       <c r="I52" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="M52" s="56"/>
-      <c r="N52" s="56"/>
     </row>
-    <row r="53" spans="1:14" ht="15.75">
+    <row r="53" spans="1:9" ht="15.75">
       <c r="A53" s="13" t="s">
         <v>228</v>
       </c>
@@ -23154,10 +23192,8 @@
       <c r="I53" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="M53" s="56"/>
-      <c r="N53" s="56"/>
     </row>
-    <row r="54" spans="1:14" ht="15.75">
+    <row r="54" spans="1:9" ht="15.75">
       <c r="A54" s="13" t="s">
         <v>228</v>
       </c>
@@ -23185,10 +23221,8 @@
       <c r="I54" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="M54" s="56"/>
-      <c r="N54" s="56"/>
     </row>
-    <row r="55" spans="1:14" ht="15.75">
+    <row r="55" spans="1:9" ht="15.75">
       <c r="A55" s="13" t="s">
         <v>228</v>
       </c>
@@ -23216,10 +23250,8 @@
       <c r="I55" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="M55" s="56"/>
-      <c r="N55" s="56"/>
     </row>
-    <row r="56" spans="1:14" ht="15.75">
+    <row r="56" spans="1:9" ht="15.75">
       <c r="A56" s="13" t="s">
         <v>229</v>
       </c>
@@ -23247,10 +23279,8 @@
       <c r="I56" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="M56" s="56"/>
-      <c r="N56" s="56"/>
     </row>
-    <row r="57" spans="1:14" ht="15.75">
+    <row r="57" spans="1:9" ht="15.75">
       <c r="A57" s="13" t="s">
         <v>229</v>
       </c>
@@ -23278,10 +23308,8 @@
       <c r="I57" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="M57" s="56"/>
-      <c r="N57" s="56"/>
     </row>
-    <row r="58" spans="1:14" ht="15.75">
+    <row r="58" spans="1:9" ht="15.75">
       <c r="A58" s="13" t="s">
         <v>229</v>
       </c>
@@ -23309,10 +23337,8 @@
       <c r="I58" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="M58" s="56"/>
-      <c r="N58" s="56"/>
     </row>
-    <row r="59" spans="1:14" ht="15.75">
+    <row r="59" spans="1:9" ht="15.75">
       <c r="A59" s="13" t="s">
         <v>229</v>
       </c>
@@ -23340,10 +23366,8 @@
       <c r="I59" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="M59" s="56"/>
-      <c r="N59" s="56"/>
     </row>
-    <row r="60" spans="1:14" ht="15.75">
+    <row r="60" spans="1:9" ht="15.75">
       <c r="A60" s="13" t="s">
         <v>229</v>
       </c>
@@ -23371,10 +23395,8 @@
       <c r="I60" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="M60" s="56"/>
-      <c r="N60" s="56"/>
     </row>
-    <row r="61" spans="1:14" ht="15.75">
+    <row r="61" spans="1:9" ht="15.75">
       <c r="A61" s="13" t="s">
         <v>229</v>
       </c>
@@ -23402,10 +23424,8 @@
       <c r="I61" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="M61" s="56"/>
-      <c r="N61" s="56"/>
     </row>
-    <row r="62" spans="1:14" ht="15.75">
+    <row r="62" spans="1:9" ht="15.75">
       <c r="A62" s="13" t="s">
         <v>230</v>
       </c>
@@ -23433,10 +23453,8 @@
       <c r="I62" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="M62" s="56"/>
-      <c r="N62" s="56"/>
     </row>
-    <row r="63" spans="1:14" ht="15.75">
+    <row r="63" spans="1:9" ht="15.75">
       <c r="A63" s="13" t="s">
         <v>230</v>
       </c>
@@ -23464,10 +23482,8 @@
       <c r="I63" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="M63" s="56"/>
-      <c r="N63" s="56"/>
     </row>
-    <row r="64" spans="1:14" ht="15.75">
+    <row r="64" spans="1:9" ht="15.75">
       <c r="A64" s="13" t="s">
         <v>230</v>
       </c>
@@ -23495,10 +23511,8 @@
       <c r="I64" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="M64" s="56"/>
-      <c r="N64" s="56"/>
     </row>
-    <row r="65" spans="1:14" ht="15.75">
+    <row r="65" spans="1:9" ht="15.75">
       <c r="A65" s="13" t="s">
         <v>230</v>
       </c>
@@ -23526,10 +23540,8 @@
       <c r="I65" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="M65" s="56"/>
-      <c r="N65" s="56"/>
     </row>
-    <row r="66" spans="1:14" ht="15.75">
+    <row r="66" spans="1:9" ht="15.75">
       <c r="A66" s="13" t="s">
         <v>230</v>
       </c>
@@ -23557,10 +23569,8 @@
       <c r="I66" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="M66" s="56"/>
-      <c r="N66" s="56"/>
     </row>
-    <row r="67" spans="1:14" ht="15.75">
+    <row r="67" spans="1:9" ht="15.75">
       <c r="A67" s="13" t="s">
         <v>231</v>
       </c>
@@ -23588,10 +23598,8 @@
       <c r="I67" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="M67" s="56"/>
-      <c r="N67" s="56"/>
     </row>
-    <row r="68" spans="1:14" ht="15.75">
+    <row r="68" spans="1:9" ht="15.75">
       <c r="A68" s="13" t="s">
         <v>231</v>
       </c>
@@ -23619,10 +23627,8 @@
       <c r="I68" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="M68" s="56"/>
-      <c r="N68" s="56"/>
     </row>
-    <row r="69" spans="1:14" ht="15.75">
+    <row r="69" spans="1:9" ht="15.75">
       <c r="A69" s="13" t="s">
         <v>231</v>
       </c>
@@ -23650,10 +23656,8 @@
       <c r="I69" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="M69" s="56"/>
-      <c r="N69" s="56"/>
     </row>
-    <row r="70" spans="1:14" ht="15.75">
+    <row r="70" spans="1:9" ht="15.75">
       <c r="A70" s="13" t="s">
         <v>231</v>
       </c>
@@ -23681,10 +23685,8 @@
       <c r="I70" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="M70" s="56"/>
-      <c r="N70" s="56"/>
     </row>
-    <row r="71" spans="1:14" ht="15.75">
+    <row r="71" spans="1:9" ht="15.75">
       <c r="A71" s="13" t="s">
         <v>231</v>
       </c>
@@ -23712,10 +23714,8 @@
       <c r="I71" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="M71" s="56"/>
-      <c r="N71" s="56"/>
     </row>
-    <row r="72" spans="1:14" ht="15.75">
+    <row r="72" spans="1:9" ht="15.75">
       <c r="A72" s="13" t="s">
         <v>231</v>
       </c>
@@ -23743,10 +23743,8 @@
       <c r="I72" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="M72" s="56"/>
-      <c r="N72" s="56"/>
     </row>
-    <row r="73" spans="1:14" ht="15.75">
+    <row r="73" spans="1:9" ht="15.75">
       <c r="A73" s="13" t="s">
         <v>231</v>
       </c>
@@ -23774,10 +23772,8 @@
       <c r="I73" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="M73" s="56"/>
-      <c r="N73" s="56"/>
     </row>
-    <row r="74" spans="1:14" ht="15.75">
+    <row r="74" spans="1:9" ht="15.75">
       <c r="A74" s="13" t="s">
         <v>231</v>
       </c>
@@ -23805,10 +23801,8 @@
       <c r="I74" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="M74" s="56"/>
-      <c r="N74" s="56"/>
     </row>
-    <row r="75" spans="1:14" ht="15.75">
+    <row r="75" spans="1:9" ht="15.75">
       <c r="A75" s="13" t="s">
         <v>232</v>
       </c>
@@ -23836,10 +23830,8 @@
       <c r="I75" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="M75" s="56"/>
-      <c r="N75" s="56"/>
     </row>
-    <row r="76" spans="1:14" ht="15.75">
+    <row r="76" spans="1:9" ht="15.75">
       <c r="A76" s="13" t="s">
         <v>232</v>
       </c>
@@ -23867,10 +23859,8 @@
       <c r="I76" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="M76" s="56"/>
-      <c r="N76" s="56"/>
     </row>
-    <row r="77" spans="1:14" ht="15.75">
+    <row r="77" spans="1:9" ht="15.75">
       <c r="A77" s="13" t="s">
         <v>232</v>
       </c>
@@ -23898,10 +23888,8 @@
       <c r="I77" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="M77" s="56"/>
-      <c r="N77" s="56"/>
     </row>
-    <row r="78" spans="1:14" ht="15.75">
+    <row r="78" spans="1:9" ht="15.75">
       <c r="A78" s="13" t="s">
         <v>232</v>
       </c>
@@ -23929,10 +23917,8 @@
       <c r="I78" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="M78" s="56"/>
-      <c r="N78" s="56"/>
     </row>
-    <row r="79" spans="1:14" ht="15.75">
+    <row r="79" spans="1:9" ht="15.75">
       <c r="A79" s="13" t="s">
         <v>232</v>
       </c>
@@ -23960,10 +23946,8 @@
       <c r="I79" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="M79" s="56"/>
-      <c r="N79" s="56"/>
     </row>
-    <row r="80" spans="1:14" ht="15.75">
+    <row r="80" spans="1:9" ht="15.75">
       <c r="A80" s="13" t="s">
         <v>232</v>
       </c>
@@ -23991,10 +23975,8 @@
       <c r="I80" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="M80" s="56"/>
-      <c r="N80" s="56"/>
     </row>
-    <row r="81" spans="1:14" ht="15.75">
+    <row r="81" spans="1:9" ht="15.75">
       <c r="A81" s="13" t="s">
         <v>232</v>
       </c>
@@ -24022,10 +24004,8 @@
       <c r="I81" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="M81" s="56"/>
-      <c r="N81" s="56"/>
     </row>
-    <row r="82" spans="1:14" ht="15.75">
+    <row r="82" spans="1:9" ht="15.75">
       <c r="A82" s="13" t="s">
         <v>232</v>
       </c>
@@ -24053,10 +24033,8 @@
       <c r="I82" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="M82" s="56"/>
-      <c r="N82" s="56"/>
     </row>
-    <row r="83" spans="1:14" ht="15.75">
+    <row r="83" spans="1:9" ht="15.75">
       <c r="A83" s="13" t="s">
         <v>232</v>
       </c>
@@ -24084,10 +24062,8 @@
       <c r="I83" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="M83" s="56"/>
-      <c r="N83" s="56"/>
     </row>
-    <row r="84" spans="1:14" ht="15.75">
+    <row r="84" spans="1:9" ht="15.75">
       <c r="A84" s="13" t="s">
         <v>233</v>
       </c>
@@ -24116,7 +24092,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="15.75">
+    <row r="85" spans="1:9" ht="15.75">
       <c r="A85" s="13" t="s">
         <v>233</v>
       </c>
@@ -24145,7 +24121,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="15.75">
+    <row r="86" spans="1:9" ht="15.75">
       <c r="A86" s="13" t="s">
         <v>233</v>
       </c>
@@ -24174,7 +24150,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="15.75">
+    <row r="87" spans="1:9" ht="15.75">
       <c r="A87" s="13" t="s">
         <v>233</v>
       </c>
@@ -24203,7 +24179,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="15.75">
+    <row r="88" spans="1:9" ht="15.75">
       <c r="A88" s="13" t="s">
         <v>233</v>
       </c>
@@ -24232,7 +24208,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="15.75">
+    <row r="89" spans="1:9" ht="15.75">
       <c r="A89" s="13" t="s">
         <v>233</v>
       </c>
@@ -24261,7 +24237,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="15.75">
+    <row r="90" spans="1:9" ht="15.75">
       <c r="A90" s="13" t="s">
         <v>233</v>
       </c>
@@ -24290,7 +24266,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="15.75">
+    <row r="91" spans="1:9" ht="15.75">
       <c r="A91" s="13" t="s">
         <v>234</v>
       </c>
@@ -24319,7 +24295,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="15.75">
+    <row r="92" spans="1:9" ht="15.75">
       <c r="A92" s="13" t="s">
         <v>234</v>
       </c>
@@ -24348,7 +24324,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="15.75">
+    <row r="93" spans="1:9" ht="15.75">
       <c r="A93" s="13" t="s">
         <v>234</v>
       </c>
@@ -24377,7 +24353,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="15.75">
+    <row r="94" spans="1:9" ht="15.75">
       <c r="A94" s="13" t="s">
         <v>234</v>
       </c>
@@ -24406,7 +24382,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="15.75">
+    <row r="95" spans="1:9" ht="15.75">
       <c r="A95" s="13" t="s">
         <v>234</v>
       </c>
@@ -24435,7 +24411,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="15.75">
+    <row r="96" spans="1:9" ht="15.75">
       <c r="A96" s="13" t="s">
         <v>234</v>
       </c>
@@ -25447,1745 +25423,1845 @@
       </c>
     </row>
     <row r="131" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A131" s="59" t="s">
+      <c r="A131" s="58" t="s">
         <v>248</v>
       </c>
-      <c r="B131" s="57" t="s">
+      <c r="B131" s="56" t="s">
         <v>249</v>
       </c>
-      <c r="C131" s="57" t="s">
+      <c r="C131" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D131" s="57" t="s">
+      <c r="D131" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E131" s="57" t="s">
+      <c r="E131" s="56" t="s">
         <v>176</v>
       </c>
-      <c r="F131" s="57" t="s">
+      <c r="F131" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="G131" s="57"/>
-      <c r="H131" s="57"/>
-      <c r="I131" s="57" t="s">
+      <c r="G131" s="56"/>
+      <c r="H131" s="56"/>
+      <c r="I131" s="56" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A132" s="59" t="s">
+      <c r="A132" s="58" t="s">
         <v>248</v>
       </c>
-      <c r="B132" s="57" t="s">
+      <c r="B132" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="C132" s="57" t="s">
+      <c r="C132" s="56" t="s">
         <v>184</v>
       </c>
-      <c r="D132" s="57" t="s">
+      <c r="D132" s="56" t="s">
         <v>185</v>
       </c>
-      <c r="E132" s="57" t="s">
+      <c r="E132" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="F132" s="57" t="s">
+      <c r="F132" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="G132" s="57"/>
-      <c r="H132" s="57"/>
-      <c r="I132" s="58" t="s">
+      <c r="G132" s="56"/>
+      <c r="H132" s="56"/>
+      <c r="I132" s="57" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="15.75">
-      <c r="A133" s="59" t="s">
+      <c r="A133" s="58" t="s">
         <v>252</v>
       </c>
-      <c r="B133" s="57" t="s">
+      <c r="B133" s="56" t="s">
         <v>191</v>
       </c>
-      <c r="C133" s="57" t="s">
+      <c r="C133" s="56" t="s">
         <v>253</v>
       </c>
-      <c r="D133" s="57" t="s">
+      <c r="D133" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="E133" s="57" t="s">
+      <c r="E133" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="F133" s="57" t="s">
+      <c r="F133" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="G133" s="57"/>
-      <c r="H133" s="57"/>
-      <c r="I133" s="57" t="s">
+      <c r="G133" s="56"/>
+      <c r="H133" s="56"/>
+      <c r="I133" s="56" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="15.75">
-      <c r="A134" s="59" t="s">
+      <c r="A134" s="58" t="s">
         <v>252</v>
       </c>
-      <c r="B134" s="57" t="s">
+      <c r="B134" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="C134" s="57" t="s">
+      <c r="C134" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D134" s="57" t="s">
+      <c r="D134" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E134" s="57" t="s">
+      <c r="E134" s="56" t="s">
         <v>176</v>
       </c>
-      <c r="F134" s="57" t="s">
+      <c r="F134" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="G134" s="57"/>
-      <c r="H134" s="57"/>
-      <c r="I134" s="57" t="s">
+      <c r="G134" s="56"/>
+      <c r="H134" s="56"/>
+      <c r="I134" s="56" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="15.75">
-      <c r="A135" s="59" t="s">
+      <c r="A135" s="58" t="s">
         <v>252</v>
       </c>
-      <c r="B135" s="57" t="s">
+      <c r="B135" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="C135" s="57" t="s">
+      <c r="C135" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="D135" s="57" t="s">
+      <c r="D135" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="E135" s="57" t="s">
+      <c r="E135" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="F135" s="57" t="s">
+      <c r="F135" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G135" s="57"/>
-      <c r="H135" s="57"/>
-      <c r="I135" s="57" t="s">
+      <c r="G135" s="56"/>
+      <c r="H135" s="56"/>
+      <c r="I135" s="56" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="15.75">
-      <c r="A136" s="59" t="s">
+      <c r="A136" s="58" t="s">
         <v>252</v>
       </c>
-      <c r="B136" s="57" t="s">
+      <c r="B136" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="C136" s="57" t="s">
+      <c r="C136" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="D136" s="57" t="s">
+      <c r="D136" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E136" s="57" t="s">
+      <c r="E136" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="F136" s="57" t="s">
+      <c r="F136" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="G136" s="57"/>
-      <c r="H136" s="57"/>
-      <c r="I136" s="57" t="s">
+      <c r="G136" s="56"/>
+      <c r="H136" s="56"/>
+      <c r="I136" s="56" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="15.75">
-      <c r="A137" s="59" t="s">
+      <c r="A137" s="58" t="s">
         <v>252</v>
       </c>
-      <c r="B137" s="57" t="s">
+      <c r="B137" s="56" t="s">
         <v>255</v>
       </c>
-      <c r="C137" s="57" t="s">
+      <c r="C137" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="D137" s="57" t="s">
+      <c r="D137" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="E137" s="57" t="s">
+      <c r="E137" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="F137" s="57" t="s">
+      <c r="F137" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="G137" s="57"/>
-      <c r="H137" s="57"/>
-      <c r="I137" s="57" t="s">
+      <c r="G137" s="56"/>
+      <c r="H137" s="56"/>
+      <c r="I137" s="56" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="15.75">
-      <c r="A138" s="59" t="s">
+      <c r="A138" s="58" t="s">
         <v>252</v>
       </c>
-      <c r="B138" s="57" t="s">
+      <c r="B138" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="C138" s="57" t="s">
+      <c r="C138" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="D138" s="57" t="s">
+      <c r="D138" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="E138" s="57" t="s">
+      <c r="E138" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="F138" s="57" t="s">
+      <c r="F138" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="G138" s="57"/>
-      <c r="H138" s="57"/>
-      <c r="I138" s="57" t="s">
+      <c r="G138" s="56"/>
+      <c r="H138" s="56"/>
+      <c r="I138" s="56" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="15.75">
-      <c r="A139" s="59" t="s">
+      <c r="A139" s="58" t="s">
         <v>252</v>
       </c>
-      <c r="B139" s="57" t="s">
+      <c r="B139" s="56" t="s">
         <v>257</v>
       </c>
-      <c r="C139" s="57" t="s">
+      <c r="C139" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="D139" s="57" t="s">
+      <c r="D139" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="E139" s="57" t="s">
+      <c r="E139" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="F139" s="57" t="s">
+      <c r="F139" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="G139" s="57"/>
-      <c r="H139" s="57"/>
-      <c r="I139" s="57" t="s">
+      <c r="G139" s="56"/>
+      <c r="H139" s="56"/>
+      <c r="I139" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="15.75">
-      <c r="A140" s="59" t="s">
+      <c r="A140" s="58" t="s">
         <v>259</v>
       </c>
-      <c r="B140" s="57" t="s">
+      <c r="B140" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="C140" s="57" t="s">
+      <c r="C140" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="D140" s="57" t="s">
+      <c r="D140" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="E140" s="57" t="s">
+      <c r="E140" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="F140" s="57" t="s">
+      <c r="F140" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="G140" s="57"/>
-      <c r="H140" s="57"/>
-      <c r="I140" s="57" t="s">
+      <c r="G140" s="56"/>
+      <c r="H140" s="56"/>
+      <c r="I140" s="56" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="141" spans="1:9" ht="15.75">
-      <c r="A141" s="59" t="s">
+      <c r="A141" s="58" t="s">
         <v>259</v>
       </c>
-      <c r="B141" s="57" t="s">
+      <c r="B141" s="56" t="s">
         <v>260</v>
       </c>
-      <c r="C141" s="57" t="s">
+      <c r="C141" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D141" s="57" t="s">
+      <c r="D141" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E141" s="57" t="s">
+      <c r="E141" s="56" t="s">
         <v>176</v>
       </c>
-      <c r="F141" s="57" t="s">
+      <c r="F141" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="G141" s="57"/>
-      <c r="H141" s="57"/>
-      <c r="I141" s="57" t="s">
+      <c r="G141" s="56"/>
+      <c r="H141" s="56"/>
+      <c r="I141" s="56" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="15.75">
-      <c r="A142" s="59" t="s">
+      <c r="A142" s="58" t="s">
         <v>259</v>
       </c>
-      <c r="B142" s="57" t="s">
+      <c r="B142" s="56" t="s">
         <v>261</v>
       </c>
-      <c r="C142" s="57" t="s">
+      <c r="C142" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="D142" s="57" t="s">
+      <c r="D142" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="E142" s="57" t="s">
+      <c r="E142" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="F142" s="57" t="s">
+      <c r="F142" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="G142" s="57"/>
-      <c r="H142" s="57"/>
-      <c r="I142" s="57" t="s">
+      <c r="G142" s="56"/>
+      <c r="H142" s="56"/>
+      <c r="I142" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="15.75">
-      <c r="A143" s="59" t="s">
+      <c r="A143" s="58" t="s">
         <v>259</v>
       </c>
-      <c r="B143" s="57" t="s">
+      <c r="B143" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="C143" s="57" t="s">
+      <c r="C143" s="56" t="s">
         <v>180</v>
       </c>
-      <c r="D143" s="57" t="s">
+      <c r="D143" s="56" t="s">
         <v>181</v>
       </c>
-      <c r="E143" s="57" t="s">
+      <c r="E143" s="56" t="s">
         <v>179</v>
       </c>
-      <c r="F143" s="57" t="s">
+      <c r="F143" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="G143" s="57"/>
-      <c r="H143" s="57"/>
-      <c r="I143" s="57" t="s">
+      <c r="G143" s="56"/>
+      <c r="H143" s="56"/>
+      <c r="I143" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="144" spans="1:9" ht="15.75">
-      <c r="A144" s="59" t="s">
+      <c r="A144" s="58" t="s">
         <v>259</v>
       </c>
-      <c r="B144" s="57" t="s">
+      <c r="B144" s="56" t="s">
         <v>154</v>
       </c>
-      <c r="C144" s="57" t="s">
+      <c r="C144" s="56" t="s">
         <v>202</v>
       </c>
-      <c r="D144" s="57" t="s">
+      <c r="D144" s="56" t="s">
         <v>203</v>
       </c>
-      <c r="E144" s="57" t="s">
+      <c r="E144" s="56" t="s">
         <v>204</v>
       </c>
-      <c r="F144" s="57" t="s">
+      <c r="F144" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="G144" s="57"/>
-      <c r="H144" s="57"/>
-      <c r="I144" s="57" t="s">
+      <c r="G144" s="56"/>
+      <c r="H144" s="56"/>
+      <c r="I144" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="15.75">
-      <c r="A145" s="59" t="s">
+      <c r="A145" s="58" t="s">
         <v>259</v>
       </c>
-      <c r="B145" s="57" t="s">
+      <c r="B145" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="C145" s="57" t="s">
+      <c r="C145" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="D145" s="57" t="s">
+      <c r="D145" s="56" t="s">
         <v>165</v>
       </c>
-      <c r="E145" s="57" t="s">
+      <c r="E145" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="F145" s="57" t="s">
+      <c r="F145" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="G145" s="57"/>
-      <c r="H145" s="57"/>
-      <c r="I145" s="57" t="s">
+      <c r="G145" s="56"/>
+      <c r="H145" s="56"/>
+      <c r="I145" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="146" spans="1:9" ht="15.75">
-      <c r="A146" s="59" t="s">
+      <c r="A146" s="58" t="s">
         <v>259</v>
       </c>
-      <c r="B146" s="57" t="s">
+      <c r="B146" s="56" t="s">
         <v>255</v>
       </c>
-      <c r="C146" s="57" t="s">
+      <c r="C146" s="56" t="s">
         <v>117</v>
       </c>
-      <c r="D146" s="57" t="s">
+      <c r="D146" s="56" t="s">
         <v>118</v>
       </c>
-      <c r="E146" s="57" t="s">
+      <c r="E146" s="56" t="s">
         <v>119</v>
       </c>
-      <c r="F146" s="57" t="s">
+      <c r="F146" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="G146" s="57"/>
-      <c r="H146" s="57"/>
-      <c r="I146" s="57" t="s">
+      <c r="G146" s="56"/>
+      <c r="H146" s="56"/>
+      <c r="I146" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="147" spans="1:9" ht="15.75">
-      <c r="A147" s="59" t="s">
+      <c r="A147" s="58" t="s">
         <v>259</v>
       </c>
-      <c r="B147" s="57" t="s">
+      <c r="B147" s="56" t="s">
         <v>262</v>
       </c>
-      <c r="C147" s="57" t="s">
+      <c r="C147" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="D147" s="57" t="s">
+      <c r="D147" s="56" t="s">
         <v>123</v>
       </c>
-      <c r="E147" s="57" t="s">
+      <c r="E147" s="56" t="s">
         <v>263</v>
       </c>
-      <c r="F147" s="57" t="s">
+      <c r="F147" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="G147" s="57"/>
-      <c r="H147" s="57"/>
-      <c r="I147" s="57" t="s">
+      <c r="G147" s="56"/>
+      <c r="H147" s="56"/>
+      <c r="I147" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="15.75">
-      <c r="A148" s="59" t="s">
+      <c r="A148" s="58" t="s">
         <v>259</v>
       </c>
-      <c r="B148" s="57" t="s">
+      <c r="B148" s="56" t="s">
         <v>264</v>
       </c>
-      <c r="C148" s="57" t="s">
+      <c r="C148" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D148" s="57" t="s">
+      <c r="D148" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E148" s="57" t="s">
+      <c r="E148" s="56" t="s">
         <v>265</v>
       </c>
-      <c r="F148" s="57" t="s">
+      <c r="F148" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G148" s="57"/>
-      <c r="H148" s="57"/>
-      <c r="I148" s="57" t="s">
+      <c r="G148" s="56"/>
+      <c r="H148" s="56"/>
+      <c r="I148" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="149" spans="1:9" ht="15.75">
-      <c r="A149" s="59" t="s">
+      <c r="A149" s="58" t="s">
         <v>259</v>
       </c>
-      <c r="B149" s="57" t="s">
+      <c r="B149" s="56" t="s">
         <v>264</v>
       </c>
-      <c r="C149" s="57" t="s">
+      <c r="C149" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="D149" s="57" t="s">
+      <c r="D149" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="E149" s="57" t="s">
+      <c r="E149" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="F149" s="57" t="s">
+      <c r="F149" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G149" s="57"/>
-      <c r="H149" s="57"/>
-      <c r="I149" s="57" t="s">
+      <c r="G149" s="56"/>
+      <c r="H149" s="56"/>
+      <c r="I149" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="150" spans="1:9" ht="15.75">
-      <c r="A150" s="59" t="s">
+      <c r="A150" s="58" t="s">
         <v>266</v>
       </c>
-      <c r="B150" s="57" t="s">
+      <c r="B150" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="C150" s="57" t="s">
+      <c r="C150" s="56" t="s">
         <v>180</v>
       </c>
-      <c r="D150" s="57" t="s">
+      <c r="D150" s="56" t="s">
         <v>181</v>
       </c>
-      <c r="E150" s="57" t="s">
+      <c r="E150" s="56" t="s">
         <v>179</v>
       </c>
-      <c r="F150" s="57" t="s">
+      <c r="F150" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="G150" s="57"/>
-      <c r="H150" s="57"/>
-      <c r="I150" s="57" t="s">
+      <c r="G150" s="56"/>
+      <c r="H150" s="56"/>
+      <c r="I150" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="15.75">
-      <c r="A151" s="59" t="s">
+      <c r="A151" s="58" t="s">
         <v>266</v>
       </c>
-      <c r="B151" s="57" t="s">
+      <c r="B151" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="C151" s="57" t="s">
+      <c r="C151" s="56" t="s">
         <v>202</v>
       </c>
-      <c r="D151" s="57" t="s">
+      <c r="D151" s="56" t="s">
         <v>203</v>
       </c>
-      <c r="E151" s="57" t="s">
+      <c r="E151" s="56" t="s">
         <v>204</v>
       </c>
-      <c r="F151" s="57" t="s">
+      <c r="F151" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="G151" s="57"/>
-      <c r="H151" s="57"/>
-      <c r="I151" s="57" t="s">
+      <c r="G151" s="56"/>
+      <c r="H151" s="56"/>
+      <c r="I151" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="15.75">
-      <c r="A152" s="59" t="s">
+      <c r="A152" s="58" t="s">
         <v>266</v>
       </c>
-      <c r="B152" s="57" t="s">
+      <c r="B152" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="C152" s="57" t="s">
+      <c r="C152" s="56" t="s">
         <v>180</v>
       </c>
-      <c r="D152" s="57" t="s">
+      <c r="D152" s="56" t="s">
         <v>181</v>
       </c>
-      <c r="E152" s="57" t="s">
+      <c r="E152" s="56" t="s">
         <v>179</v>
       </c>
-      <c r="F152" s="57" t="s">
+      <c r="F152" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="G152" s="57"/>
-      <c r="H152" s="57"/>
-      <c r="I152" s="57" t="s">
+      <c r="G152" s="56"/>
+      <c r="H152" s="56"/>
+      <c r="I152" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="153" spans="1:9" ht="15.75">
-      <c r="A153" s="59" t="s">
+      <c r="A153" s="58" t="s">
         <v>266</v>
       </c>
-      <c r="B153" s="57" t="s">
+      <c r="B153" s="56" t="s">
         <v>268</v>
       </c>
-      <c r="C153" s="57" t="s">
+      <c r="C153" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D153" s="57" t="s">
+      <c r="D153" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E153" s="57" t="s">
+      <c r="E153" s="56" t="s">
         <v>265</v>
       </c>
-      <c r="F153" s="57" t="s">
+      <c r="F153" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G153" s="57"/>
-      <c r="H153" s="57"/>
-      <c r="I153" s="57" t="s">
+      <c r="G153" s="56"/>
+      <c r="H153" s="56"/>
+      <c r="I153" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="15.75">
-      <c r="A154" s="59" t="s">
+      <c r="A154" s="58" t="s">
         <v>266</v>
       </c>
-      <c r="B154" s="57" t="s">
+      <c r="B154" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="C154" s="57" t="s">
+      <c r="C154" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="D154" s="57" t="s">
+      <c r="D154" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E154" s="57" t="s">
+      <c r="E154" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="F154" s="57" t="s">
+      <c r="F154" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="G154" s="57"/>
-      <c r="H154" s="57"/>
-      <c r="I154" s="57" t="s">
+      <c r="G154" s="56"/>
+      <c r="H154" s="56"/>
+      <c r="I154" s="56" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="155" spans="1:9" ht="15.75">
-      <c r="A155" s="59" t="s">
+      <c r="A155" s="58" t="s">
         <v>266</v>
       </c>
-      <c r="B155" s="57" t="s">
+      <c r="B155" s="56" t="s">
         <v>269</v>
       </c>
-      <c r="C155" s="57" t="s">
+      <c r="C155" s="56" t="s">
         <v>202</v>
       </c>
-      <c r="D155" s="57" t="s">
+      <c r="D155" s="56" t="s">
         <v>203</v>
       </c>
-      <c r="E155" s="57" t="s">
+      <c r="E155" s="56" t="s">
         <v>204</v>
       </c>
-      <c r="F155" s="57" t="s">
+      <c r="F155" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="G155" s="57"/>
-      <c r="H155" s="57"/>
-      <c r="I155" s="57" t="s">
+      <c r="G155" s="56"/>
+      <c r="H155" s="56"/>
+      <c r="I155" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="156" spans="1:9" ht="15.75">
-      <c r="A156" s="59" t="s">
+      <c r="A156" s="58" t="s">
         <v>266</v>
       </c>
-      <c r="B156" s="57" t="s">
+      <c r="B156" s="56" t="s">
         <v>270</v>
       </c>
-      <c r="C156" s="57" t="s">
+      <c r="C156" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D156" s="57" t="s">
+      <c r="D156" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E156" s="57" t="s">
+      <c r="E156" s="56" t="s">
         <v>265</v>
       </c>
-      <c r="F156" s="57" t="s">
+      <c r="F156" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G156" s="57"/>
-      <c r="H156" s="57"/>
-      <c r="I156" s="57" t="s">
+      <c r="G156" s="56"/>
+      <c r="H156" s="56"/>
+      <c r="I156" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="157" spans="1:9" ht="15.75">
-      <c r="A157" s="59" t="s">
+      <c r="A157" s="58" t="s">
         <v>266</v>
       </c>
-      <c r="B157" s="57" t="s">
+      <c r="B157" s="56" t="s">
         <v>271</v>
       </c>
-      <c r="C157" s="57" t="s">
+      <c r="C157" s="56" t="s">
         <v>197</v>
       </c>
-      <c r="D157" s="57" t="s">
+      <c r="D157" s="56" t="s">
         <v>198</v>
       </c>
-      <c r="E157" s="57" t="s">
+      <c r="E157" s="56" t="s">
         <v>199</v>
       </c>
-      <c r="F157" s="57" t="s">
+      <c r="F157" s="56" t="s">
         <v>200</v>
       </c>
-      <c r="G157" s="57"/>
-      <c r="H157" s="57"/>
-      <c r="I157" s="57" t="s">
+      <c r="G157" s="56"/>
+      <c r="H157" s="56"/>
+      <c r="I157" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="158" spans="1:9" ht="15.75">
-      <c r="A158" s="59" t="s">
+      <c r="A158" s="58" t="s">
         <v>272</v>
       </c>
-      <c r="B158" s="57" t="s">
+      <c r="B158" s="56" t="s">
         <v>273</v>
       </c>
-      <c r="C158" s="57" t="s">
+      <c r="C158" s="56" t="s">
         <v>202</v>
       </c>
-      <c r="D158" s="57" t="s">
+      <c r="D158" s="56" t="s">
         <v>203</v>
       </c>
-      <c r="E158" s="57" t="s">
+      <c r="E158" s="56" t="s">
         <v>204</v>
       </c>
-      <c r="F158" s="57" t="s">
+      <c r="F158" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="G158" s="57"/>
-      <c r="H158" s="57"/>
-      <c r="I158" s="57" t="s">
+      <c r="G158" s="56"/>
+      <c r="H158" s="56"/>
+      <c r="I158" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="15.75">
-      <c r="A159" s="59" t="s">
+      <c r="A159" s="58" t="s">
         <v>272</v>
       </c>
-      <c r="B159" s="57" t="s">
+      <c r="B159" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="C159" s="57" t="s">
+      <c r="C159" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D159" s="57" t="s">
+      <c r="D159" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E159" s="57" t="s">
+      <c r="E159" s="56" t="s">
         <v>265</v>
       </c>
-      <c r="F159" s="57" t="s">
+      <c r="F159" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G159" s="57"/>
-      <c r="H159" s="57"/>
-      <c r="I159" s="57" t="s">
+      <c r="G159" s="56"/>
+      <c r="H159" s="56"/>
+      <c r="I159" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="15.75">
-      <c r="A160" s="59" t="s">
+      <c r="A160" s="58" t="s">
         <v>272</v>
       </c>
-      <c r="B160" s="57" t="s">
+      <c r="B160" s="56" t="s">
         <v>274</v>
       </c>
-      <c r="C160" s="57" t="s">
+      <c r="C160" s="56" t="s">
         <v>275</v>
       </c>
-      <c r="D160" s="57" t="s">
+      <c r="D160" s="56" t="s">
         <v>276</v>
       </c>
-      <c r="E160" s="57" t="s">
+      <c r="E160" s="56" t="s">
         <v>277</v>
       </c>
-      <c r="F160" s="57" t="s">
+      <c r="F160" s="56" t="s">
         <v>164</v>
       </c>
-      <c r="G160" s="57"/>
-      <c r="H160" s="57"/>
-      <c r="I160" s="57" t="s">
+      <c r="G160" s="56"/>
+      <c r="H160" s="56"/>
+      <c r="I160" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="15.75">
-      <c r="A161" s="59" t="s">
+      <c r="A161" s="58" t="s">
         <v>278</v>
       </c>
-      <c r="B161" s="57" t="s">
+      <c r="B161" s="56" t="s">
         <v>279</v>
       </c>
-      <c r="C161" s="57" t="s">
+      <c r="C161" s="56" t="s">
         <v>129</v>
       </c>
-      <c r="D161" s="57" t="s">
+      <c r="D161" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="E161" s="57" t="s">
+      <c r="E161" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="F161" s="57" t="s">
+      <c r="F161" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G161" s="57"/>
-      <c r="H161" s="57"/>
-      <c r="I161" s="57" t="s">
+      <c r="G161" s="56"/>
+      <c r="H161" s="56"/>
+      <c r="I161" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="15.75">
-      <c r="A162" s="59" t="s">
+      <c r="A162" s="58" t="s">
         <v>278</v>
       </c>
-      <c r="B162" s="57" t="s">
+      <c r="B162" s="56" t="s">
         <v>280</v>
       </c>
-      <c r="C162" s="57" t="s">
+      <c r="C162" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D162" s="57" t="s">
+      <c r="D162" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E162" s="57" t="s">
+      <c r="E162" s="56" t="s">
         <v>265</v>
       </c>
-      <c r="F162" s="57" t="s">
+      <c r="F162" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G162" s="57"/>
-      <c r="H162" s="57"/>
-      <c r="I162" s="57" t="s">
+      <c r="G162" s="56"/>
+      <c r="H162" s="56"/>
+      <c r="I162" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="15.75">
-      <c r="A163" s="59" t="s">
+      <c r="A163" s="58" t="s">
         <v>278</v>
       </c>
-      <c r="B163" s="57" t="s">
+      <c r="B163" s="56" t="s">
         <v>281</v>
       </c>
-      <c r="C163" s="57" t="s">
+      <c r="C163" s="56" t="s">
         <v>282</v>
       </c>
-      <c r="D163" s="57" t="s">
+      <c r="D163" s="56" t="s">
         <v>241</v>
       </c>
-      <c r="E163" s="57" t="s">
+      <c r="E163" s="56" t="s">
         <v>283</v>
       </c>
-      <c r="F163" s="57" t="s">
+      <c r="F163" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G163" s="57"/>
-      <c r="H163" s="57"/>
-      <c r="I163" s="57" t="s">
+      <c r="G163" s="56"/>
+      <c r="H163" s="56"/>
+      <c r="I163" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="164" spans="1:9" ht="15.75">
-      <c r="A164" s="59" t="s">
+      <c r="A164" s="58" t="s">
         <v>278</v>
       </c>
-      <c r="B164" s="57" t="s">
+      <c r="B164" s="56" t="s">
         <v>284</v>
       </c>
-      <c r="C164" s="57" t="s">
+      <c r="C164" s="56" t="s">
         <v>285</v>
       </c>
-      <c r="D164" s="57" t="s">
+      <c r="D164" s="56" t="s">
         <v>286</v>
       </c>
-      <c r="E164" s="57" t="s">
+      <c r="E164" s="56" t="s">
         <v>287</v>
       </c>
-      <c r="F164" s="57" t="s">
+      <c r="F164" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="G164" s="57"/>
-      <c r="H164" s="57"/>
-      <c r="I164" s="57" t="s">
+      <c r="G164" s="56"/>
+      <c r="H164" s="56"/>
+      <c r="I164" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="165" spans="1:9" ht="15.75">
-      <c r="A165" s="59" t="s">
+      <c r="A165" s="58" t="s">
         <v>278</v>
       </c>
-      <c r="B165" s="57" t="s">
+      <c r="B165" s="56" t="s">
         <v>288</v>
       </c>
-      <c r="C165" s="57" t="s">
+      <c r="C165" s="56" t="s">
         <v>202</v>
       </c>
-      <c r="D165" s="57" t="s">
+      <c r="D165" s="56" t="s">
         <v>203</v>
       </c>
-      <c r="E165" s="57" t="s">
+      <c r="E165" s="56" t="s">
         <v>204</v>
       </c>
-      <c r="F165" s="57" t="s">
+      <c r="F165" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="G165" s="57"/>
-      <c r="H165" s="57"/>
-      <c r="I165" s="57" t="s">
+      <c r="G165" s="56"/>
+      <c r="H165" s="56"/>
+      <c r="I165" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="166" spans="1:9" ht="15.75">
-      <c r="A166" s="59" t="s">
+      <c r="A166" s="58" t="s">
         <v>278</v>
       </c>
-      <c r="B166" s="57" t="s">
+      <c r="B166" s="56" t="s">
         <v>289</v>
       </c>
-      <c r="C166" s="57" t="s">
+      <c r="C166" s="56" t="s">
         <v>215</v>
       </c>
-      <c r="D166" s="57" t="s">
+      <c r="D166" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="E166" s="57" t="s">
+      <c r="E166" s="56" t="s">
         <v>217</v>
       </c>
-      <c r="F166" s="57" t="s">
+      <c r="F166" s="56" t="s">
         <v>290</v>
       </c>
-      <c r="G166" s="57"/>
-      <c r="H166" s="57"/>
-      <c r="I166" s="57" t="s">
+      <c r="G166" s="56"/>
+      <c r="H166" s="56"/>
+      <c r="I166" s="56" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="167" spans="1:9" ht="63">
-      <c r="A167" s="59" t="s">
+      <c r="A167" s="58" t="s">
         <v>278</v>
       </c>
-      <c r="B167" s="57" t="s">
+      <c r="B167" s="56" t="s">
         <v>291</v>
       </c>
-      <c r="C167" s="57" t="s">
+      <c r="C167" s="56" t="s">
         <v>184</v>
       </c>
-      <c r="D167" s="57" t="s">
+      <c r="D167" s="56" t="s">
         <v>185</v>
       </c>
-      <c r="E167" s="57" t="s">
+      <c r="E167" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="F167" s="57" t="s">
+      <c r="F167" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="G167" s="57"/>
-      <c r="H167" s="57"/>
-      <c r="I167" s="58" t="s">
+      <c r="G167" s="56"/>
+      <c r="H167" s="56"/>
+      <c r="I167" s="57" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="168" spans="1:9" ht="15.75">
-      <c r="A168" s="59" t="s">
+      <c r="A168" s="58" t="s">
         <v>278</v>
       </c>
-      <c r="B168" s="57" t="s">
+      <c r="B168" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="C168" s="57" t="s">
+      <c r="C168" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="D168" s="57" t="s">
+      <c r="D168" s="56" t="s">
         <v>165</v>
       </c>
-      <c r="E168" s="57" t="s">
+      <c r="E168" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="F168" s="57" t="s">
+      <c r="F168" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="G168" s="57"/>
-      <c r="H168" s="57"/>
-      <c r="I168" s="57" t="s">
+      <c r="G168" s="56"/>
+      <c r="H168" s="56"/>
+      <c r="I168" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="15.75">
-      <c r="A169" s="59" t="s">
+      <c r="A169" s="58" t="s">
         <v>278</v>
       </c>
-      <c r="B169" s="57" t="s">
+      <c r="B169" s="56" t="s">
         <v>292</v>
       </c>
-      <c r="C169" s="57" t="s">
+      <c r="C169" s="56" t="s">
         <v>129</v>
       </c>
-      <c r="D169" s="57" t="s">
+      <c r="D169" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="E169" s="57" t="s">
+      <c r="E169" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="F169" s="57" t="s">
+      <c r="F169" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G169" s="57"/>
-      <c r="H169" s="57"/>
-      <c r="I169" s="57" t="s">
+      <c r="G169" s="56"/>
+      <c r="H169" s="56"/>
+      <c r="I169" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="170" spans="1:9" ht="15.75">
-      <c r="A170" s="59" t="s">
+      <c r="A170" s="58" t="s">
         <v>278</v>
       </c>
-      <c r="B170" s="57" t="s">
+      <c r="B170" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="C170" s="57" t="s">
+      <c r="C170" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D170" s="57" t="s">
+      <c r="D170" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E170" s="57" t="s">
+      <c r="E170" s="56" t="s">
         <v>265</v>
       </c>
-      <c r="F170" s="57" t="s">
+      <c r="F170" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G170" s="57"/>
-      <c r="H170" s="57"/>
-      <c r="I170" s="57" t="s">
+      <c r="G170" s="56"/>
+      <c r="H170" s="56"/>
+      <c r="I170" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="15.75">
-      <c r="A171" s="59" t="s">
+      <c r="A171" s="58" t="s">
         <v>278</v>
       </c>
-      <c r="B171" s="57" t="s">
+      <c r="B171" s="56" t="s">
         <v>293</v>
       </c>
-      <c r="C171" s="57" t="s">
+      <c r="C171" s="56" t="s">
         <v>129</v>
       </c>
-      <c r="D171" s="57" t="s">
+      <c r="D171" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="E171" s="57" t="s">
+      <c r="E171" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="F171" s="57" t="s">
+      <c r="F171" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G171" s="57"/>
-      <c r="H171" s="57"/>
-      <c r="I171" s="57" t="s">
+      <c r="G171" s="56"/>
+      <c r="H171" s="56"/>
+      <c r="I171" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="172" spans="1:9" ht="15.75">
-      <c r="A172" s="59" t="s">
+      <c r="A172" s="58" t="s">
         <v>278</v>
       </c>
-      <c r="B172" s="57" t="s">
+      <c r="B172" s="56" t="s">
         <v>294</v>
       </c>
-      <c r="C172" s="57" t="s">
+      <c r="C172" s="56" t="s">
         <v>275</v>
       </c>
-      <c r="D172" s="57" t="s">
+      <c r="D172" s="56" t="s">
         <v>276</v>
       </c>
-      <c r="E172" s="57" t="s">
+      <c r="E172" s="56" t="s">
         <v>277</v>
       </c>
-      <c r="F172" s="57" t="s">
+      <c r="F172" s="56" t="s">
         <v>164</v>
       </c>
-      <c r="G172" s="57"/>
-      <c r="H172" s="57"/>
-      <c r="I172" s="57" t="s">
+      <c r="G172" s="56"/>
+      <c r="H172" s="56"/>
+      <c r="I172" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="63">
-      <c r="A173" s="59" t="s">
+      <c r="A173" s="58" t="s">
         <v>295</v>
       </c>
-      <c r="B173" s="57" t="s">
+      <c r="B173" s="56" t="s">
         <v>296</v>
       </c>
-      <c r="C173" s="57" t="s">
+      <c r="C173" s="56" t="s">
         <v>184</v>
       </c>
-      <c r="D173" s="57" t="s">
+      <c r="D173" s="56" t="s">
         <v>185</v>
       </c>
-      <c r="E173" s="57" t="s">
+      <c r="E173" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="F173" s="57" t="s">
+      <c r="F173" s="56" t="s">
         <v>297</v>
       </c>
-      <c r="G173" s="57"/>
-      <c r="H173" s="57"/>
-      <c r="I173" s="58" t="s">
+      <c r="G173" s="56"/>
+      <c r="H173" s="56"/>
+      <c r="I173" s="57" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="174" spans="1:9" ht="78.75">
-      <c r="A174" s="59" t="s">
+      <c r="A174" s="58" t="s">
         <v>295</v>
       </c>
-      <c r="B174" s="57" t="s">
+      <c r="B174" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="C174" s="57" t="s">
+      <c r="C174" s="56" t="s">
         <v>275</v>
       </c>
-      <c r="D174" s="57" t="s">
+      <c r="D174" s="56" t="s">
         <v>276</v>
       </c>
-      <c r="E174" s="57" t="s">
+      <c r="E174" s="56" t="s">
         <v>277</v>
       </c>
-      <c r="F174" s="57" t="s">
+      <c r="F174" s="56" t="s">
         <v>164</v>
       </c>
-      <c r="G174" s="57" t="s">
+      <c r="G174" s="56" t="s">
         <v>298</v>
       </c>
-      <c r="H174" s="58" t="s">
+      <c r="H174" s="57" t="s">
         <v>299</v>
       </c>
-      <c r="I174" s="58" t="s">
+      <c r="I174" s="57" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="175" spans="1:9" ht="15.75">
-      <c r="A175" s="59" t="s">
+      <c r="A175" s="58" t="s">
         <v>295</v>
       </c>
-      <c r="B175" s="57" t="s">
+      <c r="B175" s="56" t="s">
         <v>301</v>
       </c>
-      <c r="C175" s="57" t="s">
+      <c r="C175" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D175" s="57" t="s">
+      <c r="D175" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E175" s="57" t="s">
+      <c r="E175" s="56" t="s">
         <v>265</v>
       </c>
-      <c r="F175" s="57" t="s">
+      <c r="F175" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G175" s="57"/>
-      <c r="H175" s="57"/>
-      <c r="I175" s="57" t="s">
+      <c r="G175" s="56"/>
+      <c r="H175" s="56"/>
+      <c r="I175" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="176" spans="1:9" ht="78.75">
-      <c r="A176" s="59" t="s">
+      <c r="A176" s="58" t="s">
         <v>295</v>
       </c>
-      <c r="B176" s="57" t="s">
+      <c r="B176" s="56" t="s">
         <v>302</v>
       </c>
-      <c r="C176" s="57" t="s">
+      <c r="C176" s="56" t="s">
         <v>129</v>
       </c>
-      <c r="D176" s="57" t="s">
+      <c r="D176" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="E176" s="57" t="s">
+      <c r="E176" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="F176" s="57" t="s">
+      <c r="F176" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G176" s="57" t="s">
+      <c r="G176" s="56" t="s">
         <v>303</v>
       </c>
-      <c r="H176" s="58" t="s">
+      <c r="H176" s="57" t="s">
         <v>304</v>
       </c>
-      <c r="I176" s="58" t="s">
+      <c r="I176" s="57" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="177" spans="1:9" ht="15.75">
-      <c r="A177" s="59" t="s">
+      <c r="A177" s="58" t="s">
         <v>306</v>
       </c>
-      <c r="B177" s="57" t="s">
+      <c r="B177" s="56" t="s">
         <v>307</v>
       </c>
-      <c r="C177" s="57" t="s">
+      <c r="C177" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="D177" s="57" t="s">
+      <c r="D177" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E177" s="57" t="s">
+      <c r="E177" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="F177" s="57" t="s">
+      <c r="F177" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="G177" s="57"/>
-      <c r="H177" s="57"/>
-      <c r="I177" s="57" t="s">
+      <c r="G177" s="56"/>
+      <c r="H177" s="56"/>
+      <c r="I177" s="56" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="178" spans="1:9" ht="15.75">
-      <c r="A178" s="59" t="s">
+      <c r="A178" s="58" t="s">
         <v>295</v>
       </c>
-      <c r="B178" s="57" t="s">
+      <c r="B178" s="56" t="s">
         <v>264</v>
       </c>
-      <c r="C178" s="57" t="s">
+      <c r="C178" s="56" t="s">
         <v>161</v>
       </c>
-      <c r="D178" s="57" t="s">
+      <c r="D178" s="56" t="s">
         <v>162</v>
       </c>
-      <c r="E178" s="57" t="s">
+      <c r="E178" s="56" t="s">
         <v>163</v>
       </c>
-      <c r="F178" s="57" t="s">
+      <c r="F178" s="56" t="s">
         <v>164</v>
       </c>
-      <c r="G178" s="57"/>
-      <c r="H178" s="57"/>
-      <c r="I178" s="57" t="s">
+      <c r="G178" s="56"/>
+      <c r="H178" s="56"/>
+      <c r="I178" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="179" spans="1:9" ht="15.75">
-      <c r="A179" s="59" t="s">
+      <c r="A179" s="58" t="s">
         <v>295</v>
       </c>
-      <c r="B179" s="57" t="s">
+      <c r="B179" s="56" t="s">
         <v>308</v>
       </c>
-      <c r="C179" s="57" t="s">
+      <c r="C179" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D179" s="57" t="s">
+      <c r="D179" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E179" s="57" t="s">
+      <c r="E179" s="56" t="s">
         <v>265</v>
       </c>
-      <c r="F179" s="57" t="s">
+      <c r="F179" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G179" s="57"/>
-      <c r="H179" s="57"/>
-      <c r="I179" s="57" t="s">
+      <c r="G179" s="56"/>
+      <c r="H179" s="56"/>
+      <c r="I179" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="180" spans="1:9" ht="15.75">
-      <c r="A180" s="59" t="s">
+      <c r="A180" s="58" t="s">
         <v>295</v>
       </c>
-      <c r="B180" s="57" t="s">
+      <c r="B180" s="56" t="s">
         <v>308</v>
       </c>
-      <c r="C180" s="57" t="s">
+      <c r="C180" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="D180" s="57" t="s">
+      <c r="D180" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="E180" s="57" t="s">
+      <c r="E180" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="F180" s="57" t="s">
+      <c r="F180" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G180" s="57"/>
-      <c r="H180" s="57"/>
-      <c r="I180" s="57" t="s">
+      <c r="G180" s="56"/>
+      <c r="H180" s="56"/>
+      <c r="I180" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="181" spans="1:9" ht="15.75">
-      <c r="A181" s="59" t="s">
+      <c r="A181" s="58" t="s">
         <v>309</v>
       </c>
-      <c r="B181" s="57" t="s">
+      <c r="B181" s="56" t="s">
         <v>310</v>
       </c>
-      <c r="C181" s="57" t="s">
+      <c r="C181" s="56" t="s">
         <v>161</v>
       </c>
-      <c r="D181" s="57" t="s">
+      <c r="D181" s="56" t="s">
         <v>162</v>
       </c>
-      <c r="E181" s="57" t="s">
+      <c r="E181" s="56" t="s">
         <v>163</v>
       </c>
-      <c r="F181" s="57" t="s">
+      <c r="F181" s="56" t="s">
         <v>164</v>
       </c>
-      <c r="G181" s="57"/>
-      <c r="H181" s="57"/>
-      <c r="I181" s="57" t="s">
+      <c r="G181" s="56"/>
+      <c r="H181" s="56"/>
+      <c r="I181" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="15.75">
-      <c r="A182" s="59" t="s">
+      <c r="A182" s="58" t="s">
         <v>309</v>
       </c>
-      <c r="B182" s="57"/>
-      <c r="C182" s="57"/>
-      <c r="D182" s="57"/>
-      <c r="E182" s="57"/>
-      <c r="F182" s="57"/>
-      <c r="G182" s="57"/>
-      <c r="H182" s="57"/>
-      <c r="I182" s="57"/>
+      <c r="B182" s="56"/>
+      <c r="C182" s="56"/>
+      <c r="D182" s="56"/>
+      <c r="E182" s="56"/>
+      <c r="F182" s="56"/>
+      <c r="G182" s="56"/>
+      <c r="H182" s="56"/>
+      <c r="I182" s="56"/>
     </row>
     <row r="183" spans="1:9" ht="63">
-      <c r="A183" s="59" t="s">
+      <c r="A183" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="B183" s="57" t="s">
+      <c r="B183" s="56" t="s">
         <v>312</v>
       </c>
-      <c r="C183" s="57" t="s">
+      <c r="C183" s="56" t="s">
         <v>184</v>
       </c>
-      <c r="D183" s="57" t="s">
+      <c r="D183" s="56" t="s">
         <v>185</v>
       </c>
-      <c r="E183" s="57" t="s">
+      <c r="E183" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="F183" s="57" t="s">
+      <c r="F183" s="56" t="s">
         <v>297</v>
       </c>
-      <c r="G183" s="57"/>
-      <c r="H183" s="57"/>
-      <c r="I183" s="58" t="s">
+      <c r="G183" s="56"/>
+      <c r="H183" s="56"/>
+      <c r="I183" s="57" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="184" spans="1:9" ht="15.75">
-      <c r="A184" s="59" t="s">
+      <c r="A184" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="B184" s="57" t="s">
+      <c r="B184" s="56" t="s">
         <v>313</v>
       </c>
-      <c r="C184" s="57" t="s">
+      <c r="C184" s="56" t="s">
         <v>140</v>
       </c>
-      <c r="D184" s="57" t="s">
+      <c r="D184" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="E184" s="57" t="s">
+      <c r="E184" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="F184" s="57" t="s">
+      <c r="F184" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="G184" s="57"/>
-      <c r="H184" s="57"/>
-      <c r="I184" s="57" t="s">
+      <c r="G184" s="56"/>
+      <c r="H184" s="56"/>
+      <c r="I184" s="56" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="15.75">
-      <c r="A185" s="59" t="s">
+      <c r="A185" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="B185" s="57" t="s">
+      <c r="B185" s="56" t="s">
         <v>274</v>
       </c>
-      <c r="C185" s="57" t="s">
+      <c r="C185" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D185" s="57" t="s">
+      <c r="D185" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E185" s="57" t="s">
+      <c r="E185" s="56" t="s">
         <v>265</v>
       </c>
-      <c r="F185" s="57" t="s">
+      <c r="F185" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G185" s="57"/>
-      <c r="H185" s="57"/>
-      <c r="I185" s="57" t="s">
+      <c r="G185" s="56"/>
+      <c r="H185" s="56"/>
+      <c r="I185" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="186" spans="1:9" ht="15.75">
-      <c r="A186" s="59" t="s">
+      <c r="A186" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="B186" s="57" t="s">
+      <c r="B186" s="56" t="s">
         <v>314</v>
       </c>
-      <c r="C186" s="57" t="s">
+      <c r="C186" s="56" t="s">
         <v>197</v>
       </c>
-      <c r="D186" s="57" t="s">
+      <c r="D186" s="56" t="s">
         <v>198</v>
       </c>
-      <c r="E186" s="57" t="s">
+      <c r="E186" s="56" t="s">
         <v>199</v>
       </c>
-      <c r="F186" s="57" t="s">
+      <c r="F186" s="56" t="s">
         <v>200</v>
       </c>
-      <c r="G186" s="57"/>
-      <c r="H186" s="57"/>
-      <c r="I186" s="57" t="s">
+      <c r="G186" s="56"/>
+      <c r="H186" s="56"/>
+      <c r="I186" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="187" spans="1:9" ht="15.75">
-      <c r="A187" s="59" t="s">
+      <c r="A187" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="B187" s="57" t="s">
+      <c r="B187" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="C187" s="57" t="s">
+      <c r="C187" s="56" t="s">
         <v>180</v>
       </c>
-      <c r="D187" s="57" t="s">
+      <c r="D187" s="56" t="s">
         <v>181</v>
       </c>
-      <c r="E187" s="57" t="s">
+      <c r="E187" s="56" t="s">
         <v>179</v>
       </c>
-      <c r="F187" s="57" t="s">
+      <c r="F187" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="G187" s="57"/>
-      <c r="H187" s="57"/>
-      <c r="I187" s="57" t="s">
+      <c r="G187" s="56"/>
+      <c r="H187" s="56"/>
+      <c r="I187" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="188" spans="1:9" ht="15.75">
-      <c r="A188" s="59" t="s">
+      <c r="A188" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="B188" s="57" t="s">
+      <c r="B188" s="56" t="s">
         <v>315</v>
       </c>
-      <c r="C188" s="57" t="s">
+      <c r="C188" s="56" t="s">
         <v>184</v>
       </c>
-      <c r="D188" s="57" t="s">
+      <c r="D188" s="56" t="s">
         <v>185</v>
       </c>
-      <c r="E188" s="57" t="s">
+      <c r="E188" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="F188" s="57"/>
-      <c r="G188" s="57"/>
-      <c r="H188" s="57"/>
-      <c r="I188" s="57" t="s">
+      <c r="F188" s="56"/>
+      <c r="G188" s="56"/>
+      <c r="H188" s="56"/>
+      <c r="I188" s="56" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="189" spans="1:9" ht="15.75">
-      <c r="A189" s="59" t="s">
+      <c r="A189" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="B189" s="57" t="s">
+      <c r="B189" s="56" t="s">
         <v>270</v>
       </c>
-      <c r="C189" s="57" t="s">
+      <c r="C189" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="D189" s="57" t="s">
+      <c r="D189" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="E189" s="57" t="s">
+      <c r="E189" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="F189" s="57" t="s">
+      <c r="F189" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="G189" s="57"/>
-      <c r="H189" s="57"/>
-      <c r="I189" s="57" t="s">
+      <c r="G189" s="56"/>
+      <c r="H189" s="56"/>
+      <c r="I189" s="56" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="190" spans="1:9" ht="15.75">
-      <c r="A190" s="59" t="s">
+      <c r="A190" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="B190" s="57" t="s">
+      <c r="B190" s="56" t="s">
         <v>316</v>
       </c>
-      <c r="C190" s="57" t="s">
+      <c r="C190" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="D190" s="57" t="s">
+      <c r="D190" s="56" t="s">
         <v>317</v>
       </c>
-      <c r="E190" s="57" t="s">
+      <c r="E190" s="56" t="s">
         <v>318</v>
       </c>
-      <c r="F190" s="57" t="s">
+      <c r="F190" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G190" s="57"/>
-      <c r="H190" s="57"/>
-      <c r="I190" s="57" t="s">
+      <c r="G190" s="56"/>
+      <c r="H190" s="56"/>
+      <c r="I190" s="56" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="191" spans="1:9" ht="15.75">
-      <c r="A191" s="59" t="s">
+      <c r="A191" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="B191" s="57" t="s">
+      <c r="B191" s="56" t="s">
         <v>316</v>
       </c>
-      <c r="C191" s="57" t="s">
+      <c r="C191" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="D191" s="57" t="s">
+      <c r="D191" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E191" s="57" t="s">
+      <c r="E191" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="F191" s="57" t="s">
+      <c r="F191" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="G191" s="57"/>
-      <c r="H191" s="57"/>
-      <c r="I191" s="57" t="s">
+      <c r="G191" s="56"/>
+      <c r="H191" s="56"/>
+      <c r="I191" s="56" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="192" spans="1:9" ht="15.75">
-      <c r="A192" s="59" t="s">
+      <c r="A192" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="B192" s="57" t="s">
+      <c r="B192" s="56" t="s">
         <v>319</v>
       </c>
-      <c r="C192" s="57" t="s">
+      <c r="C192" s="56" t="s">
         <v>129</v>
       </c>
-      <c r="D192" s="57" t="s">
+      <c r="D192" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="E192" s="57" t="s">
+      <c r="E192" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="F192" s="57" t="s">
+      <c r="F192" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G192" s="57"/>
-      <c r="H192" s="57"/>
-      <c r="I192" s="57"/>
+      <c r="G192" s="56"/>
+      <c r="H192" s="56"/>
+      <c r="I192" s="56"/>
     </row>
     <row r="193" spans="1:9" ht="15.75">
-      <c r="A193" s="59" t="s">
+      <c r="A193" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="B193" s="57" t="s">
+      <c r="B193" s="56" t="s">
         <v>139</v>
       </c>
-      <c r="C193" s="57" t="s">
+      <c r="C193" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="D193" s="57" t="s">
+      <c r="D193" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E193" s="57" t="s">
+      <c r="E193" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="F193" s="57" t="s">
+      <c r="F193" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="G193" s="57"/>
-      <c r="H193" s="57"/>
-      <c r="I193" s="57" t="s">
+      <c r="G193" s="56"/>
+      <c r="H193" s="56"/>
+      <c r="I193" s="56" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="194" spans="1:9" ht="15.75">
-      <c r="A194" s="59" t="s">
+      <c r="A194" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="B194" s="57" t="s">
+      <c r="B194" s="56" t="s">
         <v>320</v>
       </c>
-      <c r="C194" s="57" t="s">
+      <c r="C194" s="56" t="s">
         <v>202</v>
       </c>
-      <c r="D194" s="57" t="s">
+      <c r="D194" s="56" t="s">
         <v>203</v>
       </c>
-      <c r="E194" s="57" t="s">
+      <c r="E194" s="56" t="s">
         <v>204</v>
       </c>
-      <c r="F194" s="57" t="s">
+      <c r="F194" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="G194" s="57"/>
-      <c r="H194" s="57"/>
-      <c r="I194" s="57" t="s">
+      <c r="G194" s="56"/>
+      <c r="H194" s="56"/>
+      <c r="I194" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="195" spans="1:9" ht="15.75">
-      <c r="A195" s="59" t="s">
+      <c r="A195" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="B195" s="57" t="s">
+      <c r="B195" s="56" t="s">
         <v>321</v>
       </c>
-      <c r="C195" s="57" t="s">
+      <c r="C195" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="D195" s="57" t="s">
+      <c r="D195" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="E195" s="57" t="s">
+      <c r="E195" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="F195" s="57" t="s">
+      <c r="F195" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G195" s="57"/>
-      <c r="H195" s="57"/>
-      <c r="I195" s="57" t="s">
+      <c r="G195" s="56"/>
+      <c r="H195" s="56"/>
+      <c r="I195" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="196" spans="1:9" ht="15.75">
-      <c r="A196" s="59" t="s">
+      <c r="A196" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="B196" s="57" t="s">
+      <c r="B196" s="56" t="s">
         <v>321</v>
       </c>
-      <c r="C196" s="57" t="s">
+      <c r="C196" s="56" t="s">
         <v>169</v>
       </c>
-      <c r="D196" s="57" t="s">
+      <c r="D196" s="56" t="s">
         <v>322</v>
       </c>
-      <c r="E196" s="57" t="s">
+      <c r="E196" s="56" t="s">
         <v>171</v>
       </c>
-      <c r="F196" s="57" t="s">
+      <c r="F196" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="G196" s="57"/>
-      <c r="H196" s="57"/>
-      <c r="I196" s="57" t="s">
+      <c r="G196" s="56"/>
+      <c r="H196" s="56"/>
+      <c r="I196" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="197" spans="1:9" ht="15.75">
-      <c r="A197" s="59" t="s">
+      <c r="A197" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="B197" s="57" t="s">
+      <c r="B197" s="56" t="s">
         <v>323</v>
       </c>
-      <c r="C197" s="57" t="s">
+      <c r="C197" s="56" t="s">
         <v>282</v>
       </c>
-      <c r="D197" s="57" t="s">
+      <c r="D197" s="56" t="s">
         <v>241</v>
       </c>
-      <c r="E197" s="57" t="s">
+      <c r="E197" s="56" t="s">
         <v>283</v>
       </c>
-      <c r="F197" s="57" t="s">
+      <c r="F197" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G197" s="57"/>
-      <c r="H197" s="57"/>
-      <c r="I197" s="57" t="s">
+      <c r="G197" s="56"/>
+      <c r="H197" s="56"/>
+      <c r="I197" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="198" spans="1:9" ht="15.75">
-      <c r="A198" s="59" t="s">
+      <c r="A198" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="B198" s="57" t="s">
+      <c r="B198" s="56" t="s">
         <v>324</v>
       </c>
-      <c r="C198" s="57" t="s">
+      <c r="C198" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="D198" s="57" t="s">
+      <c r="D198" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="E198" s="57" t="s">
+      <c r="E198" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="F198" s="57" t="s">
+      <c r="F198" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G198" s="57"/>
-      <c r="H198" s="57"/>
-      <c r="I198" s="57" t="s">
+      <c r="G198" s="56"/>
+      <c r="H198" s="56"/>
+      <c r="I198" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="199" spans="1:9" ht="15.75">
-      <c r="A199" s="59" t="s">
+      <c r="A199" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="B199" s="57" t="s">
+      <c r="B199" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="C199" s="57" t="s">
+      <c r="C199" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D199" s="57" t="s">
+      <c r="D199" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E199" s="57" t="s">
+      <c r="E199" s="56" t="s">
         <v>265</v>
       </c>
-      <c r="F199" s="57" t="s">
+      <c r="F199" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G199" s="57"/>
-      <c r="H199" s="57"/>
-      <c r="I199" s="57" t="s">
+      <c r="G199" s="56"/>
+      <c r="H199" s="56"/>
+      <c r="I199" s="56" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="200" spans="1:9" ht="15.75">
-      <c r="A200" s="59" t="s">
+      <c r="A200" s="58" t="s">
         <v>325</v>
       </c>
-      <c r="B200" s="57" t="s">
+      <c r="B200" s="56" t="s">
         <v>326</v>
       </c>
-      <c r="C200" s="57" t="s">
+      <c r="C200" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="D200" s="57" t="s">
+      <c r="D200" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="E200" s="57" t="s">
+      <c r="E200" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="F200" s="57" t="s">
+      <c r="F200" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="G200" s="57"/>
-      <c r="H200" s="57"/>
-      <c r="I200" s="57" t="s">
-        <v>250</v>
+      <c r="G200" s="56"/>
+      <c r="H200" s="56"/>
+      <c r="I200" s="56" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" ht="15.75">
+      <c r="A201" s="58" t="s">
+        <v>325</v>
+      </c>
+      <c r="B201" s="56" t="s">
+        <v>327</v>
+      </c>
+      <c r="C201" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="D201" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="E201" s="56" t="s">
+        <v>328</v>
+      </c>
+      <c r="F201" s="56" t="s">
+        <v>329</v>
+      </c>
+      <c r="G201" s="56"/>
+      <c r="H201" s="56"/>
+      <c r="I201" s="56" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" ht="15.75">
+      <c r="A202" s="58" t="s">
+        <v>325</v>
+      </c>
+      <c r="B202" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="C202" s="56" t="s">
+        <v>330</v>
+      </c>
+      <c r="D202" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="E202" s="56" t="s">
+        <v>331</v>
+      </c>
+      <c r="F202" s="56" t="s">
+        <v>332</v>
+      </c>
+      <c r="G202" s="56"/>
+      <c r="H202" s="56"/>
+      <c r="I202" s="56" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" ht="15.75">
+      <c r="A203" s="58" t="s">
+        <v>325</v>
+      </c>
+      <c r="B203" s="56" t="s">
+        <v>334</v>
+      </c>
+      <c r="C203" s="56" t="s">
+        <v>335</v>
+      </c>
+      <c r="D203" s="56" t="s">
+        <v>203</v>
+      </c>
+      <c r="E203" s="56" t="s">
+        <v>336</v>
+      </c>
+      <c r="F203" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="G203" s="56"/>
+      <c r="H203" s="56"/>
+      <c r="I203" s="56" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" ht="15.75">
+      <c r="A204" s="58" t="s">
+        <v>325</v>
+      </c>
+      <c r="B204" s="56" t="s">
+        <v>261</v>
+      </c>
+      <c r="C204" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="D204" s="56" t="s">
+        <v>333</v>
+      </c>
+      <c r="E204" s="56" t="s">
+        <v>338</v>
+      </c>
+      <c r="F204" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="G204" s="56"/>
+      <c r="H204" s="56"/>
+      <c r="I204" s="56" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to be committed: 	modified:   Libro1.xlsx 	modified:   index.html 	modified:   meses/abril.html
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="343">
   <si>
     <t>LA FRIA</t>
   </si>
@@ -1036,6 +1036,15 @@
   </si>
   <si>
     <t>1211</t>
+  </si>
+  <si>
+    <t>BANFA-9900</t>
+  </si>
+  <si>
+    <t>1212</t>
+  </si>
+  <si>
+    <t>21/04/2025</t>
   </si>
 </sst>
 </file>
@@ -10853,7 +10862,7 @@
     <xf numFmtId="0" fontId="45" fillId="0" borderId="31"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -11008,6 +11017,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -21379,10 +21389,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N204"/>
+  <dimension ref="A1:N205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q36" sqref="Q36"/>
+    <sheetView tabSelected="1" topLeftCell="E33" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -21464,8 +21474,8 @@
       <c r="M2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "LA FRIA")</f>
+      <c r="N2" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D2)</f>
         <v>0</v>
       </c>
     </row>
@@ -21500,8 +21510,8 @@
       <c r="M3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N3" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "BARINAS")</f>
+      <c r="N3" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D9)</f>
         <v>0</v>
       </c>
     </row>
@@ -21536,8 +21546,8 @@
       <c r="M4" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="N4" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "PUERTO ORDAZ")</f>
+      <c r="N4" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, K131)</f>
         <v>0</v>
       </c>
     </row>
@@ -21572,8 +21582,8 @@
       <c r="M5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="4">
-        <f>COUNTIFS(A5:A133,A85,D5:D133, "MARACAY")</f>
+      <c r="N5" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205,D181)</f>
         <v>0</v>
       </c>
     </row>
@@ -21608,8 +21618,8 @@
       <c r="M6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="N6" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "BARCELONA")</f>
+      <c r="N6" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D31)</f>
         <v>0</v>
       </c>
     </row>
@@ -21644,8 +21654,8 @@
       <c r="M7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "CIUDAD BOLIVAR")</f>
+      <c r="N7" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D139)</f>
         <v>0</v>
       </c>
     </row>
@@ -21680,8 +21690,8 @@
       <c r="M8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N8" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "VALENCIA")</f>
+      <c r="N8" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D11)</f>
         <v>0</v>
       </c>
     </row>
@@ -21716,8 +21726,8 @@
       <c r="M9" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="N9" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "PUERTO CABELLO")</f>
+      <c r="N9" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D84)</f>
         <v>0</v>
       </c>
     </row>
@@ -21752,8 +21762,8 @@
       <c r="M10" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="N10" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "PUNTO FIJO")</f>
+      <c r="N10" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D197)</f>
         <v>0</v>
       </c>
     </row>
@@ -21788,9 +21798,9 @@
       <c r="M11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N11" s="4">
-        <f>COUNTIFS(A131:A204,A201,D131:D204, D204)</f>
-        <v>1</v>
+      <c r="N11" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D33)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75">
@@ -21824,8 +21834,8 @@
       <c r="M12" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="N12" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "HOSPITAL MILITAR DE SAN CRISTOBAL")</f>
+      <c r="N12" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205,L28)</f>
         <v>0</v>
       </c>
     </row>
@@ -21860,8 +21870,8 @@
       <c r="M13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N13" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "SAN CRISTOBAL")</f>
+      <c r="N13" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D14)</f>
         <v>0</v>
       </c>
     </row>
@@ -21896,8 +21906,8 @@
       <c r="M14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N14" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "MARACAIBO")</f>
+      <c r="N14" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205,D59)</f>
         <v>0</v>
       </c>
     </row>
@@ -21932,8 +21942,8 @@
       <c r="M15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "ZULIA")</f>
+      <c r="N15" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D32)</f>
         <v>0</v>
       </c>
     </row>
@@ -21968,8 +21978,8 @@
       <c r="M16" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="N16" s="4">
-        <f>COUNTIFS(A16:A144,A96,D16:D144, "MINISTERIO DE LA DEFENSA")</f>
+      <c r="N16" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, K29)</f>
         <v>0</v>
       </c>
     </row>
@@ -22004,8 +22014,8 @@
       <c r="M17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N17" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "ACADEMIA MILITAR")</f>
+      <c r="N17" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, J33)</f>
         <v>0</v>
       </c>
     </row>
@@ -22040,8 +22050,8 @@
       <c r="M18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N18" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "CANES")</f>
+      <c r="N18" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, K147)</f>
         <v>0</v>
       </c>
     </row>
@@ -22076,8 +22086,8 @@
       <c r="M19" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="N19" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "COMANDANCIA GENERAL DE LA GNB")</f>
+      <c r="N19" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, L39)</f>
         <v>0</v>
       </c>
     </row>
@@ -22112,8 +22122,8 @@
       <c r="M20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N20" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "GUARICO")</f>
+      <c r="N20" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D70)</f>
         <v>0</v>
       </c>
     </row>
@@ -22148,9 +22158,9 @@
       <c r="M21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N21" s="4">
-        <f>COUNTIFS(A131:A202,A200,D131:D202, D201)</f>
-        <v>3</v>
+      <c r="N21" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D82)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75">
@@ -22184,8 +22194,8 @@
       <c r="M22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N22" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "APURE")</f>
+      <c r="N22" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D69)</f>
         <v>0</v>
       </c>
     </row>
@@ -22220,8 +22230,8 @@
       <c r="M23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N23" s="4">
-        <f>COUNTIFS(A23:A151,A103,D23:D151, "MIRANDA")</f>
+      <c r="N23" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, K55)</f>
         <v>0</v>
       </c>
     </row>
@@ -22256,8 +22266,8 @@
       <c r="M24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N24" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "MONAGAS")</f>
+      <c r="N24" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D64)</f>
         <v>0</v>
       </c>
     </row>
@@ -22292,8 +22302,8 @@
       <c r="M25" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="N25" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "DELTA AMACURO")</f>
+      <c r="N25" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D34)</f>
         <v>0</v>
       </c>
     </row>
@@ -22328,8 +22338,8 @@
       <c r="M26" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="N26" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "NUEVA ESPARTA")</f>
+      <c r="N26" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D164)</f>
         <v>0</v>
       </c>
     </row>
@@ -22364,8 +22374,8 @@
       <c r="M27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="N27" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "SUCRE")</f>
+      <c r="N27" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D56)</f>
         <v>0</v>
       </c>
     </row>
@@ -22400,8 +22410,8 @@
       <c r="M28" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N28" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "TRUJILLO")</f>
+      <c r="N28" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D42)</f>
         <v>0</v>
       </c>
     </row>
@@ -22436,8 +22446,8 @@
       <c r="M29" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N29" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "MERIDA")</f>
+      <c r="N29" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205,D76)</f>
         <v>0</v>
       </c>
     </row>
@@ -22472,8 +22482,8 @@
       <c r="M30" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="N30" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "YARACUY")</f>
+      <c r="N30" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D40)</f>
         <v>0</v>
       </c>
     </row>
@@ -22508,9 +22518,9 @@
       <c r="M31" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N31" s="4">
-        <f>COUNTIFS(A131:A204,A202,D131:D204, D203)</f>
-        <v>1</v>
+      <c r="N31" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D85)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75">
@@ -22544,8 +22554,8 @@
       <c r="M32" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N32" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "AMAZONAS")</f>
+      <c r="N32" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D172)</f>
         <v>0</v>
       </c>
     </row>
@@ -22581,8 +22591,8 @@
         <v>30</v>
       </c>
       <c r="N33" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "ALTOS MIRANDINOS")</f>
-        <v>0</v>
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D205)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="15.75">
@@ -22616,8 +22626,8 @@
       <c r="M34" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="N34" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "HOSPITAL MILITAR DR. CARLOS AREVALO")</f>
+      <c r="N34" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D206)</f>
         <v>0</v>
       </c>
     </row>
@@ -22652,8 +22662,8 @@
       <c r="M35" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N35" s="4">
-        <f>COUNTIFS(A35:A163,A115,D35:D163, "RAMO VERDE")</f>
+      <c r="N35" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D207)</f>
         <v>0</v>
       </c>
     </row>
@@ -22688,8 +22698,8 @@
       <c r="M36" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N36" s="4">
-        <f>COUNTIFS(A131:A200,A200,D131:D200, "CARUPANO")</f>
+      <c r="N36" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D208)</f>
         <v>0</v>
       </c>
     </row>
@@ -22724,8 +22734,8 @@
       <c r="M37" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="N37" s="4">
-        <f>COUNTIFS(A37:A165,A117,D37:D165, "CIRCULO MILITAR")</f>
+      <c r="N37" s="56">
+        <f>COUNTIFS(A131:A205,A205,D131:D205, D209)</f>
         <v>0</v>
       </c>
     </row>
@@ -22757,9 +22767,9 @@
       <c r="I38" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="N38" s="59">
+      <c r="N38" s="60">
         <f>SUM(N2:N37)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="31.5">
@@ -25423,1844 +25433,1869 @@
       </c>
     </row>
     <row r="131" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A131" s="58" t="s">
+      <c r="A131" s="59" t="s">
         <v>248</v>
       </c>
-      <c r="B131" s="56" t="s">
+      <c r="B131" s="57" t="s">
         <v>249</v>
       </c>
-      <c r="C131" s="56" t="s">
+      <c r="C131" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D131" s="56" t="s">
+      <c r="D131" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E131" s="56" t="s">
+      <c r="E131" s="57" t="s">
         <v>176</v>
       </c>
-      <c r="F131" s="56" t="s">
+      <c r="F131" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="G131" s="56"/>
-      <c r="H131" s="56"/>
-      <c r="I131" s="56" t="s">
+      <c r="G131" s="57"/>
+      <c r="H131" s="57"/>
+      <c r="I131" s="57" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A132" s="58" t="s">
+      <c r="A132" s="59" t="s">
         <v>248</v>
       </c>
-      <c r="B132" s="56" t="s">
+      <c r="B132" s="57" t="s">
         <v>132</v>
       </c>
-      <c r="C132" s="56" t="s">
+      <c r="C132" s="57" t="s">
         <v>184</v>
       </c>
-      <c r="D132" s="56" t="s">
+      <c r="D132" s="57" t="s">
         <v>185</v>
       </c>
-      <c r="E132" s="56" t="s">
+      <c r="E132" s="57" t="s">
         <v>186</v>
       </c>
-      <c r="F132" s="56" t="s">
+      <c r="F132" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="G132" s="56"/>
-      <c r="H132" s="56"/>
-      <c r="I132" s="57" t="s">
+      <c r="G132" s="57"/>
+      <c r="H132" s="57"/>
+      <c r="I132" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="15.75">
-      <c r="A133" s="58" t="s">
+      <c r="A133" s="59" t="s">
         <v>252</v>
       </c>
-      <c r="B133" s="56" t="s">
+      <c r="B133" s="57" t="s">
         <v>191</v>
       </c>
-      <c r="C133" s="56" t="s">
+      <c r="C133" s="57" t="s">
         <v>253</v>
       </c>
-      <c r="D133" s="56" t="s">
+      <c r="D133" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="E133" s="56" t="s">
+      <c r="E133" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="F133" s="56" t="s">
+      <c r="F133" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="G133" s="56"/>
-      <c r="H133" s="56"/>
-      <c r="I133" s="56" t="s">
+      <c r="G133" s="57"/>
+      <c r="H133" s="57"/>
+      <c r="I133" s="57" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="15.75">
-      <c r="A134" s="58" t="s">
+      <c r="A134" s="59" t="s">
         <v>252</v>
       </c>
-      <c r="B134" s="56" t="s">
+      <c r="B134" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="C134" s="56" t="s">
+      <c r="C134" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D134" s="56" t="s">
+      <c r="D134" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E134" s="56" t="s">
+      <c r="E134" s="57" t="s">
         <v>176</v>
       </c>
-      <c r="F134" s="56" t="s">
+      <c r="F134" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="G134" s="56"/>
-      <c r="H134" s="56"/>
-      <c r="I134" s="56" t="s">
+      <c r="G134" s="57"/>
+      <c r="H134" s="57"/>
+      <c r="I134" s="57" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="15.75">
-      <c r="A135" s="58" t="s">
+      <c r="A135" s="59" t="s">
         <v>252</v>
       </c>
-      <c r="B135" s="56" t="s">
+      <c r="B135" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="C135" s="56" t="s">
+      <c r="C135" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="D135" s="56" t="s">
+      <c r="D135" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="E135" s="56" t="s">
+      <c r="E135" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="F135" s="56" t="s">
+      <c r="F135" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G135" s="56"/>
-      <c r="H135" s="56"/>
-      <c r="I135" s="56" t="s">
+      <c r="G135" s="57"/>
+      <c r="H135" s="57"/>
+      <c r="I135" s="57" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="15.75">
-      <c r="A136" s="58" t="s">
+      <c r="A136" s="59" t="s">
         <v>252</v>
       </c>
-      <c r="B136" s="56" t="s">
+      <c r="B136" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="C136" s="56" t="s">
+      <c r="C136" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="D136" s="56" t="s">
+      <c r="D136" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E136" s="56" t="s">
+      <c r="E136" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="F136" s="56" t="s">
+      <c r="F136" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="G136" s="56"/>
-      <c r="H136" s="56"/>
-      <c r="I136" s="56" t="s">
+      <c r="G136" s="57"/>
+      <c r="H136" s="57"/>
+      <c r="I136" s="57" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="15.75">
-      <c r="A137" s="58" t="s">
+      <c r="A137" s="59" t="s">
         <v>252</v>
       </c>
-      <c r="B137" s="56" t="s">
+      <c r="B137" s="57" t="s">
         <v>255</v>
       </c>
-      <c r="C137" s="56" t="s">
+      <c r="C137" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="D137" s="56" t="s">
+      <c r="D137" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="E137" s="56" t="s">
+      <c r="E137" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="F137" s="56" t="s">
+      <c r="F137" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="G137" s="56"/>
-      <c r="H137" s="56"/>
-      <c r="I137" s="56" t="s">
+      <c r="G137" s="57"/>
+      <c r="H137" s="57"/>
+      <c r="I137" s="57" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="15.75">
-      <c r="A138" s="58" t="s">
+      <c r="A138" s="59" t="s">
         <v>252</v>
       </c>
-      <c r="B138" s="56" t="s">
+      <c r="B138" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="C138" s="56" t="s">
+      <c r="C138" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D138" s="56" t="s">
+      <c r="D138" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="E138" s="56" t="s">
+      <c r="E138" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="F138" s="56" t="s">
+      <c r="F138" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="G138" s="56"/>
-      <c r="H138" s="56"/>
-      <c r="I138" s="56" t="s">
+      <c r="G138" s="57"/>
+      <c r="H138" s="57"/>
+      <c r="I138" s="57" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="15.75">
-      <c r="A139" s="58" t="s">
+      <c r="A139" s="59" t="s">
         <v>252</v>
       </c>
-      <c r="B139" s="56" t="s">
+      <c r="B139" s="57" t="s">
         <v>257</v>
       </c>
-      <c r="C139" s="56" t="s">
+      <c r="C139" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="D139" s="56" t="s">
+      <c r="D139" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="E139" s="56" t="s">
+      <c r="E139" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="F139" s="56" t="s">
+      <c r="F139" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="G139" s="56"/>
-      <c r="H139" s="56"/>
-      <c r="I139" s="56" t="s">
+      <c r="G139" s="57"/>
+      <c r="H139" s="57"/>
+      <c r="I139" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="15.75">
-      <c r="A140" s="58" t="s">
+      <c r="A140" s="59" t="s">
         <v>259</v>
       </c>
-      <c r="B140" s="56" t="s">
+      <c r="B140" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="C140" s="56" t="s">
+      <c r="C140" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="D140" s="56" t="s">
+      <c r="D140" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="E140" s="56" t="s">
+      <c r="E140" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="F140" s="56" t="s">
+      <c r="F140" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="G140" s="56"/>
-      <c r="H140" s="56"/>
-      <c r="I140" s="56" t="s">
+      <c r="G140" s="57"/>
+      <c r="H140" s="57"/>
+      <c r="I140" s="57" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="141" spans="1:9" ht="15.75">
-      <c r="A141" s="58" t="s">
+      <c r="A141" s="59" t="s">
         <v>259</v>
       </c>
-      <c r="B141" s="56" t="s">
+      <c r="B141" s="57" t="s">
         <v>260</v>
       </c>
-      <c r="C141" s="56" t="s">
+      <c r="C141" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D141" s="56" t="s">
+      <c r="D141" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E141" s="56" t="s">
+      <c r="E141" s="57" t="s">
         <v>176</v>
       </c>
-      <c r="F141" s="56" t="s">
+      <c r="F141" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="G141" s="56"/>
-      <c r="H141" s="56"/>
-      <c r="I141" s="56" t="s">
+      <c r="G141" s="57"/>
+      <c r="H141" s="57"/>
+      <c r="I141" s="57" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="15.75">
-      <c r="A142" s="58" t="s">
+      <c r="A142" s="59" t="s">
         <v>259</v>
       </c>
-      <c r="B142" s="56" t="s">
+      <c r="B142" s="57" t="s">
         <v>261</v>
       </c>
-      <c r="C142" s="56" t="s">
+      <c r="C142" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="D142" s="56" t="s">
+      <c r="D142" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="E142" s="56" t="s">
+      <c r="E142" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="F142" s="56" t="s">
+      <c r="F142" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="G142" s="56"/>
-      <c r="H142" s="56"/>
-      <c r="I142" s="56" t="s">
+      <c r="G142" s="57"/>
+      <c r="H142" s="57"/>
+      <c r="I142" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="15.75">
-      <c r="A143" s="58" t="s">
+      <c r="A143" s="59" t="s">
         <v>259</v>
       </c>
-      <c r="B143" s="56" t="s">
+      <c r="B143" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="C143" s="56" t="s">
+      <c r="C143" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="D143" s="56" t="s">
+      <c r="D143" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="E143" s="56" t="s">
+      <c r="E143" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="F143" s="56" t="s">
+      <c r="F143" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="G143" s="56"/>
-      <c r="H143" s="56"/>
-      <c r="I143" s="56" t="s">
+      <c r="G143" s="57"/>
+      <c r="H143" s="57"/>
+      <c r="I143" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="144" spans="1:9" ht="15.75">
-      <c r="A144" s="58" t="s">
+      <c r="A144" s="59" t="s">
         <v>259</v>
       </c>
-      <c r="B144" s="56" t="s">
+      <c r="B144" s="57" t="s">
         <v>154</v>
       </c>
-      <c r="C144" s="56" t="s">
+      <c r="C144" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="D144" s="56" t="s">
+      <c r="D144" s="57" t="s">
         <v>203</v>
       </c>
-      <c r="E144" s="56" t="s">
+      <c r="E144" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="F144" s="56" t="s">
+      <c r="F144" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="G144" s="56"/>
-      <c r="H144" s="56"/>
-      <c r="I144" s="56" t="s">
+      <c r="G144" s="57"/>
+      <c r="H144" s="57"/>
+      <c r="I144" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="15.75">
-      <c r="A145" s="58" t="s">
+      <c r="A145" s="59" t="s">
         <v>259</v>
       </c>
-      <c r="B145" s="56" t="s">
+      <c r="B145" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="C145" s="56" t="s">
+      <c r="C145" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D145" s="56" t="s">
+      <c r="D145" s="57" t="s">
         <v>165</v>
       </c>
-      <c r="E145" s="56" t="s">
+      <c r="E145" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="F145" s="56" t="s">
+      <c r="F145" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="G145" s="56"/>
-      <c r="H145" s="56"/>
-      <c r="I145" s="56" t="s">
+      <c r="G145" s="57"/>
+      <c r="H145" s="57"/>
+      <c r="I145" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="146" spans="1:9" ht="15.75">
-      <c r="A146" s="58" t="s">
+      <c r="A146" s="59" t="s">
         <v>259</v>
       </c>
-      <c r="B146" s="56" t="s">
+      <c r="B146" s="57" t="s">
         <v>255</v>
       </c>
-      <c r="C146" s="56" t="s">
+      <c r="C146" s="57" t="s">
         <v>117</v>
       </c>
-      <c r="D146" s="56" t="s">
+      <c r="D146" s="57" t="s">
         <v>118</v>
       </c>
-      <c r="E146" s="56" t="s">
+      <c r="E146" s="57" t="s">
         <v>119</v>
       </c>
-      <c r="F146" s="56" t="s">
+      <c r="F146" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="G146" s="56"/>
-      <c r="H146" s="56"/>
-      <c r="I146" s="56" t="s">
+      <c r="G146" s="57"/>
+      <c r="H146" s="57"/>
+      <c r="I146" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="147" spans="1:9" ht="15.75">
-      <c r="A147" s="58" t="s">
+      <c r="A147" s="59" t="s">
         <v>259</v>
       </c>
-      <c r="B147" s="56" t="s">
+      <c r="B147" s="57" t="s">
         <v>262</v>
       </c>
-      <c r="C147" s="56" t="s">
+      <c r="C147" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="D147" s="56" t="s">
+      <c r="D147" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="E147" s="56" t="s">
+      <c r="E147" s="57" t="s">
         <v>263</v>
       </c>
-      <c r="F147" s="56" t="s">
+      <c r="F147" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="G147" s="56"/>
-      <c r="H147" s="56"/>
-      <c r="I147" s="56" t="s">
+      <c r="G147" s="57"/>
+      <c r="H147" s="57"/>
+      <c r="I147" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="15.75">
-      <c r="A148" s="58" t="s">
+      <c r="A148" s="59" t="s">
         <v>259</v>
       </c>
-      <c r="B148" s="56" t="s">
+      <c r="B148" s="57" t="s">
         <v>264</v>
       </c>
-      <c r="C148" s="56" t="s">
+      <c r="C148" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D148" s="56" t="s">
+      <c r="D148" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E148" s="56" t="s">
+      <c r="E148" s="57" t="s">
         <v>265</v>
       </c>
-      <c r="F148" s="56" t="s">
+      <c r="F148" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G148" s="56"/>
-      <c r="H148" s="56"/>
-      <c r="I148" s="56" t="s">
+      <c r="G148" s="57"/>
+      <c r="H148" s="57"/>
+      <c r="I148" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="149" spans="1:9" ht="15.75">
-      <c r="A149" s="58" t="s">
+      <c r="A149" s="59" t="s">
         <v>259</v>
       </c>
-      <c r="B149" s="56" t="s">
+      <c r="B149" s="57" t="s">
         <v>264</v>
       </c>
-      <c r="C149" s="56" t="s">
+      <c r="C149" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="D149" s="56" t="s">
+      <c r="D149" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="E149" s="56" t="s">
+      <c r="E149" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="F149" s="56" t="s">
+      <c r="F149" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G149" s="56"/>
-      <c r="H149" s="56"/>
-      <c r="I149" s="56" t="s">
+      <c r="G149" s="57"/>
+      <c r="H149" s="57"/>
+      <c r="I149" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="150" spans="1:9" ht="15.75">
-      <c r="A150" s="58" t="s">
+      <c r="A150" s="59" t="s">
         <v>266</v>
       </c>
-      <c r="B150" s="56" t="s">
+      <c r="B150" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="C150" s="56" t="s">
+      <c r="C150" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="D150" s="56" t="s">
+      <c r="D150" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="E150" s="56" t="s">
+      <c r="E150" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="F150" s="56" t="s">
+      <c r="F150" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="G150" s="56"/>
-      <c r="H150" s="56"/>
-      <c r="I150" s="56" t="s">
+      <c r="G150" s="57"/>
+      <c r="H150" s="57"/>
+      <c r="I150" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="15.75">
-      <c r="A151" s="58" t="s">
+      <c r="A151" s="59" t="s">
         <v>266</v>
       </c>
-      <c r="B151" s="56" t="s">
+      <c r="B151" s="57" t="s">
         <v>267</v>
       </c>
-      <c r="C151" s="56" t="s">
+      <c r="C151" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="D151" s="56" t="s">
+      <c r="D151" s="57" t="s">
         <v>203</v>
       </c>
-      <c r="E151" s="56" t="s">
+      <c r="E151" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="F151" s="56" t="s">
+      <c r="F151" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="G151" s="56"/>
-      <c r="H151" s="56"/>
-      <c r="I151" s="56" t="s">
+      <c r="G151" s="57"/>
+      <c r="H151" s="57"/>
+      <c r="I151" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="15.75">
-      <c r="A152" s="58" t="s">
+      <c r="A152" s="59" t="s">
         <v>266</v>
       </c>
-      <c r="B152" s="56" t="s">
+      <c r="B152" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="C152" s="56" t="s">
+      <c r="C152" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="D152" s="56" t="s">
+      <c r="D152" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="E152" s="56" t="s">
+      <c r="E152" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="F152" s="56" t="s">
+      <c r="F152" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="G152" s="56"/>
-      <c r="H152" s="56"/>
-      <c r="I152" s="56" t="s">
+      <c r="G152" s="57"/>
+      <c r="H152" s="57"/>
+      <c r="I152" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="153" spans="1:9" ht="15.75">
-      <c r="A153" s="58" t="s">
+      <c r="A153" s="59" t="s">
         <v>266</v>
       </c>
-      <c r="B153" s="56" t="s">
+      <c r="B153" s="57" t="s">
         <v>268</v>
       </c>
-      <c r="C153" s="56" t="s">
+      <c r="C153" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D153" s="56" t="s">
+      <c r="D153" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E153" s="56" t="s">
+      <c r="E153" s="57" t="s">
         <v>265</v>
       </c>
-      <c r="F153" s="56" t="s">
+      <c r="F153" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G153" s="56"/>
-      <c r="H153" s="56"/>
-      <c r="I153" s="56" t="s">
+      <c r="G153" s="57"/>
+      <c r="H153" s="57"/>
+      <c r="I153" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="15.75">
-      <c r="A154" s="58" t="s">
+      <c r="A154" s="59" t="s">
         <v>266</v>
       </c>
-      <c r="B154" s="56" t="s">
+      <c r="B154" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="C154" s="56" t="s">
+      <c r="C154" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="D154" s="56" t="s">
+      <c r="D154" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E154" s="56" t="s">
+      <c r="E154" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="F154" s="56" t="s">
+      <c r="F154" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="G154" s="56"/>
-      <c r="H154" s="56"/>
-      <c r="I154" s="56" t="s">
+      <c r="G154" s="57"/>
+      <c r="H154" s="57"/>
+      <c r="I154" s="57" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="155" spans="1:9" ht="15.75">
-      <c r="A155" s="58" t="s">
+      <c r="A155" s="59" t="s">
         <v>266</v>
       </c>
-      <c r="B155" s="56" t="s">
+      <c r="B155" s="57" t="s">
         <v>269</v>
       </c>
-      <c r="C155" s="56" t="s">
+      <c r="C155" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="D155" s="56" t="s">
+      <c r="D155" s="57" t="s">
         <v>203</v>
       </c>
-      <c r="E155" s="56" t="s">
+      <c r="E155" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="F155" s="56" t="s">
+      <c r="F155" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="G155" s="56"/>
-      <c r="H155" s="56"/>
-      <c r="I155" s="56" t="s">
+      <c r="G155" s="57"/>
+      <c r="H155" s="57"/>
+      <c r="I155" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="156" spans="1:9" ht="15.75">
-      <c r="A156" s="58" t="s">
+      <c r="A156" s="59" t="s">
         <v>266</v>
       </c>
-      <c r="B156" s="56" t="s">
+      <c r="B156" s="57" t="s">
         <v>270</v>
       </c>
-      <c r="C156" s="56" t="s">
+      <c r="C156" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D156" s="56" t="s">
+      <c r="D156" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E156" s="56" t="s">
+      <c r="E156" s="57" t="s">
         <v>265</v>
       </c>
-      <c r="F156" s="56" t="s">
+      <c r="F156" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G156" s="56"/>
-      <c r="H156" s="56"/>
-      <c r="I156" s="56" t="s">
+      <c r="G156" s="57"/>
+      <c r="H156" s="57"/>
+      <c r="I156" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="157" spans="1:9" ht="15.75">
-      <c r="A157" s="58" t="s">
+      <c r="A157" s="59" t="s">
         <v>266</v>
       </c>
-      <c r="B157" s="56" t="s">
+      <c r="B157" s="57" t="s">
         <v>271</v>
       </c>
-      <c r="C157" s="56" t="s">
+      <c r="C157" s="57" t="s">
         <v>197</v>
       </c>
-      <c r="D157" s="56" t="s">
+      <c r="D157" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="E157" s="56" t="s">
+      <c r="E157" s="57" t="s">
         <v>199</v>
       </c>
-      <c r="F157" s="56" t="s">
+      <c r="F157" s="57" t="s">
         <v>200</v>
       </c>
-      <c r="G157" s="56"/>
-      <c r="H157" s="56"/>
-      <c r="I157" s="56" t="s">
+      <c r="G157" s="57"/>
+      <c r="H157" s="57"/>
+      <c r="I157" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="158" spans="1:9" ht="15.75">
-      <c r="A158" s="58" t="s">
+      <c r="A158" s="59" t="s">
         <v>272</v>
       </c>
-      <c r="B158" s="56" t="s">
+      <c r="B158" s="57" t="s">
         <v>273</v>
       </c>
-      <c r="C158" s="56" t="s">
+      <c r="C158" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="D158" s="56" t="s">
+      <c r="D158" s="57" t="s">
         <v>203</v>
       </c>
-      <c r="E158" s="56" t="s">
+      <c r="E158" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="F158" s="56" t="s">
+      <c r="F158" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="G158" s="56"/>
-      <c r="H158" s="56"/>
-      <c r="I158" s="56" t="s">
+      <c r="G158" s="57"/>
+      <c r="H158" s="57"/>
+      <c r="I158" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="15.75">
-      <c r="A159" s="58" t="s">
+      <c r="A159" s="59" t="s">
         <v>272</v>
       </c>
-      <c r="B159" s="56" t="s">
+      <c r="B159" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="C159" s="56" t="s">
+      <c r="C159" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D159" s="56" t="s">
+      <c r="D159" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E159" s="56" t="s">
+      <c r="E159" s="57" t="s">
         <v>265</v>
       </c>
-      <c r="F159" s="56" t="s">
+      <c r="F159" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G159" s="56"/>
-      <c r="H159" s="56"/>
-      <c r="I159" s="56" t="s">
+      <c r="G159" s="57"/>
+      <c r="H159" s="57"/>
+      <c r="I159" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="15.75">
-      <c r="A160" s="58" t="s">
+      <c r="A160" s="59" t="s">
         <v>272</v>
       </c>
-      <c r="B160" s="56" t="s">
+      <c r="B160" s="57" t="s">
         <v>274</v>
       </c>
-      <c r="C160" s="56" t="s">
+      <c r="C160" s="57" t="s">
         <v>275</v>
       </c>
-      <c r="D160" s="56" t="s">
+      <c r="D160" s="57" t="s">
         <v>276</v>
       </c>
-      <c r="E160" s="56" t="s">
+      <c r="E160" s="57" t="s">
         <v>277</v>
       </c>
-      <c r="F160" s="56" t="s">
+      <c r="F160" s="57" t="s">
         <v>164</v>
       </c>
-      <c r="G160" s="56"/>
-      <c r="H160" s="56"/>
-      <c r="I160" s="56" t="s">
+      <c r="G160" s="57"/>
+      <c r="H160" s="57"/>
+      <c r="I160" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="15.75">
-      <c r="A161" s="58" t="s">
+      <c r="A161" s="59" t="s">
         <v>278</v>
       </c>
-      <c r="B161" s="56" t="s">
+      <c r="B161" s="57" t="s">
         <v>279</v>
       </c>
-      <c r="C161" s="56" t="s">
+      <c r="C161" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="D161" s="56" t="s">
+      <c r="D161" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="E161" s="56" t="s">
+      <c r="E161" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="F161" s="56" t="s">
+      <c r="F161" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G161" s="56"/>
-      <c r="H161" s="56"/>
-      <c r="I161" s="56" t="s">
+      <c r="G161" s="57"/>
+      <c r="H161" s="57"/>
+      <c r="I161" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="15.75">
-      <c r="A162" s="58" t="s">
+      <c r="A162" s="59" t="s">
         <v>278</v>
       </c>
-      <c r="B162" s="56" t="s">
+      <c r="B162" s="57" t="s">
         <v>280</v>
       </c>
-      <c r="C162" s="56" t="s">
+      <c r="C162" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D162" s="56" t="s">
+      <c r="D162" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E162" s="56" t="s">
+      <c r="E162" s="57" t="s">
         <v>265</v>
       </c>
-      <c r="F162" s="56" t="s">
+      <c r="F162" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G162" s="56"/>
-      <c r="H162" s="56"/>
-      <c r="I162" s="56" t="s">
+      <c r="G162" s="57"/>
+      <c r="H162" s="57"/>
+      <c r="I162" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="15.75">
-      <c r="A163" s="58" t="s">
+      <c r="A163" s="59" t="s">
         <v>278</v>
       </c>
-      <c r="B163" s="56" t="s">
+      <c r="B163" s="57" t="s">
         <v>281</v>
       </c>
-      <c r="C163" s="56" t="s">
+      <c r="C163" s="57" t="s">
         <v>282</v>
       </c>
-      <c r="D163" s="56" t="s">
+      <c r="D163" s="57" t="s">
         <v>241</v>
       </c>
-      <c r="E163" s="56" t="s">
+      <c r="E163" s="57" t="s">
         <v>283</v>
       </c>
-      <c r="F163" s="56" t="s">
+      <c r="F163" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G163" s="56"/>
-      <c r="H163" s="56"/>
-      <c r="I163" s="56" t="s">
+      <c r="G163" s="57"/>
+      <c r="H163" s="57"/>
+      <c r="I163" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="164" spans="1:9" ht="15.75">
-      <c r="A164" s="58" t="s">
+      <c r="A164" s="59" t="s">
         <v>278</v>
       </c>
-      <c r="B164" s="56" t="s">
+      <c r="B164" s="57" t="s">
         <v>284</v>
       </c>
-      <c r="C164" s="56" t="s">
+      <c r="C164" s="57" t="s">
         <v>285</v>
       </c>
-      <c r="D164" s="56" t="s">
+      <c r="D164" s="57" t="s">
         <v>286</v>
       </c>
-      <c r="E164" s="56" t="s">
+      <c r="E164" s="57" t="s">
         <v>287</v>
       </c>
-      <c r="F164" s="56" t="s">
+      <c r="F164" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="G164" s="56"/>
-      <c r="H164" s="56"/>
-      <c r="I164" s="56" t="s">
+      <c r="G164" s="57"/>
+      <c r="H164" s="57"/>
+      <c r="I164" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="165" spans="1:9" ht="15.75">
-      <c r="A165" s="58" t="s">
+      <c r="A165" s="59" t="s">
         <v>278</v>
       </c>
-      <c r="B165" s="56" t="s">
+      <c r="B165" s="57" t="s">
         <v>288</v>
       </c>
-      <c r="C165" s="56" t="s">
+      <c r="C165" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="D165" s="56" t="s">
+      <c r="D165" s="57" t="s">
         <v>203</v>
       </c>
-      <c r="E165" s="56" t="s">
+      <c r="E165" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="F165" s="56" t="s">
+      <c r="F165" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="G165" s="56"/>
-      <c r="H165" s="56"/>
-      <c r="I165" s="56" t="s">
+      <c r="G165" s="57"/>
+      <c r="H165" s="57"/>
+      <c r="I165" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="166" spans="1:9" ht="15.75">
-      <c r="A166" s="58" t="s">
+      <c r="A166" s="59" t="s">
         <v>278</v>
       </c>
-      <c r="B166" s="56" t="s">
+      <c r="B166" s="57" t="s">
         <v>289</v>
       </c>
-      <c r="C166" s="56" t="s">
+      <c r="C166" s="57" t="s">
         <v>215</v>
       </c>
-      <c r="D166" s="56" t="s">
+      <c r="D166" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="E166" s="56" t="s">
+      <c r="E166" s="57" t="s">
         <v>217</v>
       </c>
-      <c r="F166" s="56" t="s">
+      <c r="F166" s="57" t="s">
         <v>290</v>
       </c>
-      <c r="G166" s="56"/>
-      <c r="H166" s="56"/>
-      <c r="I166" s="56" t="s">
+      <c r="G166" s="57"/>
+      <c r="H166" s="57"/>
+      <c r="I166" s="57" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="167" spans="1:9" ht="63">
-      <c r="A167" s="58" t="s">
+      <c r="A167" s="59" t="s">
         <v>278</v>
       </c>
-      <c r="B167" s="56" t="s">
+      <c r="B167" s="57" t="s">
         <v>291</v>
       </c>
-      <c r="C167" s="56" t="s">
+      <c r="C167" s="57" t="s">
         <v>184</v>
       </c>
-      <c r="D167" s="56" t="s">
+      <c r="D167" s="57" t="s">
         <v>185</v>
       </c>
-      <c r="E167" s="56" t="s">
+      <c r="E167" s="57" t="s">
         <v>186</v>
       </c>
-      <c r="F167" s="56" t="s">
+      <c r="F167" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="G167" s="56"/>
-      <c r="H167" s="56"/>
-      <c r="I167" s="57" t="s">
+      <c r="G167" s="57"/>
+      <c r="H167" s="57"/>
+      <c r="I167" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="168" spans="1:9" ht="15.75">
-      <c r="A168" s="58" t="s">
+      <c r="A168" s="59" t="s">
         <v>278</v>
       </c>
-      <c r="B168" s="56" t="s">
+      <c r="B168" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="C168" s="56" t="s">
+      <c r="C168" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D168" s="56" t="s">
+      <c r="D168" s="57" t="s">
         <v>165</v>
       </c>
-      <c r="E168" s="56" t="s">
+      <c r="E168" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="F168" s="56" t="s">
+      <c r="F168" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="G168" s="56"/>
-      <c r="H168" s="56"/>
-      <c r="I168" s="56" t="s">
+      <c r="G168" s="57"/>
+      <c r="H168" s="57"/>
+      <c r="I168" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="15.75">
-      <c r="A169" s="58" t="s">
+      <c r="A169" s="59" t="s">
         <v>278</v>
       </c>
-      <c r="B169" s="56" t="s">
+      <c r="B169" s="57" t="s">
         <v>292</v>
       </c>
-      <c r="C169" s="56" t="s">
+      <c r="C169" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="D169" s="56" t="s">
+      <c r="D169" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="E169" s="56" t="s">
+      <c r="E169" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="F169" s="56" t="s">
+      <c r="F169" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G169" s="56"/>
-      <c r="H169" s="56"/>
-      <c r="I169" s="56" t="s">
+      <c r="G169" s="57"/>
+      <c r="H169" s="57"/>
+      <c r="I169" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="170" spans="1:9" ht="15.75">
-      <c r="A170" s="58" t="s">
+      <c r="A170" s="59" t="s">
         <v>278</v>
       </c>
-      <c r="B170" s="56" t="s">
+      <c r="B170" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="C170" s="56" t="s">
+      <c r="C170" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D170" s="56" t="s">
+      <c r="D170" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E170" s="56" t="s">
+      <c r="E170" s="57" t="s">
         <v>265</v>
       </c>
-      <c r="F170" s="56" t="s">
+      <c r="F170" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G170" s="56"/>
-      <c r="H170" s="56"/>
-      <c r="I170" s="56" t="s">
+      <c r="G170" s="57"/>
+      <c r="H170" s="57"/>
+      <c r="I170" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="15.75">
-      <c r="A171" s="58" t="s">
+      <c r="A171" s="59" t="s">
         <v>278</v>
       </c>
-      <c r="B171" s="56" t="s">
+      <c r="B171" s="57" t="s">
         <v>293</v>
       </c>
-      <c r="C171" s="56" t="s">
+      <c r="C171" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="D171" s="56" t="s">
+      <c r="D171" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="E171" s="56" t="s">
+      <c r="E171" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="F171" s="56" t="s">
+      <c r="F171" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G171" s="56"/>
-      <c r="H171" s="56"/>
-      <c r="I171" s="56" t="s">
+      <c r="G171" s="57"/>
+      <c r="H171" s="57"/>
+      <c r="I171" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="172" spans="1:9" ht="15.75">
-      <c r="A172" s="58" t="s">
+      <c r="A172" s="59" t="s">
         <v>278</v>
       </c>
-      <c r="B172" s="56" t="s">
+      <c r="B172" s="57" t="s">
         <v>294</v>
       </c>
-      <c r="C172" s="56" t="s">
+      <c r="C172" s="57" t="s">
         <v>275</v>
       </c>
-      <c r="D172" s="56" t="s">
+      <c r="D172" s="57" t="s">
         <v>276</v>
       </c>
-      <c r="E172" s="56" t="s">
+      <c r="E172" s="57" t="s">
         <v>277</v>
       </c>
-      <c r="F172" s="56" t="s">
+      <c r="F172" s="57" t="s">
         <v>164</v>
       </c>
-      <c r="G172" s="56"/>
-      <c r="H172" s="56"/>
-      <c r="I172" s="56" t="s">
+      <c r="G172" s="57"/>
+      <c r="H172" s="57"/>
+      <c r="I172" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="63">
-      <c r="A173" s="58" t="s">
+      <c r="A173" s="59" t="s">
         <v>295</v>
       </c>
-      <c r="B173" s="56" t="s">
+      <c r="B173" s="57" t="s">
         <v>296</v>
       </c>
-      <c r="C173" s="56" t="s">
+      <c r="C173" s="57" t="s">
         <v>184</v>
       </c>
-      <c r="D173" s="56" t="s">
+      <c r="D173" s="57" t="s">
         <v>185</v>
       </c>
-      <c r="E173" s="56" t="s">
+      <c r="E173" s="57" t="s">
         <v>186</v>
       </c>
-      <c r="F173" s="56" t="s">
+      <c r="F173" s="57" t="s">
         <v>297</v>
       </c>
-      <c r="G173" s="56"/>
-      <c r="H173" s="56"/>
-      <c r="I173" s="57" t="s">
+      <c r="G173" s="57"/>
+      <c r="H173" s="57"/>
+      <c r="I173" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="174" spans="1:9" ht="78.75">
-      <c r="A174" s="58" t="s">
+      <c r="A174" s="59" t="s">
         <v>295</v>
       </c>
-      <c r="B174" s="56" t="s">
+      <c r="B174" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="C174" s="56" t="s">
+      <c r="C174" s="57" t="s">
         <v>275</v>
       </c>
-      <c r="D174" s="56" t="s">
+      <c r="D174" s="57" t="s">
         <v>276</v>
       </c>
-      <c r="E174" s="56" t="s">
+      <c r="E174" s="57" t="s">
         <v>277</v>
       </c>
-      <c r="F174" s="56" t="s">
+      <c r="F174" s="57" t="s">
         <v>164</v>
       </c>
-      <c r="G174" s="56" t="s">
+      <c r="G174" s="57" t="s">
         <v>298</v>
       </c>
-      <c r="H174" s="57" t="s">
+      <c r="H174" s="58" t="s">
         <v>299</v>
       </c>
-      <c r="I174" s="57" t="s">
+      <c r="I174" s="58" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="175" spans="1:9" ht="15.75">
-      <c r="A175" s="58" t="s">
+      <c r="A175" s="59" t="s">
         <v>295</v>
       </c>
-      <c r="B175" s="56" t="s">
+      <c r="B175" s="57" t="s">
         <v>301</v>
       </c>
-      <c r="C175" s="56" t="s">
+      <c r="C175" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D175" s="56" t="s">
+      <c r="D175" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E175" s="56" t="s">
+      <c r="E175" s="57" t="s">
         <v>265</v>
       </c>
-      <c r="F175" s="56" t="s">
+      <c r="F175" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G175" s="56"/>
-      <c r="H175" s="56"/>
-      <c r="I175" s="56" t="s">
+      <c r="G175" s="57"/>
+      <c r="H175" s="57"/>
+      <c r="I175" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="176" spans="1:9" ht="78.75">
-      <c r="A176" s="58" t="s">
+      <c r="A176" s="59" t="s">
         <v>295</v>
       </c>
-      <c r="B176" s="56" t="s">
+      <c r="B176" s="57" t="s">
         <v>302</v>
       </c>
-      <c r="C176" s="56" t="s">
+      <c r="C176" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="D176" s="56" t="s">
+      <c r="D176" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="E176" s="56" t="s">
+      <c r="E176" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="F176" s="56" t="s">
+      <c r="F176" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G176" s="56" t="s">
+      <c r="G176" s="57" t="s">
         <v>303</v>
       </c>
-      <c r="H176" s="57" t="s">
+      <c r="H176" s="58" t="s">
         <v>304</v>
       </c>
-      <c r="I176" s="57" t="s">
+      <c r="I176" s="58" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="177" spans="1:9" ht="15.75">
-      <c r="A177" s="58" t="s">
+      <c r="A177" s="59" t="s">
         <v>306</v>
       </c>
-      <c r="B177" s="56" t="s">
+      <c r="B177" s="57" t="s">
         <v>307</v>
       </c>
-      <c r="C177" s="56" t="s">
+      <c r="C177" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="D177" s="56" t="s">
+      <c r="D177" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E177" s="56" t="s">
+      <c r="E177" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="F177" s="56" t="s">
+      <c r="F177" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="G177" s="56"/>
-      <c r="H177" s="56"/>
-      <c r="I177" s="56" t="s">
+      <c r="G177" s="57"/>
+      <c r="H177" s="57"/>
+      <c r="I177" s="57" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="178" spans="1:9" ht="15.75">
-      <c r="A178" s="58" t="s">
+      <c r="A178" s="59" t="s">
         <v>295</v>
       </c>
-      <c r="B178" s="56" t="s">
+      <c r="B178" s="57" t="s">
         <v>264</v>
       </c>
-      <c r="C178" s="56" t="s">
+      <c r="C178" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="D178" s="56" t="s">
+      <c r="D178" s="57" t="s">
         <v>162</v>
       </c>
-      <c r="E178" s="56" t="s">
+      <c r="E178" s="57" t="s">
         <v>163</v>
       </c>
-      <c r="F178" s="56" t="s">
+      <c r="F178" s="57" t="s">
         <v>164</v>
       </c>
-      <c r="G178" s="56"/>
-      <c r="H178" s="56"/>
-      <c r="I178" s="56" t="s">
+      <c r="G178" s="57"/>
+      <c r="H178" s="57"/>
+      <c r="I178" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="179" spans="1:9" ht="15.75">
-      <c r="A179" s="58" t="s">
+      <c r="A179" s="59" t="s">
         <v>295</v>
       </c>
-      <c r="B179" s="56" t="s">
+      <c r="B179" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="C179" s="56" t="s">
+      <c r="C179" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D179" s="56" t="s">
+      <c r="D179" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E179" s="56" t="s">
+      <c r="E179" s="57" t="s">
         <v>265</v>
       </c>
-      <c r="F179" s="56" t="s">
+      <c r="F179" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G179" s="56"/>
-      <c r="H179" s="56"/>
-      <c r="I179" s="56" t="s">
+      <c r="G179" s="57"/>
+      <c r="H179" s="57"/>
+      <c r="I179" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="180" spans="1:9" ht="15.75">
-      <c r="A180" s="58" t="s">
+      <c r="A180" s="59" t="s">
         <v>295</v>
       </c>
-      <c r="B180" s="56" t="s">
+      <c r="B180" s="57" t="s">
         <v>308</v>
       </c>
-      <c r="C180" s="56" t="s">
+      <c r="C180" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="D180" s="56" t="s">
+      <c r="D180" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="E180" s="56" t="s">
+      <c r="E180" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="F180" s="56" t="s">
+      <c r="F180" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G180" s="56"/>
-      <c r="H180" s="56"/>
-      <c r="I180" s="56" t="s">
+      <c r="G180" s="57"/>
+      <c r="H180" s="57"/>
+      <c r="I180" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="181" spans="1:9" ht="15.75">
-      <c r="A181" s="58" t="s">
+      <c r="A181" s="59" t="s">
         <v>309</v>
       </c>
-      <c r="B181" s="56" t="s">
+      <c r="B181" s="57" t="s">
         <v>310</v>
       </c>
-      <c r="C181" s="56" t="s">
+      <c r="C181" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="D181" s="56" t="s">
+      <c r="D181" s="57" t="s">
         <v>162</v>
       </c>
-      <c r="E181" s="56" t="s">
+      <c r="E181" s="57" t="s">
         <v>163</v>
       </c>
-      <c r="F181" s="56" t="s">
+      <c r="F181" s="57" t="s">
         <v>164</v>
       </c>
-      <c r="G181" s="56"/>
-      <c r="H181" s="56"/>
-      <c r="I181" s="56" t="s">
+      <c r="G181" s="57"/>
+      <c r="H181" s="57"/>
+      <c r="I181" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="15.75">
-      <c r="A182" s="58" t="s">
+      <c r="A182" s="59" t="s">
         <v>309</v>
       </c>
-      <c r="B182" s="56"/>
-      <c r="C182" s="56"/>
-      <c r="D182" s="56"/>
-      <c r="E182" s="56"/>
-      <c r="F182" s="56"/>
-      <c r="G182" s="56"/>
-      <c r="H182" s="56"/>
-      <c r="I182" s="56"/>
+      <c r="B182" s="57"/>
+      <c r="C182" s="57"/>
+      <c r="D182" s="57"/>
+      <c r="E182" s="57"/>
+      <c r="F182" s="57"/>
+      <c r="G182" s="57"/>
+      <c r="H182" s="57"/>
+      <c r="I182" s="57"/>
     </row>
     <row r="183" spans="1:9" ht="63">
-      <c r="A183" s="58" t="s">
+      <c r="A183" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="B183" s="56" t="s">
+      <c r="B183" s="57" t="s">
         <v>312</v>
       </c>
-      <c r="C183" s="56" t="s">
+      <c r="C183" s="57" t="s">
         <v>184</v>
       </c>
-      <c r="D183" s="56" t="s">
+      <c r="D183" s="57" t="s">
         <v>185</v>
       </c>
-      <c r="E183" s="56" t="s">
+      <c r="E183" s="57" t="s">
         <v>186</v>
       </c>
-      <c r="F183" s="56" t="s">
+      <c r="F183" s="57" t="s">
         <v>297</v>
       </c>
-      <c r="G183" s="56"/>
-      <c r="H183" s="56"/>
-      <c r="I183" s="57" t="s">
+      <c r="G183" s="57"/>
+      <c r="H183" s="57"/>
+      <c r="I183" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="184" spans="1:9" ht="15.75">
-      <c r="A184" s="58" t="s">
+      <c r="A184" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="B184" s="56" t="s">
+      <c r="B184" s="57" t="s">
         <v>313</v>
       </c>
-      <c r="C184" s="56" t="s">
+      <c r="C184" s="57" t="s">
         <v>140</v>
       </c>
-      <c r="D184" s="56" t="s">
+      <c r="D184" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="E184" s="56" t="s">
+      <c r="E184" s="57" t="s">
         <v>142</v>
       </c>
-      <c r="F184" s="56" t="s">
+      <c r="F184" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="G184" s="56"/>
-      <c r="H184" s="56"/>
-      <c r="I184" s="56" t="s">
+      <c r="G184" s="57"/>
+      <c r="H184" s="57"/>
+      <c r="I184" s="57" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="15.75">
-      <c r="A185" s="58" t="s">
+      <c r="A185" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="B185" s="56" t="s">
+      <c r="B185" s="57" t="s">
         <v>274</v>
       </c>
-      <c r="C185" s="56" t="s">
+      <c r="C185" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D185" s="56" t="s">
+      <c r="D185" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E185" s="56" t="s">
+      <c r="E185" s="57" t="s">
         <v>265</v>
       </c>
-      <c r="F185" s="56" t="s">
+      <c r="F185" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G185" s="56"/>
-      <c r="H185" s="56"/>
-      <c r="I185" s="56" t="s">
+      <c r="G185" s="57"/>
+      <c r="H185" s="57"/>
+      <c r="I185" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="186" spans="1:9" ht="15.75">
-      <c r="A186" s="58" t="s">
+      <c r="A186" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="B186" s="56" t="s">
+      <c r="B186" s="57" t="s">
         <v>314</v>
       </c>
-      <c r="C186" s="56" t="s">
+      <c r="C186" s="57" t="s">
         <v>197</v>
       </c>
-      <c r="D186" s="56" t="s">
+      <c r="D186" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="E186" s="56" t="s">
+      <c r="E186" s="57" t="s">
         <v>199</v>
       </c>
-      <c r="F186" s="56" t="s">
+      <c r="F186" s="57" t="s">
         <v>200</v>
       </c>
-      <c r="G186" s="56"/>
-      <c r="H186" s="56"/>
-      <c r="I186" s="56" t="s">
+      <c r="G186" s="57"/>
+      <c r="H186" s="57"/>
+      <c r="I186" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="187" spans="1:9" ht="15.75">
-      <c r="A187" s="58" t="s">
+      <c r="A187" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="B187" s="56" t="s">
+      <c r="B187" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="C187" s="56" t="s">
+      <c r="C187" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="D187" s="56" t="s">
+      <c r="D187" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="E187" s="56" t="s">
+      <c r="E187" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="F187" s="56" t="s">
+      <c r="F187" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="G187" s="56"/>
-      <c r="H187" s="56"/>
-      <c r="I187" s="56" t="s">
+      <c r="G187" s="57"/>
+      <c r="H187" s="57"/>
+      <c r="I187" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="188" spans="1:9" ht="15.75">
-      <c r="A188" s="58" t="s">
+      <c r="A188" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="B188" s="56" t="s">
+      <c r="B188" s="57" t="s">
         <v>315</v>
       </c>
-      <c r="C188" s="56" t="s">
+      <c r="C188" s="57" t="s">
         <v>184</v>
       </c>
-      <c r="D188" s="56" t="s">
+      <c r="D188" s="57" t="s">
         <v>185</v>
       </c>
-      <c r="E188" s="56" t="s">
+      <c r="E188" s="57" t="s">
         <v>186</v>
       </c>
-      <c r="F188" s="56"/>
-      <c r="G188" s="56"/>
-      <c r="H188" s="56"/>
-      <c r="I188" s="56" t="s">
+      <c r="F188" s="57"/>
+      <c r="G188" s="57"/>
+      <c r="H188" s="57"/>
+      <c r="I188" s="57" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="189" spans="1:9" ht="15.75">
-      <c r="A189" s="58" t="s">
+      <c r="A189" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="B189" s="56" t="s">
+      <c r="B189" s="57" t="s">
         <v>270</v>
       </c>
-      <c r="C189" s="56" t="s">
+      <c r="C189" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D189" s="56" t="s">
+      <c r="D189" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="E189" s="56" t="s">
+      <c r="E189" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="F189" s="56" t="s">
+      <c r="F189" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="G189" s="56"/>
-      <c r="H189" s="56"/>
-      <c r="I189" s="56" t="s">
+      <c r="G189" s="57"/>
+      <c r="H189" s="57"/>
+      <c r="I189" s="57" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="190" spans="1:9" ht="15.75">
-      <c r="A190" s="58" t="s">
+      <c r="A190" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="B190" s="56" t="s">
+      <c r="B190" s="57" t="s">
         <v>316</v>
       </c>
-      <c r="C190" s="56" t="s">
+      <c r="C190" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="D190" s="56" t="s">
+      <c r="D190" s="57" t="s">
         <v>317</v>
       </c>
-      <c r="E190" s="56" t="s">
+      <c r="E190" s="57" t="s">
         <v>318</v>
       </c>
-      <c r="F190" s="56" t="s">
+      <c r="F190" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G190" s="56"/>
-      <c r="H190" s="56"/>
-      <c r="I190" s="56" t="s">
+      <c r="G190" s="57"/>
+      <c r="H190" s="57"/>
+      <c r="I190" s="57" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="191" spans="1:9" ht="15.75">
-      <c r="A191" s="58" t="s">
+      <c r="A191" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="B191" s="56" t="s">
+      <c r="B191" s="57" t="s">
         <v>316</v>
       </c>
-      <c r="C191" s="56" t="s">
+      <c r="C191" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="D191" s="56" t="s">
+      <c r="D191" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E191" s="56" t="s">
+      <c r="E191" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="F191" s="56" t="s">
+      <c r="F191" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="G191" s="56"/>
-      <c r="H191" s="56"/>
-      <c r="I191" s="56" t="s">
+      <c r="G191" s="57"/>
+      <c r="H191" s="57"/>
+      <c r="I191" s="57" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="192" spans="1:9" ht="15.75">
-      <c r="A192" s="58" t="s">
+      <c r="A192" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="B192" s="56" t="s">
+      <c r="B192" s="57" t="s">
         <v>319</v>
       </c>
-      <c r="C192" s="56" t="s">
+      <c r="C192" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="D192" s="56" t="s">
+      <c r="D192" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="E192" s="56" t="s">
+      <c r="E192" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="F192" s="56" t="s">
+      <c r="F192" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G192" s="56"/>
-      <c r="H192" s="56"/>
-      <c r="I192" s="56"/>
+      <c r="G192" s="57"/>
+      <c r="H192" s="57"/>
+      <c r="I192" s="57"/>
     </row>
     <row r="193" spans="1:9" ht="15.75">
-      <c r="A193" s="58" t="s">
+      <c r="A193" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="B193" s="56" t="s">
+      <c r="B193" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="C193" s="56" t="s">
+      <c r="C193" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="D193" s="56" t="s">
+      <c r="D193" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E193" s="56" t="s">
+      <c r="E193" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="F193" s="56" t="s">
+      <c r="F193" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="G193" s="56"/>
-      <c r="H193" s="56"/>
-      <c r="I193" s="56" t="s">
+      <c r="G193" s="57"/>
+      <c r="H193" s="57"/>
+      <c r="I193" s="57" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="194" spans="1:9" ht="15.75">
-      <c r="A194" s="58" t="s">
+      <c r="A194" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="B194" s="56" t="s">
+      <c r="B194" s="57" t="s">
         <v>320</v>
       </c>
-      <c r="C194" s="56" t="s">
+      <c r="C194" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="D194" s="56" t="s">
+      <c r="D194" s="57" t="s">
         <v>203</v>
       </c>
-      <c r="E194" s="56" t="s">
+      <c r="E194" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="F194" s="56" t="s">
+      <c r="F194" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="G194" s="56"/>
-      <c r="H194" s="56"/>
-      <c r="I194" s="56" t="s">
+      <c r="G194" s="57"/>
+      <c r="H194" s="57"/>
+      <c r="I194" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="195" spans="1:9" ht="15.75">
-      <c r="A195" s="58" t="s">
+      <c r="A195" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="B195" s="56" t="s">
+      <c r="B195" s="57" t="s">
         <v>321</v>
       </c>
-      <c r="C195" s="56" t="s">
+      <c r="C195" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="D195" s="56" t="s">
+      <c r="D195" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="E195" s="56" t="s">
+      <c r="E195" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="F195" s="56" t="s">
+      <c r="F195" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G195" s="56"/>
-      <c r="H195" s="56"/>
-      <c r="I195" s="56" t="s">
+      <c r="G195" s="57"/>
+      <c r="H195" s="57"/>
+      <c r="I195" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="196" spans="1:9" ht="15.75">
-      <c r="A196" s="58" t="s">
+      <c r="A196" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="B196" s="56" t="s">
+      <c r="B196" s="57" t="s">
         <v>321</v>
       </c>
-      <c r="C196" s="56" t="s">
+      <c r="C196" s="57" t="s">
         <v>169</v>
       </c>
-      <c r="D196" s="56" t="s">
+      <c r="D196" s="57" t="s">
         <v>322</v>
       </c>
-      <c r="E196" s="56" t="s">
+      <c r="E196" s="57" t="s">
         <v>171</v>
       </c>
-      <c r="F196" s="56" t="s">
+      <c r="F196" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="G196" s="56"/>
-      <c r="H196" s="56"/>
-      <c r="I196" s="56" t="s">
+      <c r="G196" s="57"/>
+      <c r="H196" s="57"/>
+      <c r="I196" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="197" spans="1:9" ht="15.75">
-      <c r="A197" s="58" t="s">
+      <c r="A197" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="B197" s="56" t="s">
+      <c r="B197" s="57" t="s">
         <v>323</v>
       </c>
-      <c r="C197" s="56" t="s">
+      <c r="C197" s="57" t="s">
         <v>282</v>
       </c>
-      <c r="D197" s="56" t="s">
+      <c r="D197" s="57" t="s">
         <v>241</v>
       </c>
-      <c r="E197" s="56" t="s">
+      <c r="E197" s="57" t="s">
         <v>283</v>
       </c>
-      <c r="F197" s="56" t="s">
+      <c r="F197" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G197" s="56"/>
-      <c r="H197" s="56"/>
-      <c r="I197" s="56" t="s">
+      <c r="G197" s="57"/>
+      <c r="H197" s="57"/>
+      <c r="I197" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="198" spans="1:9" ht="15.75">
-      <c r="A198" s="58" t="s">
+      <c r="A198" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="B198" s="56" t="s">
+      <c r="B198" s="57" t="s">
         <v>324</v>
       </c>
-      <c r="C198" s="56" t="s">
+      <c r="C198" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="D198" s="56" t="s">
+      <c r="D198" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="E198" s="56" t="s">
+      <c r="E198" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="F198" s="56" t="s">
+      <c r="F198" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G198" s="56"/>
-      <c r="H198" s="56"/>
-      <c r="I198" s="56" t="s">
+      <c r="G198" s="57"/>
+      <c r="H198" s="57"/>
+      <c r="I198" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="199" spans="1:9" ht="15.75">
-      <c r="A199" s="58" t="s">
+      <c r="A199" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="B199" s="56" t="s">
+      <c r="B199" s="57" t="s">
         <v>160</v>
       </c>
-      <c r="C199" s="56" t="s">
+      <c r="C199" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D199" s="56" t="s">
+      <c r="D199" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E199" s="56" t="s">
+      <c r="E199" s="57" t="s">
         <v>265</v>
       </c>
-      <c r="F199" s="56" t="s">
+      <c r="F199" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G199" s="56"/>
-      <c r="H199" s="56"/>
-      <c r="I199" s="56" t="s">
+      <c r="G199" s="57"/>
+      <c r="H199" s="57"/>
+      <c r="I199" s="57" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="200" spans="1:9" ht="15.75">
-      <c r="A200" s="58" t="s">
+      <c r="A200" s="59" t="s">
         <v>325</v>
       </c>
-      <c r="B200" s="56" t="s">
+      <c r="B200" s="57" t="s">
         <v>326</v>
       </c>
-      <c r="C200" s="56" t="s">
+      <c r="C200" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="D200" s="56" t="s">
+      <c r="D200" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="E200" s="56" t="s">
+      <c r="E200" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="F200" s="56" t="s">
+      <c r="F200" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="G200" s="56"/>
-      <c r="H200" s="56"/>
-      <c r="I200" s="56" t="s">
+      <c r="G200" s="57"/>
+      <c r="H200" s="57"/>
+      <c r="I200" s="57" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="201" spans="1:9" ht="15.75">
-      <c r="A201" s="58" t="s">
+      <c r="A201" s="59" t="s">
         <v>325</v>
       </c>
-      <c r="B201" s="56" t="s">
+      <c r="B201" s="57" t="s">
         <v>327</v>
       </c>
-      <c r="C201" s="56" t="s">
+      <c r="C201" s="57" t="s">
         <v>177</v>
       </c>
-      <c r="D201" s="56" t="s">
+      <c r="D201" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="E201" s="56" t="s">
+      <c r="E201" s="57" t="s">
         <v>328</v>
       </c>
-      <c r="F201" s="56" t="s">
+      <c r="F201" s="57" t="s">
         <v>329</v>
       </c>
-      <c r="G201" s="56"/>
-      <c r="H201" s="56"/>
-      <c r="I201" s="56" t="s">
+      <c r="G201" s="57"/>
+      <c r="H201" s="57"/>
+      <c r="I201" s="57" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="202" spans="1:9" ht="15.75">
-      <c r="A202" s="58" t="s">
+      <c r="A202" s="59" t="s">
         <v>325</v>
       </c>
-      <c r="B202" s="56" t="s">
+      <c r="B202" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="C202" s="56" t="s">
+      <c r="C202" s="57" t="s">
         <v>330</v>
       </c>
-      <c r="D202" s="56" t="s">
+      <c r="D202" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="E202" s="56" t="s">
+      <c r="E202" s="57" t="s">
         <v>331</v>
       </c>
-      <c r="F202" s="56" t="s">
+      <c r="F202" s="57" t="s">
         <v>332</v>
       </c>
-      <c r="G202" s="56"/>
-      <c r="H202" s="56"/>
-      <c r="I202" s="56" t="s">
+      <c r="G202" s="57"/>
+      <c r="H202" s="57"/>
+      <c r="I202" s="57" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="203" spans="1:9" ht="15.75">
-      <c r="A203" s="58" t="s">
+      <c r="A203" s="59" t="s">
         <v>325</v>
       </c>
-      <c r="B203" s="56" t="s">
+      <c r="B203" s="57" t="s">
         <v>334</v>
       </c>
-      <c r="C203" s="56" t="s">
+      <c r="C203" s="57" t="s">
         <v>335</v>
       </c>
-      <c r="D203" s="56" t="s">
+      <c r="D203" s="57" t="s">
         <v>203</v>
       </c>
-      <c r="E203" s="56" t="s">
+      <c r="E203" s="57" t="s">
         <v>336</v>
       </c>
-      <c r="F203" s="56" t="s">
+      <c r="F203" s="57" t="s">
         <v>337</v>
       </c>
-      <c r="G203" s="56"/>
-      <c r="H203" s="56"/>
-      <c r="I203" s="56" t="s">
+      <c r="G203" s="57"/>
+      <c r="H203" s="57"/>
+      <c r="I203" s="57" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="204" spans="1:9" ht="15.75">
-      <c r="A204" s="58" t="s">
+      <c r="A204" s="59" t="s">
         <v>325</v>
       </c>
-      <c r="B204" s="56" t="s">
+      <c r="B204" s="57" t="s">
         <v>261</v>
       </c>
-      <c r="C204" s="56" t="s">
+      <c r="C204" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="D204" s="56" t="s">
+      <c r="D204" s="57" t="s">
         <v>333</v>
       </c>
-      <c r="E204" s="56" t="s">
+      <c r="E204" s="57" t="s">
         <v>338</v>
       </c>
-      <c r="F204" s="56" t="s">
+      <c r="F204" s="57" t="s">
         <v>339</v>
       </c>
-      <c r="G204" s="56"/>
-      <c r="H204" s="56"/>
-      <c r="I204" s="56" t="s">
+      <c r="G204" s="57"/>
+      <c r="H204" s="57"/>
+      <c r="I204" s="57" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" ht="15.75">
+      <c r="A205" s="59" t="s">
+        <v>342</v>
+      </c>
+      <c r="B205" s="57" t="s">
+        <v>85</v>
+      </c>
+      <c r="C205" s="57" t="s">
+        <v>215</v>
+      </c>
+      <c r="D205" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="E205" s="57" t="s">
+        <v>340</v>
+      </c>
+      <c r="F205" s="57" t="s">
+        <v>341</v>
+      </c>
+      <c r="G205" s="57"/>
+      <c r="H205" s="57"/>
+      <c r="I205" s="57" t="s">
         <v>256</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes to be committed: 	modified:   Libro1.xlsx 	modified:   index.html 	modified:   src/charts.js 	modified:   src/charts3.js 	modified:   styless/header.css
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -7,16 +7,16 @@
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Estadística Marzo" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Estadistica Abril" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="343">
   <si>
     <t>LA FRIA</t>
   </si>
@@ -19766,6 +19766,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -19778,7 +19779,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$C$1:$C$1</c:f>
+              <c:f>'Estadística Marzo'!$C$1:$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -19789,7 +19790,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$A$2:$A$37</c:f>
+              <c:f>'Estadística Marzo'!$A$2:$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
@@ -19905,7 +19906,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$2:$C$37</c:f>
+              <c:f>'Estadística Marzo'!$C$2:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
@@ -20000,6 +20001,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -20029,6 +20031,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -20043,7 +20046,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$B$1</c:f>
+              <c:f>'Estadística Marzo'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -20055,7 +20058,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$A$2:$A$37</c:f>
+              <c:f>'Estadística Marzo'!$A$2:$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
@@ -20171,7 +20174,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$B$37</c:f>
+              <c:f>'Estadística Marzo'!$B$2:$B$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="36"/>
@@ -20296,6 +20299,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -20325,6 +20329,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -20339,7 +20344,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$C$1</c:f>
+              <c:f>'Estadística Marzo'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -20358,7 +20363,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$A$2:$A$37</c:f>
+              <c:f>'Estadística Marzo'!$A$2:$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
@@ -20474,7 +20479,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$2:$C$39</c:f>
+              <c:f>'Estadística Marzo'!$C$2:$C$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="38"/>
@@ -20605,6 +20610,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -21007,8 +21013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C37"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -21391,19 +21397,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E33" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132:I153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" customWidth="1"/>
     <col min="8" max="8" width="17.140625" customWidth="1"/>
     <col min="9" max="9" width="30.28515625" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="43" customWidth="1"/>
     <col min="14" max="14" width="18.42578125" customWidth="1"/>
   </cols>
@@ -27306,12 +27312,384 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.73</v>
+      </c>
+      <c r="C2" s="56">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.12</v>
+      </c>
+      <c r="C3" s="56">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="C5" s="56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C6" s="56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="C7" s="56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="C8" s="56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="C9" s="56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="56"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="C11" s="56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="56"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.73</v>
+      </c>
+      <c r="C13" s="56">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="C14" s="56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="C15" s="56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="56"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="56"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="56"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="56"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="C20" s="56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0.22</v>
+      </c>
+      <c r="C21" s="56">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C22" s="56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="56"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="C24" s="56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="C25" s="56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="56"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="5">
+        <v>0.12</v>
+      </c>
+      <c r="C27" s="56">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C28" s="56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="C29" s="56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C30" s="56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="C31" s="56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="56"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="C33" s="56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="56"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="56"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="C36" s="56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="56">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="C38">
+        <f>SUM(C2:C37)</f>
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes to be committed: 	modified:   Libro1.xlsx 	modified:   src/weekly.js 	modified:   styless/header.css 	deleted:    ~$Libro1.xlsx
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="360">
   <si>
     <t>LA FRIA</t>
   </si>
@@ -1038,13 +1038,64 @@
     <t>1211</t>
   </si>
   <si>
-    <t>BANFA-9900</t>
-  </si>
-  <si>
-    <t>1212</t>
-  </si>
-  <si>
     <t>21/04/2025</t>
+  </si>
+  <si>
+    <t>9:05</t>
+  </si>
+  <si>
+    <t>585155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yorman Naveda </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se hicieron pruebas de primer nivel, se creó el ticket nro. 585155. El analista de cantv indico que se encontraban puertos inhibidos, reliazo reinicios de puertos. Agencia activa. </t>
+  </si>
+  <si>
+    <t>585178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freider  Cedeño </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se hicieron pruebas de primer nivel, se creó el ticket nro. 585178. El analista de cantv indico que se encuentra con falla de intermitencia.  Indico fallas al personal de datos. </t>
+  </si>
+  <si>
+    <t>585186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se hicieron pruebas de primer nivel, se creó el ticket nro. 585186. El analista de cantv indico que se encuentra con falla de intermitencia.  Indico fallas al personal de datos. </t>
+  </si>
+  <si>
+    <t>2:35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin servicio, a la espera de realizar pruebas de primer nivel </t>
+  </si>
+  <si>
+    <t>2:36</t>
+  </si>
+  <si>
+    <t>Abril %</t>
+  </si>
+  <si>
+    <t>Semana 1</t>
+  </si>
+  <si>
+    <t>Lunes</t>
+  </si>
+  <si>
+    <t>Martes</t>
+  </si>
+  <si>
+    <t>Miércoles</t>
+  </si>
+  <si>
+    <t>Jueves</t>
+  </si>
+  <si>
+    <t>Viernes</t>
   </si>
 </sst>
 </file>
@@ -1726,7 +1777,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -2149,6 +2200,54 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -10862,7 +10961,7 @@
     <xf numFmtId="0" fontId="45" fillId="0" borderId="31"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -11028,6 +11127,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8704">
     <cellStyle name="20% - Énfasis1 1" xfId="3"/>
@@ -19739,8 +19862,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFF4EF"/>
       <color rgb="FFAFD7FF"/>
-      <color rgb="FFFFF4EF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -19766,272 +19889,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:doughnutChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Estadística Marzo'!$C$1:$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>TOTAL DE FALLAS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Estadística Marzo'!$A$2:$A$37</c:f>
-              <c:strCache>
-                <c:ptCount val="36"/>
-                <c:pt idx="0">
-                  <c:v>LA FRIA</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>BARINAS</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>PRTO. ORDAZ</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>MARACAY</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>BARCELONA</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>CIUDAD BOLIVAR</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>VALENCIA</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>PRTO. CABELLO</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>PTO. FIJO</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>LARA</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>HOSP. MLTR. SAN CRISTOBAL</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>SAN CRISTOBAL</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>MARACAIBO</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>ZULIA</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>MNRO. DE LA DEFENSA</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>ACADEMIA MILITAR</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>CANES</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>C.G GNB</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>GUARICO</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>PORTUGUESA</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>APURE</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>MIRANDA</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>MONAGAS</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>DTA. AMACURO</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>NVA. ESPARTA</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>SUCRE</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>TRUJILLO</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>MERIDA</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>YARACUY</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>COJEDES</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>AMAZONAS</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>ALTOS MIRANDINOS</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>HOSP. MLTR. DR. CARLOS AREVALO</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>RAMO VERDE</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>CARUPANO</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>CIRCULO MILITAR</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Estadística Marzo'!$C$2:$C$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
-                <c:pt idx="0">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
-        <c:firstSliceAng val="0"/>
-        <c:holeSize val="50"/>
-      </c:doughnutChart>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-VE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -20260,11 +20117,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="193213568"/>
-        <c:axId val="193215104"/>
+        <c:axId val="193960576"/>
+        <c:axId val="193970560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="193213568"/>
+        <c:axId val="193960576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20273,7 +20130,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193215104"/>
+        <c:crossAx val="193970560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20281,7 +20138,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193215104"/>
+        <c:axId val="193970560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20292,14 +20149,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193213568"/>
+        <c:crossAx val="193960576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -20314,7 +20170,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-VE"/>
@@ -20329,7 +20185,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -20571,11 +20426,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="193260160"/>
-        <c:axId val="195625344"/>
+        <c:axId val="193999232"/>
+        <c:axId val="194000768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="193260160"/>
+        <c:axId val="193999232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20584,7 +20439,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195625344"/>
+        <c:crossAx val="194000768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20592,7 +20447,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195625344"/>
+        <c:axId val="194000768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20603,14 +20458,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193260160"/>
+        <c:crossAx val="193999232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -20627,36 +20481,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>53975</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>349250</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="1 Gráfico"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -20683,7 +20507,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -20715,7 +20539,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -21013,8 +20837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C38"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -21395,10 +21219,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N205"/>
+  <dimension ref="A1:N210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="A132" sqref="A132:I153"/>
+    <sheetView tabSelected="1" topLeftCell="E206" workbookViewId="0">
+      <selection activeCell="M207" sqref="M207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -21407,7 +21231,7 @@
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="34.5703125" customWidth="1"/>
     <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
     <col min="9" max="9" width="30.28515625" customWidth="1"/>
     <col min="11" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="43" customWidth="1"/>
@@ -21481,7 +21305,7 @@
         <v>0</v>
       </c>
       <c r="N2" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D2)</f>
+        <f>COUNTIFS(A131:A210,J2,D131:D210, D2)</f>
         <v>0</v>
       </c>
     </row>
@@ -21517,7 +21341,7 @@
         <v>38</v>
       </c>
       <c r="N3" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D9)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D9)</f>
         <v>0</v>
       </c>
     </row>
@@ -21553,7 +21377,7 @@
         <v>239</v>
       </c>
       <c r="N4" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, K131)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, K131)</f>
         <v>0</v>
       </c>
     </row>
@@ -21589,7 +21413,7 @@
         <v>11</v>
       </c>
       <c r="N5" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205,D181)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204,D181)</f>
         <v>0</v>
       </c>
     </row>
@@ -21625,7 +21449,7 @@
         <v>2</v>
       </c>
       <c r="N6" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D31)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D31)</f>
         <v>0</v>
       </c>
     </row>
@@ -21661,7 +21485,7 @@
         <v>3</v>
       </c>
       <c r="N7" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D139)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D139)</f>
         <v>0</v>
       </c>
     </row>
@@ -21697,7 +21521,7 @@
         <v>4</v>
       </c>
       <c r="N8" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D11)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D11)</f>
         <v>0</v>
       </c>
     </row>
@@ -21733,7 +21557,7 @@
         <v>240</v>
       </c>
       <c r="N9" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D84)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D84)</f>
         <v>0</v>
       </c>
     </row>
@@ -21769,7 +21593,7 @@
         <v>241</v>
       </c>
       <c r="N10" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D197)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D197)</f>
         <v>0</v>
       </c>
     </row>
@@ -21805,7 +21629,7 @@
         <v>7</v>
       </c>
       <c r="N11" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D33)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D33)</f>
         <v>0</v>
       </c>
     </row>
@@ -21841,7 +21665,7 @@
         <v>242</v>
       </c>
       <c r="N12" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205,L28)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204,L28)</f>
         <v>0</v>
       </c>
     </row>
@@ -21877,7 +21701,7 @@
         <v>9</v>
       </c>
       <c r="N13" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D14)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D14)</f>
         <v>0</v>
       </c>
     </row>
@@ -21913,7 +21737,7 @@
         <v>10</v>
       </c>
       <c r="N14" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205,D59)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204,D59)</f>
         <v>0</v>
       </c>
     </row>
@@ -21949,7 +21773,7 @@
         <v>12</v>
       </c>
       <c r="N15" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D32)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D32)</f>
         <v>0</v>
       </c>
     </row>
@@ -21985,7 +21809,7 @@
         <v>243</v>
       </c>
       <c r="N16" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, K29)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, K29)</f>
         <v>0</v>
       </c>
     </row>
@@ -22021,7 +21845,7 @@
         <v>14</v>
       </c>
       <c r="N17" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, J33)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, J33)</f>
         <v>0</v>
       </c>
     </row>
@@ -22057,7 +21881,7 @@
         <v>15</v>
       </c>
       <c r="N18" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, K147)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, K147)</f>
         <v>0</v>
       </c>
     </row>
@@ -22093,7 +21917,7 @@
         <v>244</v>
       </c>
       <c r="N19" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, L39)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, L39)</f>
         <v>0</v>
       </c>
     </row>
@@ -22129,7 +21953,7 @@
         <v>17</v>
       </c>
       <c r="N20" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D70)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D70)</f>
         <v>0</v>
       </c>
     </row>
@@ -22165,7 +21989,7 @@
         <v>18</v>
       </c>
       <c r="N21" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D82)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D82)</f>
         <v>0</v>
       </c>
     </row>
@@ -22201,7 +22025,7 @@
         <v>19</v>
       </c>
       <c r="N22" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D69)</f>
+        <f>COUNTIFS(A131:A210,#REF!,D131:D210, D69)</f>
         <v>0</v>
       </c>
     </row>
@@ -22237,7 +22061,7 @@
         <v>20</v>
       </c>
       <c r="N23" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, K55)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, K55)</f>
         <v>0</v>
       </c>
     </row>
@@ -22273,7 +22097,7 @@
         <v>21</v>
       </c>
       <c r="N24" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D64)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D64)</f>
         <v>0</v>
       </c>
     </row>
@@ -22309,7 +22133,7 @@
         <v>245</v>
       </c>
       <c r="N25" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D34)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D34)</f>
         <v>0</v>
       </c>
     </row>
@@ -22345,7 +22169,7 @@
         <v>246</v>
       </c>
       <c r="N26" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D164)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D164)</f>
         <v>0</v>
       </c>
     </row>
@@ -22381,7 +22205,7 @@
         <v>24</v>
       </c>
       <c r="N27" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D56)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D56)</f>
         <v>0</v>
       </c>
     </row>
@@ -22417,7 +22241,7 @@
         <v>25</v>
       </c>
       <c r="N28" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D42)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D42)</f>
         <v>0</v>
       </c>
     </row>
@@ -22453,7 +22277,7 @@
         <v>26</v>
       </c>
       <c r="N29" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205,D76)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204,D76)</f>
         <v>0</v>
       </c>
     </row>
@@ -22489,7 +22313,7 @@
         <v>27</v>
       </c>
       <c r="N30" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D40)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D40)</f>
         <v>0</v>
       </c>
     </row>
@@ -22525,7 +22349,7 @@
         <v>28</v>
       </c>
       <c r="N31" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D85)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D85)</f>
         <v>0</v>
       </c>
     </row>
@@ -22561,7 +22385,7 @@
         <v>29</v>
       </c>
       <c r="N32" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D172)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D172)</f>
         <v>0</v>
       </c>
     </row>
@@ -22597,8 +22421,8 @@
         <v>30</v>
       </c>
       <c r="N33" s="4">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D205)</f>
-        <v>1</v>
+        <f xml:space="preserve"> COUNTIFS(A131:A204,#REF!,D131:D204,#REF!)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="15.75">
@@ -22633,7 +22457,7 @@
         <v>247</v>
       </c>
       <c r="N34" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D206)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D205)</f>
         <v>0</v>
       </c>
     </row>
@@ -22669,7 +22493,7 @@
         <v>32</v>
       </c>
       <c r="N35" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D207)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D206)</f>
         <v>0</v>
       </c>
     </row>
@@ -22705,7 +22529,7 @@
         <v>33</v>
       </c>
       <c r="N36" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D208)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D207)</f>
         <v>0</v>
       </c>
     </row>
@@ -22741,11 +22565,11 @@
         <v>34</v>
       </c>
       <c r="N37" s="56">
-        <f>COUNTIFS(A131:A205,A205,D131:D205, D209)</f>
+        <f>COUNTIFS(A131:A204,#REF!,D131:D204, D208)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="31.5">
+    <row r="38" spans="1:14" ht="15.75">
       <c r="A38" s="13" t="s">
         <v>226</v>
       </c>
@@ -22775,7 +22599,7 @@
       </c>
       <c r="N38" s="60">
         <f>SUM(N2:N37)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="31.5">
@@ -23151,7 +22975,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="31.5">
+    <row r="52" spans="1:9" ht="15.75">
       <c r="A52" s="13" t="s">
         <v>228</v>
       </c>
@@ -27280,29 +27104,167 @@
         <v>256</v>
       </c>
     </row>
-    <row r="205" spans="1:9" ht="15.75">
-      <c r="A205" s="59" t="s">
+    <row r="205" spans="1:9" ht="110.25">
+      <c r="A205" s="66" t="s">
+        <v>340</v>
+      </c>
+      <c r="B205" s="63" t="s">
+        <v>341</v>
+      </c>
+      <c r="C205" s="63" t="s">
+        <v>161</v>
+      </c>
+      <c r="D205" s="63" t="s">
+        <v>162</v>
+      </c>
+      <c r="E205" s="63" t="s">
+        <v>163</v>
+      </c>
+      <c r="F205" s="63" t="s">
+        <v>164</v>
+      </c>
+      <c r="G205" s="63" t="s">
         <v>342</v>
       </c>
-      <c r="B205" s="57" t="s">
-        <v>85</v>
-      </c>
-      <c r="C205" s="57" t="s">
+      <c r="H205" s="64" t="s">
+        <v>343</v>
+      </c>
+      <c r="I205" s="64" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" ht="94.5">
+      <c r="A206" s="66" t="s">
+        <v>340</v>
+      </c>
+      <c r="B206" s="63" t="s">
+        <v>206</v>
+      </c>
+      <c r="C206" s="63" t="s">
+        <v>76</v>
+      </c>
+      <c r="D206" s="63" t="s">
+        <v>165</v>
+      </c>
+      <c r="E206" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="F206" s="63" t="s">
+        <v>79</v>
+      </c>
+      <c r="G206" s="63" t="s">
+        <v>345</v>
+      </c>
+      <c r="H206" s="64" t="s">
+        <v>346</v>
+      </c>
+      <c r="I206" s="64" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" ht="94.5">
+      <c r="A207" s="66" t="s">
+        <v>340</v>
+      </c>
+      <c r="B207" s="63" t="s">
+        <v>75</v>
+      </c>
+      <c r="C207" s="63" t="s">
         <v>215</v>
       </c>
-      <c r="D205" s="57" t="s">
+      <c r="D207" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="E205" s="57" t="s">
+      <c r="E207" s="63" t="s">
+        <v>217</v>
+      </c>
+      <c r="F207" s="63" t="s">
+        <v>290</v>
+      </c>
+      <c r="G207" s="63" t="s">
+        <v>348</v>
+      </c>
+      <c r="H207" s="64" t="s">
+        <v>346</v>
+      </c>
+      <c r="I207" s="64" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" ht="47.25">
+      <c r="A208" s="66" t="s">
         <v>340</v>
       </c>
-      <c r="F205" s="57" t="s">
-        <v>341</v>
-      </c>
-      <c r="G205" s="57"/>
-      <c r="H205" s="57"/>
-      <c r="I205" s="57" t="s">
-        <v>256</v>
+      <c r="B208" s="63" t="s">
+        <v>350</v>
+      </c>
+      <c r="C208" s="63" t="s">
+        <v>275</v>
+      </c>
+      <c r="D208" s="63" t="s">
+        <v>276</v>
+      </c>
+      <c r="E208" s="63" t="s">
+        <v>277</v>
+      </c>
+      <c r="F208" s="63" t="s">
+        <v>164</v>
+      </c>
+      <c r="G208" s="63"/>
+      <c r="H208" s="63"/>
+      <c r="I208" s="64" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13" ht="47.25">
+      <c r="A209" s="66" t="s">
+        <v>340</v>
+      </c>
+      <c r="B209" s="63" t="s">
+        <v>352</v>
+      </c>
+      <c r="C209" s="63" t="s">
+        <v>112</v>
+      </c>
+      <c r="D209" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="E209" s="63" t="s">
+        <v>114</v>
+      </c>
+      <c r="F209" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="G209" s="63"/>
+      <c r="H209" s="63"/>
+      <c r="I209" s="64" t="s">
+        <v>351</v>
+      </c>
+      <c r="M209" s="70"/>
+    </row>
+    <row r="210" spans="1:13" ht="15.75">
+      <c r="A210" s="66" t="s">
+        <v>340</v>
+      </c>
+      <c r="B210" s="63" t="s">
+        <v>145</v>
+      </c>
+      <c r="C210" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="D210" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="E210" s="63" t="s">
+        <v>265</v>
+      </c>
+      <c r="F210" s="63" t="s">
+        <v>50</v>
+      </c>
+      <c r="G210" s="63"/>
+      <c r="H210" s="63"/>
+      <c r="I210" s="63" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -27312,10 +27274,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -27330,9 +27292,9 @@
         <v>35</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -27340,23 +27302,15 @@
       <c r="A2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5">
-        <v>0.73</v>
-      </c>
-      <c r="C2" s="56">
-        <v>30</v>
-      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="56"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="5">
-        <v>0.12</v>
-      </c>
-      <c r="C3" s="56">
-        <v>5</v>
-      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="56"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="56" t="s">
@@ -27369,56 +27323,36 @@
       <c r="A5" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="C5" s="56">
-        <v>6</v>
-      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="56"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C6" s="56">
-        <v>3</v>
-      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="56"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="C7" s="56">
-        <v>2</v>
-      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="56"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="C8" s="56">
-        <v>6</v>
-      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="56"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="C9" s="56">
-        <v>4</v>
-      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="56"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="56" t="s">
@@ -27431,12 +27365,8 @@
       <c r="A11" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="C11" s="56">
-        <v>2</v>
-      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="56"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="56" t="s">
@@ -27449,34 +27379,22 @@
       <c r="A13" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="5">
-        <v>0.73</v>
-      </c>
-      <c r="C13" s="56">
-        <v>30</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="56"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="5">
-        <v>0.02</v>
-      </c>
-      <c r="C14" s="56">
-        <v>1</v>
-      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="56"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="5">
-        <v>0.02</v>
-      </c>
-      <c r="C15" s="56">
-        <v>1</v>
-      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="56"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="56" t="s">
@@ -27510,34 +27428,22 @@
       <c r="A20" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="5">
-        <v>0.02</v>
-      </c>
-      <c r="C20" s="56">
-        <v>1</v>
-      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="56"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="5">
-        <v>0.22</v>
-      </c>
-      <c r="C21" s="56">
-        <v>10</v>
-      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="56"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C22" s="56">
-        <v>3</v>
-      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="56"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="56" t="s">
@@ -27550,23 +27456,15 @@
       <c r="A24" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="C24" s="56">
-        <v>2</v>
-      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="56"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="5">
-        <v>0.02</v>
-      </c>
-      <c r="C25" s="56">
-        <v>1</v>
-      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="56"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="56" t="s">
@@ -27579,56 +27477,36 @@
       <c r="A27" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="5">
-        <v>0.12</v>
-      </c>
-      <c r="C27" s="56">
-        <v>5</v>
-      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="56"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C28" s="56">
-        <v>3</v>
-      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="56"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="C29" s="56">
-        <v>2</v>
-      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="56"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C30" s="56">
-        <v>3</v>
-      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="56"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="C31" s="56">
-        <v>2</v>
-      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="56"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="56" t="s">
@@ -27637,58 +27515,77 @@
       <c r="B32" s="5"/>
       <c r="C32" s="56"/>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:5">
       <c r="A33" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="C33" s="56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="B33" s="5"/>
+      <c r="C33" s="56"/>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="56" t="s">
         <v>31</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="56"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:5">
       <c r="A35" s="56" t="s">
         <v>32</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="56"/>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:5">
       <c r="A36" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="C36" s="56">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="B36" s="5"/>
+      <c r="C36" s="56"/>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="56" t="s">
         <v>34</v>
       </c>
       <c r="B37" s="5"/>
-      <c r="C37" s="56">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="C37" s="56"/>
+    </row>
+    <row r="38" spans="1:5">
       <c r="C38">
         <f>SUM(C2:C37)</f>
-        <v>133</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="67" t="s">
+        <v>354</v>
+      </c>
+      <c r="B40" s="68"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="69"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="62" t="s">
+        <v>355</v>
+      </c>
+      <c r="B41" s="61" t="s">
+        <v>356</v>
+      </c>
+      <c r="C41" s="61" t="s">
+        <v>357</v>
+      </c>
+      <c r="D41" s="61" t="s">
+        <v>358</v>
+      </c>
+      <c r="E41" s="65" t="s">
+        <v>359</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A40:E40"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
modified:   Libro1.xlsx 	modified:   index.html 	modified:   src/charts.js 	modified:   src/weekly.js 	new file:   ~$Libro1.xlsx
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="361">
   <si>
     <t>LA FRIA</t>
   </si>
@@ -1096,6 +1096,9 @@
   </si>
   <si>
     <t>Viernes</t>
+  </si>
+  <si>
+    <t>SEMANA-1</t>
   </si>
 </sst>
 </file>
@@ -10961,7 +10964,7 @@
     <xf numFmtId="0" fontId="45" fillId="0" borderId="31"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -11139,6 +11142,9 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -11148,7 +11154,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -19889,6 +19895,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -20117,11 +20124,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="193960576"/>
-        <c:axId val="193970560"/>
+        <c:axId val="183605888"/>
+        <c:axId val="183615872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="193960576"/>
+        <c:axId val="183605888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20130,7 +20137,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193970560"/>
+        <c:crossAx val="183615872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20138,7 +20145,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193970560"/>
+        <c:axId val="183615872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20149,13 +20156,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193960576"/>
+        <c:crossAx val="183605888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -20185,6 +20193,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -20426,11 +20435,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="193999232"/>
-        <c:axId val="194000768"/>
+        <c:axId val="183648640"/>
+        <c:axId val="183650176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="193999232"/>
+        <c:axId val="183648640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20439,7 +20448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194000768"/>
+        <c:crossAx val="183650176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20447,7 +20456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="194000768"/>
+        <c:axId val="183650176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20458,13 +20467,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193999232"/>
+        <c:crossAx val="183648640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -20838,7 +20848,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -21219,10 +21229,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N210"/>
+  <dimension ref="A1:P210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E206" workbookViewId="0">
-      <selection activeCell="M207" sqref="M207"/>
+    <sheetView tabSelected="1" topLeftCell="G124" workbookViewId="0">
+      <selection activeCell="M137" sqref="M137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -21234,8 +21244,8 @@
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
     <col min="9" max="9" width="30.28515625" customWidth="1"/>
     <col min="11" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="43" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" customWidth="1"/>
+    <col min="13" max="13" width="38.85546875" customWidth="1"/>
+    <col min="14" max="14" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="32.25" thickBot="1">
@@ -25208,7 +25218,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="16.5" thickBot="1">
+    <row r="129" spans="1:16" ht="16.5" thickBot="1">
       <c r="A129" s="13" t="s">
         <v>238</v>
       </c>
@@ -25233,7 +25243,7 @@
       <c r="H129" s="55"/>
       <c r="I129" s="49"/>
     </row>
-    <row r="130" spans="1:9" ht="16.5" thickBot="1">
+    <row r="130" spans="1:16" ht="16.5" thickBot="1">
       <c r="A130" s="13" t="s">
         <v>238</v>
       </c>
@@ -25262,7 +25272,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="30.75" customHeight="1">
+    <row r="131" spans="1:16" ht="30.75" customHeight="1">
       <c r="A131" s="59" t="s">
         <v>248</v>
       </c>
@@ -25286,8 +25296,15 @@
       <c r="I131" s="57" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" ht="30.75" customHeight="1">
+      <c r="L131" s="71" t="s">
+        <v>360</v>
+      </c>
+      <c r="M131" s="71"/>
+      <c r="N131" s="71"/>
+      <c r="O131" s="71"/>
+      <c r="P131" s="71"/>
+    </row>
+    <row r="132" spans="1:16" ht="30.75" customHeight="1">
       <c r="A132" s="59" t="s">
         <v>248</v>
       </c>
@@ -25311,8 +25328,23 @@
       <c r="I132" s="58" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" ht="15.75">
+      <c r="L132" s="67" t="s">
+        <v>355</v>
+      </c>
+      <c r="M132" s="67" t="s">
+        <v>356</v>
+      </c>
+      <c r="N132" s="67" t="s">
+        <v>357</v>
+      </c>
+      <c r="O132" s="67" t="s">
+        <v>358</v>
+      </c>
+      <c r="P132" s="67" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16" ht="15.75">
       <c r="A133" s="59" t="s">
         <v>252</v>
       </c>
@@ -25336,8 +25368,24 @@
       <c r="I133" s="57" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" ht="15.75">
+      <c r="M133">
+        <f>COUNTIF(A:A,A131)</f>
+        <v>2</v>
+      </c>
+      <c r="N133">
+        <f>COUNTIF(A:A,A133)</f>
+        <v>7</v>
+      </c>
+      <c r="O133">
+        <f>COUNTIF(A:A,A40)</f>
+        <v>10</v>
+      </c>
+      <c r="P133">
+        <f>COUNTIF(A:A,A150)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16" ht="15.75">
       <c r="A134" s="59" t="s">
         <v>252</v>
       </c>
@@ -25362,7 +25410,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="15.75">
+    <row r="135" spans="1:16" ht="15.75">
       <c r="A135" s="59" t="s">
         <v>252</v>
       </c>
@@ -25387,7 +25435,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="15.75">
+    <row r="136" spans="1:16" ht="15.75">
       <c r="A136" s="59" t="s">
         <v>252</v>
       </c>
@@ -25412,7 +25460,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="15.75">
+    <row r="137" spans="1:16" ht="15.75">
       <c r="A137" s="59" t="s">
         <v>252</v>
       </c>
@@ -25437,7 +25485,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="15.75">
+    <row r="138" spans="1:16" ht="15.75">
       <c r="A138" s="59" t="s">
         <v>252</v>
       </c>
@@ -25462,7 +25510,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="15.75">
+    <row r="139" spans="1:16" ht="15.75">
       <c r="A139" s="59" t="s">
         <v>252</v>
       </c>
@@ -25487,7 +25535,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="15.75">
+    <row r="140" spans="1:16" ht="15.75">
       <c r="A140" s="59" t="s">
         <v>259</v>
       </c>
@@ -25512,7 +25560,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="15.75">
+    <row r="141" spans="1:16" ht="15.75">
       <c r="A141" s="59" t="s">
         <v>259</v>
       </c>
@@ -25537,7 +25585,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="142" spans="1:9" ht="15.75">
+    <row r="142" spans="1:16" ht="15.75">
       <c r="A142" s="59" t="s">
         <v>259</v>
       </c>
@@ -25562,7 +25610,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="15.75">
+    <row r="143" spans="1:16" ht="15.75">
       <c r="A143" s="59" t="s">
         <v>259</v>
       </c>
@@ -25587,7 +25635,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="15.75">
+    <row r="144" spans="1:16" ht="15.75">
       <c r="A144" s="59" t="s">
         <v>259</v>
       </c>
@@ -27240,7 +27288,7 @@
       <c r="I209" s="64" t="s">
         <v>351</v>
       </c>
-      <c r="M209" s="70"/>
+      <c r="M209" s="67"/>
     </row>
     <row r="210" spans="1:13" ht="15.75">
       <c r="A210" s="66" t="s">
@@ -27268,6 +27316,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L131:P131"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -27557,13 +27608,13 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="67" t="s">
+      <c r="A40" s="68" t="s">
         <v>354</v>
       </c>
-      <c r="B40" s="68"/>
-      <c r="C40" s="68"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="69"/>
+      <c r="B40" s="69"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="69"/>
+      <c r="E40" s="70"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="62" t="s">

</xml_diff>

<commit_message>
Changes to be committed: 	modified:   Libro1.xlsx 	modified:   src/weekly.js
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Estadística Marzo 0" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3541" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3541" uniqueCount="411">
   <si>
     <t>LA FRIA</t>
   </si>
@@ -1226,6 +1226,30 @@
   </si>
   <si>
     <t>Fallos</t>
+  </si>
+  <si>
+    <t>MÉRIDA</t>
+  </si>
+  <si>
+    <t>Días-4</t>
+  </si>
+  <si>
+    <t>Fallos-4</t>
+  </si>
+  <si>
+    <t>21-04-2025/Lunes</t>
+  </si>
+  <si>
+    <t>22-04-2025/Martes</t>
+  </si>
+  <si>
+    <t>23-04-2025/Miércoles</t>
+  </si>
+  <si>
+    <t>24-04-2025/Jueves</t>
+  </si>
+  <si>
+    <t>25-04-2025/Viernes</t>
   </si>
 </sst>
 </file>
@@ -21522,8 +21546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I247" sqref="I247"/>
+    <sheetView topLeftCell="G10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -22634,7 +22658,7 @@
       <c r="J29" s="112"/>
       <c r="K29" s="112"/>
       <c r="M29" s="4" t="s">
-        <v>26</v>
+        <v>403</v>
       </c>
       <c r="N29" s="54">
         <f>COUNTIFS(A131:A242,A239,D131:D242,D242)</f>
@@ -28912,8 +28936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R240"/>
   <sheetViews>
-    <sheetView topLeftCell="G67" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -28926,7 +28950,7 @@
     <col min="10" max="10" width="14.42578125" customWidth="1"/>
     <col min="11" max="11" width="22.5703125" customWidth="1"/>
     <col min="13" max="13" width="5.42578125" customWidth="1"/>
-    <col min="14" max="14" width="15" customWidth="1"/>
+    <col min="14" max="14" width="21" customWidth="1"/>
     <col min="15" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -29357,10 +29381,10 @@
         <v>402</v>
       </c>
       <c r="N11" s="117" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="O11" s="117" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.75">
@@ -29399,7 +29423,7 @@
         <v>5</v>
       </c>
       <c r="N12" s="127" t="s">
-        <v>354</v>
+        <v>406</v>
       </c>
       <c r="O12" s="123">
         <f>COUNTIF(A:A,A218)</f>
@@ -29442,7 +29466,7 @@
         <v>9</v>
       </c>
       <c r="N13" s="127" t="s">
-        <v>355</v>
+        <v>407</v>
       </c>
       <c r="O13" s="123">
         <f>COUNTIF(A:A,A224)</f>
@@ -29485,7 +29509,7 @@
         <v>4</v>
       </c>
       <c r="N14" s="127" t="s">
-        <v>356</v>
+        <v>408</v>
       </c>
       <c r="O14" s="123">
         <f>COUNTIF(A:A,A230)</f>
@@ -29528,7 +29552,7 @@
         <v>0</v>
       </c>
       <c r="N15" s="127" t="s">
-        <v>357</v>
+        <v>409</v>
       </c>
       <c r="O15" s="123">
         <f>COUNTIF(A:A,A239)</f>
@@ -29571,7 +29595,7 @@
         <v>0</v>
       </c>
       <c r="N16" s="127" t="s">
-        <v>358</v>
+        <v>410</v>
       </c>
       <c r="O16" s="123">
         <f>COUNTIF(A:A,)</f>

</xml_diff>

<commit_message>
Changes to be committed: 	modified:   Libro1.xlsx 	modified:   meses/enero.html 	modified:   src/weekly.js
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Diario 1" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3609" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4221" uniqueCount="501">
   <si>
     <t>LA FRIA</t>
   </si>
@@ -1247,6 +1247,288 @@
   </si>
   <si>
     <t>11:01</t>
+  </si>
+  <si>
+    <t>03/01/2025</t>
+  </si>
+  <si>
+    <t>01:47</t>
+  </si>
+  <si>
+    <t>03:39</t>
+  </si>
+  <si>
+    <t>07/01/2025</t>
+  </si>
+  <si>
+    <t>11:47</t>
+  </si>
+  <si>
+    <t>01:41</t>
+  </si>
+  <si>
+    <t>08/01/2025</t>
+  </si>
+  <si>
+    <t>08:42</t>
+  </si>
+  <si>
+    <t>01:48</t>
+  </si>
+  <si>
+    <t>ZODI YARACUY</t>
+  </si>
+  <si>
+    <t>10/01/2025</t>
+  </si>
+  <si>
+    <t>11:13</t>
+  </si>
+  <si>
+    <t>4941-0001389</t>
+  </si>
+  <si>
+    <t>2:37</t>
+  </si>
+  <si>
+    <t>14/01/2025</t>
+  </si>
+  <si>
+    <t>2:13</t>
+  </si>
+  <si>
+    <t>15/01/2025</t>
+  </si>
+  <si>
+    <t>12.14</t>
+  </si>
+  <si>
+    <t>2:46</t>
+  </si>
+  <si>
+    <t>3:55</t>
+  </si>
+  <si>
+    <t>16/01/2025</t>
+  </si>
+  <si>
+    <t>01:53</t>
+  </si>
+  <si>
+    <t>17/01/2025</t>
+  </si>
+  <si>
+    <t>8:40</t>
+  </si>
+  <si>
+    <t>02:22</t>
+  </si>
+  <si>
+    <t>21/01/2025</t>
+  </si>
+  <si>
+    <t>08:22</t>
+  </si>
+  <si>
+    <t>08:32</t>
+  </si>
+  <si>
+    <t>09:00</t>
+  </si>
+  <si>
+    <t>22/01/2025</t>
+  </si>
+  <si>
+    <t>12:24</t>
+  </si>
+  <si>
+    <t>1:12</t>
+  </si>
+  <si>
+    <t>01:00</t>
+  </si>
+  <si>
+    <t>PUNTP FIJO</t>
+  </si>
+  <si>
+    <t>02:00</t>
+  </si>
+  <si>
+    <t>02:21</t>
+  </si>
+  <si>
+    <t>2:33</t>
+  </si>
+  <si>
+    <t>03:29</t>
+  </si>
+  <si>
+    <t>8:09</t>
+  </si>
+  <si>
+    <t>8:10</t>
+  </si>
+  <si>
+    <t>8:14</t>
+  </si>
+  <si>
+    <t>12:05</t>
+  </si>
+  <si>
+    <t>2:10</t>
+  </si>
+  <si>
+    <t>3.20</t>
+  </si>
+  <si>
+    <t>3:21</t>
+  </si>
+  <si>
+    <t>7684-0007943</t>
+  </si>
+  <si>
+    <t>3:34</t>
+  </si>
+  <si>
+    <t>23/01/2025</t>
+  </si>
+  <si>
+    <t>7:53</t>
+  </si>
+  <si>
+    <t>8:56</t>
+  </si>
+  <si>
+    <t>12:09</t>
+  </si>
+  <si>
+    <t>24/01/2025</t>
+  </si>
+  <si>
+    <t>02:59</t>
+  </si>
+  <si>
+    <t>09:10</t>
+  </si>
+  <si>
+    <t>9:42</t>
+  </si>
+  <si>
+    <t>12:04</t>
+  </si>
+  <si>
+    <t>27/01/2025</t>
+  </si>
+  <si>
+    <t>08:44</t>
+  </si>
+  <si>
+    <t>29/01/2025</t>
+  </si>
+  <si>
+    <t>12:32</t>
+  </si>
+  <si>
+    <t>03:06</t>
+  </si>
+  <si>
+    <t>28/01/2025</t>
+  </si>
+  <si>
+    <t>8:21</t>
+  </si>
+  <si>
+    <t>09:16</t>
+  </si>
+  <si>
+    <t>02:10</t>
+  </si>
+  <si>
+    <t>09:11</t>
+  </si>
+  <si>
+    <t>10:56</t>
+  </si>
+  <si>
+    <t>01:20</t>
+  </si>
+  <si>
+    <t>02:32</t>
+  </si>
+  <si>
+    <t>30/01/2025</t>
+  </si>
+  <si>
+    <t>2:48</t>
+  </si>
+  <si>
+    <t>2:53</t>
+  </si>
+  <si>
+    <t>30/01/2024</t>
+  </si>
+  <si>
+    <t>8:57</t>
+  </si>
+  <si>
+    <t>3:33</t>
+  </si>
+  <si>
+    <t>3:36</t>
+  </si>
+  <si>
+    <t>31/01/2025</t>
+  </si>
+  <si>
+    <t>7:42</t>
+  </si>
+  <si>
+    <t>9.01</t>
+  </si>
+  <si>
+    <t>9:09</t>
+  </si>
+  <si>
+    <t>09:01</t>
+  </si>
+  <si>
+    <t>09:09</t>
+  </si>
+  <si>
+    <t>03:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Horas en solucionar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">En proceso </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 Minutos en solucionar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 horas en solucionar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 hora y 30 minutos en resolver </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 horas en solucionar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 horas y 30mnts en solucionar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">48 horas en solucionar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 Minutos en resolver </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No solventada debido a  fallas internas del router </t>
+  </si>
+  <si>
+    <t>Enero %</t>
   </si>
 </sst>
 </file>
@@ -1940,7 +2222,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -2435,6 +2717,84 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -11148,7 +11508,7 @@
     <xf numFmtId="0" fontId="45" fillId="0" borderId="30"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -11569,6 +11929,68 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="64" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8704">
@@ -28050,12 +28472,3215 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AD121"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="11" max="11" width="28.140625" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" s="153" customFormat="1" ht="42" customHeight="1" thickBot="1">
+      <c r="A1" s="159" t="s">
+        <v>219</v>
+      </c>
+      <c r="B1" s="159" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="160" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="157" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="161" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="162" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="155" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="152"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="93" t="s">
+        <v>398</v>
+      </c>
+      <c r="R1" s="93" t="s">
+        <v>399</v>
+      </c>
+      <c r="S1" s="156"/>
+      <c r="T1" s="93" t="s">
+        <v>396</v>
+      </c>
+      <c r="U1" s="93" t="s">
+        <v>397</v>
+      </c>
+      <c r="V1" s="156"/>
+      <c r="W1" s="93" t="s">
+        <v>400</v>
+      </c>
+      <c r="X1" s="93" t="s">
+        <v>401</v>
+      </c>
+      <c r="Y1" s="156"/>
+      <c r="Z1" s="93" t="s">
+        <v>402</v>
+      </c>
+      <c r="AA1" s="93" t="s">
+        <v>403</v>
+      </c>
+      <c r="AB1" s="156"/>
+      <c r="AC1" s="93" t="s">
+        <v>404</v>
+      </c>
+      <c r="AD1" s="93" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" ht="31.5" customHeight="1">
+      <c r="A2" s="165" t="s">
+        <v>407</v>
+      </c>
+      <c r="B2" s="166" t="s">
+        <v>365</v>
+      </c>
+      <c r="C2" s="167" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="168" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="F2" s="170">
+        <v>405</v>
+      </c>
+      <c r="G2" s="172"/>
+      <c r="H2" s="163"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="158" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5">
+        <f>COUNTIF(D:D,D19)/41</f>
+        <v>0.43902439024390244</v>
+      </c>
+      <c r="M2" s="158">
+        <f>COUNTIF(D:D,D19)</f>
+        <v>18</v>
+      </c>
+      <c r="Q2" s="164" t="s">
+        <v>354</v>
+      </c>
+      <c r="R2" s="158">
+        <f>COUNTIF(A:A,A3)</f>
+        <v>3</v>
+      </c>
+      <c r="S2" s="156"/>
+      <c r="T2" s="164" t="s">
+        <v>354</v>
+      </c>
+      <c r="U2" s="158"/>
+      <c r="V2" s="156"/>
+      <c r="W2" s="164" t="s">
+        <v>354</v>
+      </c>
+      <c r="X2" s="158">
+        <f>COUNTIF(A:A,)</f>
+        <v>0</v>
+      </c>
+      <c r="Y2" s="156"/>
+      <c r="Z2" s="164" t="s">
+        <v>354</v>
+      </c>
+      <c r="AA2" s="158">
+        <f>COUNTIF(A:A,A33)</f>
+        <v>11</v>
+      </c>
+      <c r="AB2" s="156"/>
+      <c r="AC2" s="164" t="s">
+        <v>354</v>
+      </c>
+      <c r="AD2" s="173">
+        <f>COUNTIF(A:A,A60)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="31.5" customHeight="1">
+      <c r="A3" s="165" t="s">
+        <v>407</v>
+      </c>
+      <c r="B3" s="166" t="s">
+        <v>408</v>
+      </c>
+      <c r="C3" s="167" t="s">
+        <v>215</v>
+      </c>
+      <c r="D3" s="168" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="170" t="s">
+        <v>217</v>
+      </c>
+      <c r="F3" s="170">
+        <v>707</v>
+      </c>
+      <c r="G3" s="171"/>
+      <c r="H3" s="163"/>
+      <c r="I3" s="154"/>
+      <c r="J3" s="154"/>
+      <c r="K3" s="158" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="5">
+        <f>COUNTIF(D:D,)/41</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="173">
+        <f>COUNTIF(D:D,)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="164" t="s">
+        <v>355</v>
+      </c>
+      <c r="R3" s="173">
+        <f>COUNTIF(A:A,)</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="156"/>
+      <c r="T3" s="164" t="s">
+        <v>355</v>
+      </c>
+      <c r="U3" s="173">
+        <f>COUNTIF(A:A,A5)</f>
+        <v>2</v>
+      </c>
+      <c r="V3" s="156"/>
+      <c r="W3" s="164" t="s">
+        <v>355</v>
+      </c>
+      <c r="X3" s="158">
+        <f>COUNTIF(A:A,A14)</f>
+        <v>8</v>
+      </c>
+      <c r="Y3" s="156"/>
+      <c r="Z3" s="164" t="s">
+        <v>355</v>
+      </c>
+      <c r="AA3" s="173">
+        <f>COUNTIF(A:A,A44)</f>
+        <v>8</v>
+      </c>
+      <c r="AB3" s="156"/>
+      <c r="AC3" s="164" t="s">
+        <v>355</v>
+      </c>
+      <c r="AD3" s="173">
+        <f>COUNTIF(A:A,A63)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" ht="31.5" customHeight="1">
+      <c r="A4" s="165" t="s">
+        <v>407</v>
+      </c>
+      <c r="B4" s="166" t="s">
+        <v>409</v>
+      </c>
+      <c r="C4" s="167" t="s">
+        <v>215</v>
+      </c>
+      <c r="D4" s="168" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="170" t="s">
+        <v>217</v>
+      </c>
+      <c r="F4" s="170">
+        <v>707</v>
+      </c>
+      <c r="G4" s="171"/>
+      <c r="H4" s="163"/>
+      <c r="I4" s="154"/>
+      <c r="J4" s="154"/>
+      <c r="K4" s="158" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="5">
+        <f>COUNTIF(D:D,)/41</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="173">
+        <f>COUNTIF(D:D,)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="164" t="s">
+        <v>356</v>
+      </c>
+      <c r="R4" s="173">
+        <f>COUNTIF(A:A,)</f>
+        <v>0</v>
+      </c>
+      <c r="S4" s="156"/>
+      <c r="T4" s="164" t="s">
+        <v>356</v>
+      </c>
+      <c r="U4" s="173">
+        <f>COUNTIF(A:A,A7)</f>
+        <v>3</v>
+      </c>
+      <c r="V4" s="156"/>
+      <c r="W4" s="164" t="s">
+        <v>356</v>
+      </c>
+      <c r="X4" s="173">
+        <f>COUNTIF(A:A,A22)</f>
+        <v>5</v>
+      </c>
+      <c r="Y4" s="156"/>
+      <c r="Z4" s="164" t="s">
+        <v>356</v>
+      </c>
+      <c r="AA4" s="173">
+        <f>COUNTIF(A:A,A52)</f>
+        <v>5</v>
+      </c>
+      <c r="AB4" s="156"/>
+      <c r="AC4" s="164" t="s">
+        <v>356</v>
+      </c>
+      <c r="AD4" s="173">
+        <f>COUNTIF(A:A,A68)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" ht="15.75">
+      <c r="A5" s="165" t="s">
+        <v>410</v>
+      </c>
+      <c r="B5" s="166" t="s">
+        <v>411</v>
+      </c>
+      <c r="C5" s="167" t="s">
+        <v>275</v>
+      </c>
+      <c r="D5" s="167" t="s">
+        <v>276</v>
+      </c>
+      <c r="E5" s="169" t="s">
+        <v>277</v>
+      </c>
+      <c r="F5" s="169" t="s">
+        <v>164</v>
+      </c>
+      <c r="G5" s="171"/>
+      <c r="H5" s="163"/>
+      <c r="I5" s="154"/>
+      <c r="J5" s="154"/>
+      <c r="K5" s="158" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="5">
+        <f>COUNTIF(D:D,D78)/41</f>
+        <v>2.4390243902439025E-2</v>
+      </c>
+      <c r="M5" s="173">
+        <f>COUNTIF(D:D,D78)</f>
+        <v>1</v>
+      </c>
+      <c r="Q5" s="164" t="s">
+        <v>357</v>
+      </c>
+      <c r="R5" s="173">
+        <f>COUNTIF(A:A,)</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="156"/>
+      <c r="T5" s="164" t="s">
+        <v>357</v>
+      </c>
+      <c r="U5" s="173">
+        <f>COUNTIF(A:A,)</f>
+        <v>0</v>
+      </c>
+      <c r="V5" s="156"/>
+      <c r="W5" s="164" t="s">
+        <v>357</v>
+      </c>
+      <c r="X5" s="173">
+        <f>COUNTIF(A:A,A27)</f>
+        <v>4</v>
+      </c>
+      <c r="Y5" s="156"/>
+      <c r="Z5" s="164" t="s">
+        <v>357</v>
+      </c>
+      <c r="AA5" s="173">
+        <f>COUNTIF(A:A,A57)</f>
+        <v>3</v>
+      </c>
+      <c r="AB5" s="156"/>
+      <c r="AC5" s="164" t="s">
+        <v>357</v>
+      </c>
+      <c r="AD5" s="173">
+        <f>COUNTIF(A:A,A76)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" ht="15.75">
+      <c r="A6" s="165" t="s">
+        <v>410</v>
+      </c>
+      <c r="B6" s="166" t="s">
+        <v>412</v>
+      </c>
+      <c r="C6" s="167" t="s">
+        <v>197</v>
+      </c>
+      <c r="D6" s="167" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" s="169" t="s">
+        <v>199</v>
+      </c>
+      <c r="F6" s="169" t="s">
+        <v>200</v>
+      </c>
+      <c r="G6" s="171"/>
+      <c r="H6" s="163"/>
+      <c r="I6" s="154"/>
+      <c r="J6" s="154"/>
+      <c r="K6" s="158" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="5">
+        <f>COUNTIF(D:D,)/41</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="173">
+        <f>COUNTIF(D:D,)</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="164" t="s">
+        <v>358</v>
+      </c>
+      <c r="R6" s="173">
+        <f>COUNTIF(A:A,)</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="156"/>
+      <c r="T6" s="164" t="s">
+        <v>358</v>
+      </c>
+      <c r="U6" s="173">
+        <f>COUNTIF(A:A,A10)</f>
+        <v>4</v>
+      </c>
+      <c r="V6" s="156"/>
+      <c r="W6" s="164" t="s">
+        <v>358</v>
+      </c>
+      <c r="X6" s="173">
+        <f>COUNTIF(A:A,A31)</f>
+        <v>2</v>
+      </c>
+      <c r="Y6" s="156"/>
+      <c r="Z6" s="164" t="s">
+        <v>358</v>
+      </c>
+      <c r="AA6" s="173">
+        <f>COUNTIF(A:A,)</f>
+        <v>0</v>
+      </c>
+      <c r="AB6" s="156"/>
+      <c r="AC6" s="164" t="s">
+        <v>358</v>
+      </c>
+      <c r="AD6" s="173">
+        <f>COUNTIF(A:A,A66)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" ht="15.75">
+      <c r="A7" s="165" t="s">
+        <v>413</v>
+      </c>
+      <c r="B7" s="166" t="s">
+        <v>414</v>
+      </c>
+      <c r="C7" s="167" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="169" t="s">
+        <v>159</v>
+      </c>
+      <c r="F7" s="169">
+        <v>403</v>
+      </c>
+      <c r="G7" s="171"/>
+      <c r="H7" s="163"/>
+      <c r="I7" s="154"/>
+      <c r="J7" s="154"/>
+      <c r="K7" s="158" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="5">
+        <f>COUNTIF(D:D,)/41</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="173">
+        <f>COUNTIF(D:D,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" ht="15.75">
+      <c r="A8" s="165" t="s">
+        <v>413</v>
+      </c>
+      <c r="B8" s="166" t="s">
+        <v>415</v>
+      </c>
+      <c r="C8" s="167" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="167" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="169" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="171"/>
+      <c r="H8" s="163"/>
+      <c r="I8" s="154"/>
+      <c r="J8" s="154"/>
+      <c r="K8" s="158" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" s="5">
+        <f>COUNTIF(D:D,D83)/41</f>
+        <v>2.4390243902439025E-2</v>
+      </c>
+      <c r="M8" s="173">
+        <f>COUNTIF(D:D,D83)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" ht="31.5">
+      <c r="A9" s="165" t="s">
+        <v>413</v>
+      </c>
+      <c r="B9" s="166" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="167" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="167" t="s">
+        <v>416</v>
+      </c>
+      <c r="E9" s="169" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="174" t="s">
+        <v>490</v>
+      </c>
+      <c r="H9" s="163"/>
+      <c r="I9" s="154"/>
+      <c r="J9" s="154"/>
+      <c r="K9" s="158" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="5">
+        <f>COUNTIF(D:D,D6)/41</f>
+        <v>0.12195121951219512</v>
+      </c>
+      <c r="M9" s="173">
+        <f>COUNTIF(D:D,D6)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="15.75">
+      <c r="A10" s="165" t="s">
+        <v>417</v>
+      </c>
+      <c r="B10" s="166" t="s">
+        <v>418</v>
+      </c>
+      <c r="C10" s="167" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="167" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="169" t="s">
+        <v>150</v>
+      </c>
+      <c r="F10" s="169" t="s">
+        <v>151</v>
+      </c>
+      <c r="G10" s="171"/>
+      <c r="H10" s="163"/>
+      <c r="I10" s="154"/>
+      <c r="J10" s="154"/>
+      <c r="K10" s="158" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="5">
+        <f>COUNTIF(D:D,D38)/41</f>
+        <v>2.4390243902439025E-2</v>
+      </c>
+      <c r="M10" s="173">
+        <f>COUNTIF(D:D,D83)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" ht="15.75">
+      <c r="A11" s="165" t="s">
+        <v>417</v>
+      </c>
+      <c r="B11" s="166" t="s">
+        <v>352</v>
+      </c>
+      <c r="C11" s="167" t="s">
+        <v>177</v>
+      </c>
+      <c r="D11" s="167" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="169" t="s">
+        <v>419</v>
+      </c>
+      <c r="F11" s="169" t="s">
+        <v>125</v>
+      </c>
+      <c r="G11" s="171"/>
+      <c r="H11" s="163"/>
+      <c r="I11" s="154"/>
+      <c r="J11" s="154"/>
+      <c r="K11" s="158" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="5">
+        <f>COUNTIF(D:D,D8)/41</f>
+        <v>2.4390243902439025E-2</v>
+      </c>
+      <c r="M11" s="173">
+        <f>COUNTIF(D:D,D8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" ht="15.75">
+      <c r="A12" s="165" t="s">
+        <v>417</v>
+      </c>
+      <c r="B12" s="166" t="s">
+        <v>420</v>
+      </c>
+      <c r="C12" s="167" t="s">
+        <v>158</v>
+      </c>
+      <c r="D12" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="169" t="s">
+        <v>159</v>
+      </c>
+      <c r="F12" s="169" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="171"/>
+      <c r="H12" s="163"/>
+      <c r="I12" s="154"/>
+      <c r="J12" s="154"/>
+      <c r="K12" s="158" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" s="5">
+        <f>COUNTIF(D:D,D50)/41</f>
+        <v>4.878048780487805E-2</v>
+      </c>
+      <c r="M12" s="173">
+        <f>COUNTIF(D:D,D50)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" ht="15.75">
+      <c r="A13" s="165" t="s">
+        <v>417</v>
+      </c>
+      <c r="B13" s="166" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="167" t="s">
+        <v>202</v>
+      </c>
+      <c r="D13" s="167" t="s">
+        <v>203</v>
+      </c>
+      <c r="E13" s="169" t="s">
+        <v>204</v>
+      </c>
+      <c r="F13" s="169" t="s">
+        <v>151</v>
+      </c>
+      <c r="G13" s="171"/>
+      <c r="H13" s="163"/>
+      <c r="I13" s="154"/>
+      <c r="J13" s="154"/>
+      <c r="K13" s="158" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" s="5">
+        <f>COUNTIF(D:D,D15)/41</f>
+        <v>0.17073170731707318</v>
+      </c>
+      <c r="M13" s="173">
+        <f>COUNTIF(D:D,D15)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" ht="15.75">
+      <c r="A14" s="165" t="s">
+        <v>421</v>
+      </c>
+      <c r="B14" s="166" t="s">
+        <v>191</v>
+      </c>
+      <c r="C14" s="167" t="s">
+        <v>202</v>
+      </c>
+      <c r="D14" s="167" t="s">
+        <v>203</v>
+      </c>
+      <c r="E14" s="169" t="s">
+        <v>204</v>
+      </c>
+      <c r="F14" s="169" t="s">
+        <v>151</v>
+      </c>
+      <c r="G14" s="171"/>
+      <c r="H14" s="163"/>
+      <c r="I14" s="154"/>
+      <c r="J14" s="154"/>
+      <c r="K14" s="158" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="5">
+        <f>COUNTIF(D:D,D17)/41</f>
+        <v>4.878048780487805E-2</v>
+      </c>
+      <c r="M14" s="173">
+        <f>COUNTIF(D:D,D17)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" ht="15.75">
+      <c r="A15" s="165" t="s">
+        <v>421</v>
+      </c>
+      <c r="B15" s="166" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="167" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="167" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="169" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="171"/>
+      <c r="H15" s="163"/>
+      <c r="I15" s="154"/>
+      <c r="J15" s="154"/>
+      <c r="K15" s="158" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="5">
+        <f>COUNTIF(D:D,D24)/41</f>
+        <v>7.3170731707317069E-2</v>
+      </c>
+      <c r="M15" s="173">
+        <f>COUNTIF(D:D,D24)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" ht="15.75">
+      <c r="A16" s="165" t="s">
+        <v>421</v>
+      </c>
+      <c r="B16" s="166" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" s="167" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="167" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="169" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="171"/>
+      <c r="H16" s="163"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="158" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" s="5">
+        <f>COUNTIF(D:D,)/41</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="173">
+        <f>COUNTIF(D:D,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75">
+      <c r="A17" s="165" t="s">
+        <v>421</v>
+      </c>
+      <c r="B17" s="166" t="s">
+        <v>168</v>
+      </c>
+      <c r="C17" s="167" t="s">
+        <v>169</v>
+      </c>
+      <c r="D17" s="167" t="s">
+        <v>170</v>
+      </c>
+      <c r="E17" s="169" t="s">
+        <v>171</v>
+      </c>
+      <c r="F17" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="171"/>
+      <c r="H17" s="163"/>
+      <c r="I17" s="154"/>
+      <c r="J17" s="154"/>
+      <c r="K17" s="158" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="5">
+        <f>COUNTIF(D:D,)/41</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="173">
+        <f>COUNTIF(D:D,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75">
+      <c r="A18" s="165" t="s">
+        <v>421</v>
+      </c>
+      <c r="B18" s="166" t="s">
+        <v>422</v>
+      </c>
+      <c r="C18" s="167" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="167" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="169" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="171"/>
+      <c r="H18" s="163"/>
+      <c r="I18" s="154"/>
+      <c r="J18" s="154"/>
+      <c r="K18" s="158" t="s">
+        <v>15</v>
+      </c>
+      <c r="L18" s="5">
+        <f>COUNTIF(D:D,)/41</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="173">
+        <f>COUNTIF(D:D,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15.75">
+      <c r="A19" s="165" t="s">
+        <v>421</v>
+      </c>
+      <c r="B19" s="166" t="s">
+        <v>315</v>
+      </c>
+      <c r="C19" s="167" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="167" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="169" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="171"/>
+      <c r="H19" s="163"/>
+      <c r="I19" s="154"/>
+      <c r="J19" s="154"/>
+      <c r="K19" s="158" t="s">
+        <v>16</v>
+      </c>
+      <c r="L19" s="5">
+        <f>COUNTIF(D:D,)/41</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="173">
+        <f>COUNTIF(D:D,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15.75">
+      <c r="A20" s="165" t="s">
+        <v>421</v>
+      </c>
+      <c r="B20" s="166" t="s">
+        <v>316</v>
+      </c>
+      <c r="C20" s="167" t="s">
+        <v>140</v>
+      </c>
+      <c r="D20" s="167" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" s="169" t="s">
+        <v>142</v>
+      </c>
+      <c r="F20" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="171"/>
+      <c r="H20" s="163"/>
+      <c r="I20" s="154"/>
+      <c r="J20" s="154"/>
+      <c r="K20" s="158" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="5">
+        <f>COUNTIF(D:D,)/41</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="173">
+        <f>COUNTIF(D:D,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75">
+      <c r="A21" s="165" t="s">
+        <v>421</v>
+      </c>
+      <c r="B21" s="166" t="s">
+        <v>262</v>
+      </c>
+      <c r="C21" s="167" t="s">
+        <v>184</v>
+      </c>
+      <c r="D21" s="167" t="s">
+        <v>185</v>
+      </c>
+      <c r="E21" s="169" t="s">
+        <v>186</v>
+      </c>
+      <c r="F21" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="171"/>
+      <c r="H21" s="163"/>
+      <c r="I21" s="154"/>
+      <c r="J21" s="154"/>
+      <c r="K21" s="158" t="s">
+        <v>18</v>
+      </c>
+      <c r="L21" s="5">
+        <f>COUNTIF(D:D,D55)/41</f>
+        <v>7.3170731707317069E-2</v>
+      </c>
+      <c r="M21" s="173">
+        <f>COUNTIF(D:D,D55)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A22" s="165" t="s">
+        <v>423</v>
+      </c>
+      <c r="B22" s="166" t="s">
+        <v>379</v>
+      </c>
+      <c r="C22" s="167" t="s">
+        <v>215</v>
+      </c>
+      <c r="D22" s="167" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="170" t="s">
+        <v>217</v>
+      </c>
+      <c r="F22" s="170">
+        <v>707</v>
+      </c>
+      <c r="G22" s="171"/>
+      <c r="H22" s="163"/>
+      <c r="I22" s="154"/>
+      <c r="J22" s="154"/>
+      <c r="K22" s="158" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22" s="5">
+        <f>COUNTIF(D:D,D29)/41</f>
+        <v>2.4390243902439025E-2</v>
+      </c>
+      <c r="M22" s="173">
+        <f>COUNTIF(D:D,D29)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15.75">
+      <c r="A23" s="165" t="s">
+        <v>423</v>
+      </c>
+      <c r="B23" s="166" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="167" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="167" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" s="169" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="171"/>
+      <c r="H23" s="163"/>
+      <c r="I23" s="154"/>
+      <c r="J23" s="154"/>
+      <c r="K23" s="158" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="5">
+        <f>COUNTIF(D:D,)/41</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="173">
+        <f>COUNTIF(D:D,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15.75">
+      <c r="A24" s="165" t="s">
+        <v>423</v>
+      </c>
+      <c r="B24" s="166" t="s">
+        <v>424</v>
+      </c>
+      <c r="C24" s="167" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="167" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="169" t="s">
+        <v>119</v>
+      </c>
+      <c r="F24" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" s="171"/>
+      <c r="H24" s="163"/>
+      <c r="I24" s="154"/>
+      <c r="J24" s="154"/>
+      <c r="K24" s="158" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" s="5">
+        <f>COUNTIF(D:D,D80)/41</f>
+        <v>4.878048780487805E-2</v>
+      </c>
+      <c r="M24" s="173">
+        <f>COUNTIF(D:D,D80)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15.75">
+      <c r="A25" s="165" t="s">
+        <v>423</v>
+      </c>
+      <c r="B25" s="166" t="s">
+        <v>425</v>
+      </c>
+      <c r="C25" s="167" t="s">
+        <v>275</v>
+      </c>
+      <c r="D25" s="167" t="s">
+        <v>276</v>
+      </c>
+      <c r="E25" s="169" t="s">
+        <v>277</v>
+      </c>
+      <c r="F25" s="169" t="s">
+        <v>164</v>
+      </c>
+      <c r="G25" s="171"/>
+      <c r="H25" s="163"/>
+      <c r="I25" s="154"/>
+      <c r="J25" s="154"/>
+      <c r="K25" s="158" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25" s="5">
+        <f>COUNTIF(D:D,D41)/41</f>
+        <v>4.878048780487805E-2</v>
+      </c>
+      <c r="M25" s="173">
+        <f>COUNTIF(D:D,D41)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15.75">
+      <c r="A26" s="165" t="s">
+        <v>423</v>
+      </c>
+      <c r="B26" s="166" t="s">
+        <v>426</v>
+      </c>
+      <c r="C26" s="167" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="167" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="169" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="171"/>
+      <c r="H26" s="163"/>
+      <c r="I26" s="154"/>
+      <c r="J26" s="154"/>
+      <c r="K26" s="158" t="s">
+        <v>23</v>
+      </c>
+      <c r="L26" s="5">
+        <f>COUNTIF(D:D,)/41</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="173">
+        <f>COUNTIF(D:D,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="15.75">
+      <c r="A27" s="165" t="s">
+        <v>427</v>
+      </c>
+      <c r="B27" s="166" t="s">
+        <v>418</v>
+      </c>
+      <c r="C27" s="167" t="s">
+        <v>140</v>
+      </c>
+      <c r="D27" s="167" t="s">
+        <v>141</v>
+      </c>
+      <c r="E27" s="169" t="s">
+        <v>142</v>
+      </c>
+      <c r="F27" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G27" s="171"/>
+      <c r="H27" s="163"/>
+      <c r="I27" s="154"/>
+      <c r="J27" s="154"/>
+      <c r="K27" s="158" t="s">
+        <v>24</v>
+      </c>
+      <c r="L27" s="5">
+        <f>COUNTIF(D:D,D71)/41</f>
+        <v>4.878048780487805E-2</v>
+      </c>
+      <c r="M27" s="173">
+        <f>COUNTIF(D:D,D71)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="15.75">
+      <c r="A28" s="165" t="s">
+        <v>427</v>
+      </c>
+      <c r="B28" s="166" t="s">
+        <v>428</v>
+      </c>
+      <c r="C28" s="167" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="167" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="169" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="171"/>
+      <c r="H28" s="163"/>
+      <c r="I28" s="154"/>
+      <c r="J28" s="154"/>
+      <c r="K28" s="158" t="s">
+        <v>25</v>
+      </c>
+      <c r="L28" s="5">
+        <f>COUNTIF(D:D,D27)/41</f>
+        <v>7.3170731707317069E-2</v>
+      </c>
+      <c r="M28" s="173">
+        <f>COUNTIF(D:D,D27)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="15.75">
+      <c r="A29" s="165" t="s">
+        <v>427</v>
+      </c>
+      <c r="B29" s="166" t="s">
+        <v>361</v>
+      </c>
+      <c r="C29" s="167" t="s">
+        <v>177</v>
+      </c>
+      <c r="D29" s="167" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="169" t="s">
+        <v>419</v>
+      </c>
+      <c r="F29" s="169" t="s">
+        <v>125</v>
+      </c>
+      <c r="G29" s="171"/>
+      <c r="H29" s="163"/>
+      <c r="I29" s="154"/>
+      <c r="J29" s="154"/>
+      <c r="K29" s="158" t="s">
+        <v>26</v>
+      </c>
+      <c r="L29" s="5">
+        <f>COUNTIF(D:D,D39)/41</f>
+        <v>0.12195121951219512</v>
+      </c>
+      <c r="M29" s="173">
+        <f>COUNTIF(D:D,D39)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="15.75">
+      <c r="A30" s="165" t="s">
+        <v>427</v>
+      </c>
+      <c r="B30" s="166" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" s="167" t="s">
+        <v>275</v>
+      </c>
+      <c r="D30" s="167" t="s">
+        <v>276</v>
+      </c>
+      <c r="E30" s="169" t="s">
+        <v>277</v>
+      </c>
+      <c r="F30" s="169" t="s">
+        <v>164</v>
+      </c>
+      <c r="G30" s="175" t="s">
+        <v>491</v>
+      </c>
+      <c r="H30" s="163"/>
+      <c r="I30" s="154"/>
+      <c r="J30" s="154"/>
+      <c r="K30" s="158" t="s">
+        <v>27</v>
+      </c>
+      <c r="L30" s="5">
+        <f>COUNTIF(D:D,D9)/41</f>
+        <v>7.3170731707317069E-2</v>
+      </c>
+      <c r="M30" s="173">
+        <f>COUNTIF(D:D,D9)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="30">
+      <c r="A31" s="165" t="s">
+        <v>429</v>
+      </c>
+      <c r="B31" s="166" t="s">
+        <v>430</v>
+      </c>
+      <c r="C31" s="167" t="s">
+        <v>275</v>
+      </c>
+      <c r="D31" s="167" t="s">
+        <v>276</v>
+      </c>
+      <c r="E31" s="169" t="s">
+        <v>277</v>
+      </c>
+      <c r="F31" s="169" t="s">
+        <v>164</v>
+      </c>
+      <c r="G31" s="175" t="s">
+        <v>492</v>
+      </c>
+      <c r="H31" s="163"/>
+      <c r="I31" s="154"/>
+      <c r="J31" s="154"/>
+      <c r="K31" s="158" t="s">
+        <v>28</v>
+      </c>
+      <c r="L31" s="5">
+        <f>COUNTIF(D:D,D13)/41</f>
+        <v>4.878048780487805E-2</v>
+      </c>
+      <c r="M31" s="173">
+        <f>COUNTIF(D:D,D13)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="15.75">
+      <c r="A32" s="165" t="s">
+        <v>429</v>
+      </c>
+      <c r="B32" s="166" t="s">
+        <v>431</v>
+      </c>
+      <c r="C32" s="167" t="s">
+        <v>169</v>
+      </c>
+      <c r="D32" s="167" t="s">
+        <v>170</v>
+      </c>
+      <c r="E32" s="169" t="s">
+        <v>171</v>
+      </c>
+      <c r="F32" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G32" s="171"/>
+      <c r="H32" s="163"/>
+      <c r="I32" s="154"/>
+      <c r="J32" s="154"/>
+      <c r="K32" s="158" t="s">
+        <v>29</v>
+      </c>
+      <c r="L32" s="5">
+        <f>COUNTIF(D:D,D25)/41</f>
+        <v>0.14634146341463414</v>
+      </c>
+      <c r="M32" s="173">
+        <f>COUNTIF(D:D,D25)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="15.75">
+      <c r="A33" s="165" t="s">
+        <v>432</v>
+      </c>
+      <c r="B33" s="166" t="s">
+        <v>433</v>
+      </c>
+      <c r="C33" s="167" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="167" t="s">
+        <v>416</v>
+      </c>
+      <c r="E33" s="169" t="s">
+        <v>97</v>
+      </c>
+      <c r="F33" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G33" s="171"/>
+      <c r="H33" s="163"/>
+      <c r="I33" s="154"/>
+      <c r="J33" s="154"/>
+      <c r="K33" s="158" t="s">
+        <v>30</v>
+      </c>
+      <c r="L33" s="5">
+        <f>COUNTIF(D:D,D22)/41</f>
+        <v>0.17073170731707318</v>
+      </c>
+      <c r="M33" s="173">
+        <f>COUNTIF(D:D,D22)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="15.75">
+      <c r="A34" s="165" t="s">
+        <v>432</v>
+      </c>
+      <c r="B34" s="166" t="s">
+        <v>434</v>
+      </c>
+      <c r="C34" s="167" t="s">
+        <v>197</v>
+      </c>
+      <c r="D34" s="167" t="s">
+        <v>198</v>
+      </c>
+      <c r="E34" s="169" t="s">
+        <v>199</v>
+      </c>
+      <c r="F34" s="169" t="s">
+        <v>200</v>
+      </c>
+      <c r="G34" s="171"/>
+      <c r="H34" s="163"/>
+      <c r="I34" s="154"/>
+      <c r="J34" s="154"/>
+      <c r="K34" s="158" t="s">
+        <v>31</v>
+      </c>
+      <c r="L34" s="5">
+        <f>COUNTIF(D:D,)/41</f>
+        <v>0</v>
+      </c>
+      <c r="M34" s="173">
+        <f>COUNTIF(D:D,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="30">
+      <c r="A35" s="165" t="s">
+        <v>432</v>
+      </c>
+      <c r="B35" s="166" t="s">
+        <v>435</v>
+      </c>
+      <c r="C35" s="167" t="s">
+        <v>275</v>
+      </c>
+      <c r="D35" s="167" t="s">
+        <v>276</v>
+      </c>
+      <c r="E35" s="169" t="s">
+        <v>277</v>
+      </c>
+      <c r="F35" s="169" t="s">
+        <v>164</v>
+      </c>
+      <c r="G35" s="175" t="s">
+        <v>493</v>
+      </c>
+      <c r="H35" s="163"/>
+      <c r="I35" s="154"/>
+      <c r="J35" s="154"/>
+      <c r="K35" s="158" t="s">
+        <v>32</v>
+      </c>
+      <c r="L35" s="5">
+        <f>COUNTIF(D:D,)/41</f>
+        <v>0</v>
+      </c>
+      <c r="M35" s="173">
+        <f>COUNTIF(D:D,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A36" s="165" t="s">
+        <v>432</v>
+      </c>
+      <c r="B36" s="166" t="s">
+        <v>437</v>
+      </c>
+      <c r="C36" s="167" t="s">
+        <v>215</v>
+      </c>
+      <c r="D36" s="167" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" s="170" t="s">
+        <v>217</v>
+      </c>
+      <c r="F36" s="170">
+        <v>707</v>
+      </c>
+      <c r="G36" s="175"/>
+      <c r="H36" s="163"/>
+      <c r="I36" s="154"/>
+      <c r="J36" s="154"/>
+      <c r="K36" s="158" t="s">
+        <v>33</v>
+      </c>
+      <c r="L36" s="5">
+        <f>COUNTIF(D:D,D88)/41</f>
+        <v>0.14634146341463414</v>
+      </c>
+      <c r="M36" s="173">
+        <f>COUNTIF(D:D,D88)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A37" s="165" t="s">
+        <v>432</v>
+      </c>
+      <c r="B37" s="166" t="s">
+        <v>438</v>
+      </c>
+      <c r="C37" s="167" t="s">
+        <v>215</v>
+      </c>
+      <c r="D37" s="167" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" s="170" t="s">
+        <v>217</v>
+      </c>
+      <c r="F37" s="170">
+        <v>707</v>
+      </c>
+      <c r="G37" s="175"/>
+      <c r="H37" s="163"/>
+      <c r="I37" s="154"/>
+      <c r="J37" s="154"/>
+      <c r="K37" s="158" t="s">
+        <v>34</v>
+      </c>
+      <c r="L37" s="5">
+        <f>COUNTIF(D:D,)/41</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="173">
+        <f>COUNTIF(D:D,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="15.75">
+      <c r="A38" s="165" t="s">
+        <v>432</v>
+      </c>
+      <c r="B38" s="166" t="s">
+        <v>439</v>
+      </c>
+      <c r="C38" s="167" t="s">
+        <v>282</v>
+      </c>
+      <c r="D38" s="167" t="s">
+        <v>440</v>
+      </c>
+      <c r="E38" s="169" t="s">
+        <v>283</v>
+      </c>
+      <c r="F38" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38" s="171"/>
+      <c r="H38" s="163"/>
+      <c r="I38" s="154"/>
+      <c r="J38" s="154"/>
+      <c r="K38" s="156"/>
+      <c r="L38" s="156"/>
+      <c r="M38" s="151">
+        <f>SUM(M2:M37)</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="30">
+      <c r="A39" s="165" t="s">
+        <v>432</v>
+      </c>
+      <c r="B39" s="166" t="s">
+        <v>441</v>
+      </c>
+      <c r="C39" s="167" t="s">
+        <v>184</v>
+      </c>
+      <c r="D39" s="167" t="s">
+        <v>185</v>
+      </c>
+      <c r="E39" s="169" t="s">
+        <v>186</v>
+      </c>
+      <c r="F39" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G39" s="175" t="s">
+        <v>493</v>
+      </c>
+      <c r="H39" s="163"/>
+      <c r="I39" s="154"/>
+      <c r="J39" s="154"/>
+    </row>
+    <row r="40" spans="1:13" ht="15.75">
+      <c r="A40" s="165" t="s">
+        <v>432</v>
+      </c>
+      <c r="B40" s="166" t="s">
+        <v>315</v>
+      </c>
+      <c r="C40" s="167" t="s">
+        <v>282</v>
+      </c>
+      <c r="D40" s="167" t="s">
+        <v>241</v>
+      </c>
+      <c r="E40" s="169" t="s">
+        <v>283</v>
+      </c>
+      <c r="F40" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G40" s="171"/>
+      <c r="H40" s="163"/>
+      <c r="I40" s="154"/>
+      <c r="J40" s="154"/>
+    </row>
+    <row r="41" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A41" s="165" t="s">
+        <v>432</v>
+      </c>
+      <c r="B41" s="166" t="s">
+        <v>442</v>
+      </c>
+      <c r="C41" s="167" t="s">
+        <v>122</v>
+      </c>
+      <c r="D41" s="168" t="s">
+        <v>123</v>
+      </c>
+      <c r="E41" s="170" t="s">
+        <v>263</v>
+      </c>
+      <c r="F41" s="170">
+        <v>405</v>
+      </c>
+      <c r="G41" s="171"/>
+      <c r="H41" s="163"/>
+      <c r="I41" s="154"/>
+      <c r="J41" s="154"/>
+    </row>
+    <row r="42" spans="1:13" ht="31.5" customHeight="1">
+      <c r="A42" s="165" t="s">
+        <v>432</v>
+      </c>
+      <c r="B42" s="166" t="s">
+        <v>443</v>
+      </c>
+      <c r="C42" s="167" t="s">
+        <v>215</v>
+      </c>
+      <c r="D42" s="167" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" s="170" t="s">
+        <v>217</v>
+      </c>
+      <c r="F42" s="170">
+        <v>707</v>
+      </c>
+      <c r="G42" s="171"/>
+      <c r="H42" s="163"/>
+      <c r="I42" s="154"/>
+      <c r="J42" s="154"/>
+    </row>
+    <row r="43" spans="1:13" ht="15.75">
+      <c r="A43" s="165" t="s">
+        <v>432</v>
+      </c>
+      <c r="B43" s="166" t="s">
+        <v>444</v>
+      </c>
+      <c r="C43" s="167" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="167" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="169" t="s">
+        <v>49</v>
+      </c>
+      <c r="F43" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G43" s="171"/>
+      <c r="H43" s="163"/>
+      <c r="I43" s="154"/>
+      <c r="J43" s="154"/>
+    </row>
+    <row r="44" spans="1:13" ht="15.75">
+      <c r="A44" s="165" t="s">
+        <v>436</v>
+      </c>
+      <c r="B44" s="166" t="s">
+        <v>445</v>
+      </c>
+      <c r="C44" s="167" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="167" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="169" t="s">
+        <v>49</v>
+      </c>
+      <c r="F44" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G44" s="171"/>
+      <c r="H44" s="163"/>
+      <c r="I44" s="154"/>
+      <c r="J44" s="154"/>
+    </row>
+    <row r="45" spans="1:13" ht="15.75">
+      <c r="A45" s="165" t="s">
+        <v>436</v>
+      </c>
+      <c r="B45" s="166" t="s">
+        <v>446</v>
+      </c>
+      <c r="C45" s="167" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" s="167" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="169" t="s">
+        <v>83</v>
+      </c>
+      <c r="F45" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G45" s="171"/>
+      <c r="H45" s="163"/>
+      <c r="I45" s="154"/>
+      <c r="J45" s="154"/>
+    </row>
+    <row r="46" spans="1:13" ht="15.75">
+      <c r="A46" s="165" t="s">
+        <v>436</v>
+      </c>
+      <c r="B46" s="166" t="s">
+        <v>447</v>
+      </c>
+      <c r="C46" s="167" t="s">
+        <v>184</v>
+      </c>
+      <c r="D46" s="167" t="s">
+        <v>185</v>
+      </c>
+      <c r="E46" s="169" t="s">
+        <v>186</v>
+      </c>
+      <c r="F46" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G46" s="171"/>
+      <c r="H46" s="163"/>
+      <c r="I46" s="154"/>
+      <c r="J46" s="154"/>
+    </row>
+    <row r="47" spans="1:13" ht="15.75">
+      <c r="A47" s="165" t="s">
+        <v>436</v>
+      </c>
+      <c r="B47" s="166" t="s">
+        <v>448</v>
+      </c>
+      <c r="C47" s="167" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="167" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="169" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G47" s="171"/>
+      <c r="H47" s="163"/>
+      <c r="I47" s="154"/>
+      <c r="J47" s="154"/>
+    </row>
+    <row r="48" spans="1:13" ht="30">
+      <c r="A48" s="165" t="s">
+        <v>436</v>
+      </c>
+      <c r="B48" s="166" t="s">
+        <v>449</v>
+      </c>
+      <c r="C48" s="167" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="167" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="169" t="s">
+        <v>83</v>
+      </c>
+      <c r="F48" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G48" s="175" t="s">
+        <v>494</v>
+      </c>
+      <c r="H48" s="163"/>
+      <c r="I48" s="154"/>
+      <c r="J48" s="154"/>
+    </row>
+    <row r="49" spans="1:10" ht="15.75">
+      <c r="A49" s="165" t="s">
+        <v>436</v>
+      </c>
+      <c r="B49" s="166" t="s">
+        <v>450</v>
+      </c>
+      <c r="C49" s="167" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" s="167" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="169" t="s">
+        <v>49</v>
+      </c>
+      <c r="F49" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G49" s="171"/>
+      <c r="H49" s="163"/>
+      <c r="I49" s="154"/>
+      <c r="J49" s="154"/>
+    </row>
+    <row r="50" spans="1:10" ht="15.75">
+      <c r="A50" s="165" t="s">
+        <v>436</v>
+      </c>
+      <c r="B50" s="166" t="s">
+        <v>451</v>
+      </c>
+      <c r="C50" s="167" t="s">
+        <v>129</v>
+      </c>
+      <c r="D50" s="167" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="169" t="s">
+        <v>452</v>
+      </c>
+      <c r="F50" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G50" s="171"/>
+      <c r="H50" s="163"/>
+      <c r="I50" s="154"/>
+      <c r="J50" s="154"/>
+    </row>
+    <row r="51" spans="1:10" ht="15.75">
+      <c r="A51" s="165" t="s">
+        <v>436</v>
+      </c>
+      <c r="B51" s="166" t="s">
+        <v>453</v>
+      </c>
+      <c r="C51" s="167" t="s">
+        <v>140</v>
+      </c>
+      <c r="D51" s="167" t="s">
+        <v>141</v>
+      </c>
+      <c r="E51" s="169" t="s">
+        <v>142</v>
+      </c>
+      <c r="F51" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G51" s="171"/>
+      <c r="H51" s="163"/>
+      <c r="I51" s="154"/>
+      <c r="J51" s="154"/>
+    </row>
+    <row r="52" spans="1:10" ht="15.75">
+      <c r="A52" s="165" t="s">
+        <v>454</v>
+      </c>
+      <c r="B52" s="166" t="s">
+        <v>455</v>
+      </c>
+      <c r="C52" s="167" t="s">
+        <v>282</v>
+      </c>
+      <c r="D52" s="167" t="s">
+        <v>241</v>
+      </c>
+      <c r="E52" s="169" t="s">
+        <v>283</v>
+      </c>
+      <c r="F52" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G52" s="171"/>
+      <c r="H52" s="163"/>
+      <c r="I52" s="154"/>
+      <c r="J52" s="154"/>
+    </row>
+    <row r="53" spans="1:10" ht="15.75">
+      <c r="A53" s="165" t="s">
+        <v>454</v>
+      </c>
+      <c r="B53" s="166" t="s">
+        <v>456</v>
+      </c>
+      <c r="C53" s="167" t="s">
+        <v>48</v>
+      </c>
+      <c r="D53" s="167" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="169" t="s">
+        <v>49</v>
+      </c>
+      <c r="F53" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G53" s="171"/>
+      <c r="H53" s="163"/>
+      <c r="I53" s="154"/>
+      <c r="J53" s="154"/>
+    </row>
+    <row r="54" spans="1:10" ht="30">
+      <c r="A54" s="165" t="s">
+        <v>454</v>
+      </c>
+      <c r="B54" s="166" t="s">
+        <v>457</v>
+      </c>
+      <c r="C54" s="167" t="s">
+        <v>184</v>
+      </c>
+      <c r="D54" s="167" t="s">
+        <v>185</v>
+      </c>
+      <c r="E54" s="169" t="s">
+        <v>186</v>
+      </c>
+      <c r="F54" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G54" s="175" t="s">
+        <v>495</v>
+      </c>
+      <c r="H54" s="163"/>
+      <c r="I54" s="154"/>
+      <c r="J54" s="154"/>
+    </row>
+    <row r="55" spans="1:10" ht="15.75">
+      <c r="A55" s="165" t="s">
+        <v>454</v>
+      </c>
+      <c r="B55" s="166" t="s">
+        <v>91</v>
+      </c>
+      <c r="C55" s="167" t="s">
+        <v>71</v>
+      </c>
+      <c r="D55" s="167" t="s">
+        <v>72</v>
+      </c>
+      <c r="E55" s="169" t="s">
+        <v>73</v>
+      </c>
+      <c r="F55" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G55" s="171"/>
+      <c r="H55" s="163"/>
+      <c r="I55" s="154"/>
+      <c r="J55" s="154"/>
+    </row>
+    <row r="56" spans="1:10" ht="15.75">
+      <c r="A56" s="165" t="s">
+        <v>454</v>
+      </c>
+      <c r="B56" s="166" t="s">
+        <v>459</v>
+      </c>
+      <c r="C56" s="167" t="s">
+        <v>76</v>
+      </c>
+      <c r="D56" s="167" t="s">
+        <v>165</v>
+      </c>
+      <c r="E56" s="169" t="s">
+        <v>78</v>
+      </c>
+      <c r="F56" s="169" t="s">
+        <v>79</v>
+      </c>
+      <c r="G56" s="171"/>
+      <c r="H56" s="163"/>
+      <c r="I56" s="154"/>
+      <c r="J56" s="154"/>
+    </row>
+    <row r="57" spans="1:10" ht="30">
+      <c r="A57" s="165" t="s">
+        <v>458</v>
+      </c>
+      <c r="B57" s="166" t="s">
+        <v>460</v>
+      </c>
+      <c r="C57" s="167" t="s">
+        <v>197</v>
+      </c>
+      <c r="D57" s="167" t="s">
+        <v>198</v>
+      </c>
+      <c r="E57" s="169" t="s">
+        <v>199</v>
+      </c>
+      <c r="F57" s="169" t="s">
+        <v>200</v>
+      </c>
+      <c r="G57" s="175" t="s">
+        <v>496</v>
+      </c>
+      <c r="H57" s="163"/>
+      <c r="I57" s="154"/>
+      <c r="J57" s="154"/>
+    </row>
+    <row r="58" spans="1:10" ht="30">
+      <c r="A58" s="165" t="s">
+        <v>458</v>
+      </c>
+      <c r="B58" s="166" t="s">
+        <v>461</v>
+      </c>
+      <c r="C58" s="167" t="s">
+        <v>96</v>
+      </c>
+      <c r="D58" s="167" t="s">
+        <v>416</v>
+      </c>
+      <c r="E58" s="169" t="s">
+        <v>97</v>
+      </c>
+      <c r="F58" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G58" s="175" t="s">
+        <v>496</v>
+      </c>
+      <c r="H58" s="163"/>
+      <c r="I58" s="154"/>
+      <c r="J58" s="154"/>
+    </row>
+    <row r="59" spans="1:10" ht="15.75">
+      <c r="A59" s="165" t="s">
+        <v>458</v>
+      </c>
+      <c r="B59" s="166" t="s">
+        <v>462</v>
+      </c>
+      <c r="C59" s="167" t="s">
+        <v>48</v>
+      </c>
+      <c r="D59" s="167" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59" s="169" t="s">
+        <v>49</v>
+      </c>
+      <c r="F59" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G59" s="171"/>
+      <c r="H59" s="163"/>
+      <c r="I59" s="154"/>
+      <c r="J59" s="154"/>
+    </row>
+    <row r="60" spans="1:10" ht="30">
+      <c r="A60" s="165" t="s">
+        <v>463</v>
+      </c>
+      <c r="B60" s="166" t="s">
+        <v>464</v>
+      </c>
+      <c r="C60" s="167" t="s">
+        <v>275</v>
+      </c>
+      <c r="D60" s="167" t="s">
+        <v>276</v>
+      </c>
+      <c r="E60" s="169" t="s">
+        <v>277</v>
+      </c>
+      <c r="F60" s="169" t="s">
+        <v>164</v>
+      </c>
+      <c r="G60" s="175" t="s">
+        <v>497</v>
+      </c>
+      <c r="H60" s="163"/>
+      <c r="I60" s="154"/>
+      <c r="J60" s="154"/>
+    </row>
+    <row r="61" spans="1:10" ht="15.75">
+      <c r="A61" s="165" t="s">
+        <v>463</v>
+      </c>
+      <c r="B61" s="166" t="s">
+        <v>466</v>
+      </c>
+      <c r="C61" s="167" t="s">
+        <v>71</v>
+      </c>
+      <c r="D61" s="167" t="s">
+        <v>72</v>
+      </c>
+      <c r="E61" s="169" t="s">
+        <v>73</v>
+      </c>
+      <c r="F61" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G61" s="171"/>
+      <c r="H61" s="163"/>
+      <c r="I61" s="154"/>
+      <c r="J61" s="154"/>
+    </row>
+    <row r="62" spans="1:10" ht="15.75">
+      <c r="A62" s="165" t="s">
+        <v>463</v>
+      </c>
+      <c r="B62" s="166" t="s">
+        <v>467</v>
+      </c>
+      <c r="C62" s="167" t="s">
+        <v>48</v>
+      </c>
+      <c r="D62" s="167" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="169" t="s">
+        <v>49</v>
+      </c>
+      <c r="F62" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G62" s="171"/>
+      <c r="H62" s="163"/>
+      <c r="I62" s="154"/>
+      <c r="J62" s="154"/>
+    </row>
+    <row r="63" spans="1:10" ht="15.75">
+      <c r="A63" s="165" t="s">
+        <v>468</v>
+      </c>
+      <c r="B63" s="166" t="s">
+        <v>378</v>
+      </c>
+      <c r="C63" s="167" t="s">
+        <v>282</v>
+      </c>
+      <c r="D63" s="167" t="s">
+        <v>241</v>
+      </c>
+      <c r="E63" s="169" t="s">
+        <v>283</v>
+      </c>
+      <c r="F63" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G63" s="171"/>
+      <c r="H63" s="163"/>
+      <c r="I63" s="154"/>
+      <c r="J63" s="154"/>
+    </row>
+    <row r="64" spans="1:10" ht="15.75">
+      <c r="A64" s="165" t="s">
+        <v>468</v>
+      </c>
+      <c r="B64" s="166" t="s">
+        <v>469</v>
+      </c>
+      <c r="C64" s="167" t="s">
+        <v>48</v>
+      </c>
+      <c r="D64" s="167" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="169" t="s">
+        <v>49</v>
+      </c>
+      <c r="F64" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G64" s="171"/>
+      <c r="H64" s="163"/>
+      <c r="I64" s="154"/>
+      <c r="J64" s="154"/>
+    </row>
+    <row r="65" spans="1:10" ht="30">
+      <c r="A65" s="165" t="s">
+        <v>468</v>
+      </c>
+      <c r="B65" s="166" t="s">
+        <v>470</v>
+      </c>
+      <c r="C65" s="167" t="s">
+        <v>82</v>
+      </c>
+      <c r="D65" s="167" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="169" t="s">
+        <v>83</v>
+      </c>
+      <c r="F65" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G65" s="175" t="s">
+        <v>498</v>
+      </c>
+      <c r="H65" s="163"/>
+      <c r="I65" s="154"/>
+      <c r="J65" s="154"/>
+    </row>
+    <row r="66" spans="1:10" ht="15.75">
+      <c r="A66" s="165" t="s">
+        <v>468</v>
+      </c>
+      <c r="B66" s="166" t="s">
+        <v>448</v>
+      </c>
+      <c r="C66" s="167" t="s">
+        <v>48</v>
+      </c>
+      <c r="D66" s="167" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="169" t="s">
+        <v>49</v>
+      </c>
+      <c r="F66" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G66" s="171"/>
+      <c r="H66" s="163"/>
+      <c r="I66" s="154"/>
+      <c r="J66" s="154"/>
+    </row>
+    <row r="67" spans="1:10" ht="30">
+      <c r="A67" s="165" t="s">
+        <v>468</v>
+      </c>
+      <c r="B67" s="166" t="s">
+        <v>471</v>
+      </c>
+      <c r="C67" s="167" t="s">
+        <v>184</v>
+      </c>
+      <c r="D67" s="167" t="s">
+        <v>185</v>
+      </c>
+      <c r="E67" s="169" t="s">
+        <v>186</v>
+      </c>
+      <c r="F67" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G67" s="175" t="s">
+        <v>495</v>
+      </c>
+      <c r="H67" s="163"/>
+      <c r="I67" s="154"/>
+      <c r="J67" s="154"/>
+    </row>
+    <row r="68" spans="1:10" ht="15.75">
+      <c r="A68" s="165" t="s">
+        <v>465</v>
+      </c>
+      <c r="B68" s="166" t="s">
+        <v>472</v>
+      </c>
+      <c r="C68" s="167" t="s">
+        <v>48</v>
+      </c>
+      <c r="D68" s="167" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="169" t="s">
+        <v>49</v>
+      </c>
+      <c r="F68" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G68" s="171"/>
+      <c r="H68" s="163"/>
+      <c r="I68" s="154"/>
+      <c r="J68" s="154"/>
+    </row>
+    <row r="69" spans="1:10" ht="30">
+      <c r="A69" s="165" t="s">
+        <v>465</v>
+      </c>
+      <c r="B69" s="166" t="s">
+        <v>100</v>
+      </c>
+      <c r="C69" s="167" t="s">
+        <v>129</v>
+      </c>
+      <c r="D69" s="167" t="s">
+        <v>130</v>
+      </c>
+      <c r="E69" s="169" t="s">
+        <v>131</v>
+      </c>
+      <c r="F69" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G69" s="175" t="s">
+        <v>498</v>
+      </c>
+      <c r="H69" s="163"/>
+      <c r="I69" s="154"/>
+      <c r="J69" s="154"/>
+    </row>
+    <row r="70" spans="1:10" ht="15.75">
+      <c r="A70" s="165" t="s">
+        <v>465</v>
+      </c>
+      <c r="B70" s="166" t="s">
+        <v>473</v>
+      </c>
+      <c r="C70" s="167" t="s">
+        <v>158</v>
+      </c>
+      <c r="D70" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="E70" s="169" t="s">
+        <v>159</v>
+      </c>
+      <c r="F70" s="169">
+        <v>403</v>
+      </c>
+      <c r="G70" s="171"/>
+      <c r="H70" s="163"/>
+      <c r="I70" s="154"/>
+      <c r="J70" s="154"/>
+    </row>
+    <row r="71" spans="1:10" ht="15.75">
+      <c r="A71" s="165" t="s">
+        <v>465</v>
+      </c>
+      <c r="B71" s="166" t="s">
+        <v>474</v>
+      </c>
+      <c r="C71" s="167" t="s">
+        <v>76</v>
+      </c>
+      <c r="D71" s="167" t="s">
+        <v>165</v>
+      </c>
+      <c r="E71" s="169" t="s">
+        <v>166</v>
+      </c>
+      <c r="F71" s="169" t="s">
+        <v>79</v>
+      </c>
+      <c r="G71" s="171"/>
+      <c r="H71" s="163"/>
+      <c r="I71" s="154"/>
+      <c r="J71" s="154"/>
+    </row>
+    <row r="72" spans="1:10" ht="30">
+      <c r="A72" s="165" t="s">
+        <v>465</v>
+      </c>
+      <c r="B72" s="166" t="s">
+        <v>475</v>
+      </c>
+      <c r="C72" s="167" t="s">
+        <v>215</v>
+      </c>
+      <c r="D72" s="167" t="s">
+        <v>30</v>
+      </c>
+      <c r="E72" s="169" t="s">
+        <v>217</v>
+      </c>
+      <c r="F72" s="169" t="s">
+        <v>290</v>
+      </c>
+      <c r="G72" s="175" t="s">
+        <v>493</v>
+      </c>
+      <c r="H72" s="163"/>
+      <c r="I72" s="154"/>
+      <c r="J72" s="154"/>
+    </row>
+    <row r="73" spans="1:10" ht="15.75">
+      <c r="A73" s="165" t="s">
+        <v>465</v>
+      </c>
+      <c r="B73" s="166" t="s">
+        <v>477</v>
+      </c>
+      <c r="C73" s="167" t="s">
+        <v>48</v>
+      </c>
+      <c r="D73" s="167" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="169" t="s">
+        <v>49</v>
+      </c>
+      <c r="F73" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G73" s="171"/>
+      <c r="H73" s="163"/>
+      <c r="I73" s="154"/>
+      <c r="J73" s="154"/>
+    </row>
+    <row r="74" spans="1:10" ht="15.75">
+      <c r="A74" s="165" t="s">
+        <v>465</v>
+      </c>
+      <c r="B74" s="166" t="s">
+        <v>478</v>
+      </c>
+      <c r="C74" s="167" t="s">
+        <v>82</v>
+      </c>
+      <c r="D74" s="167" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="169" t="s">
+        <v>83</v>
+      </c>
+      <c r="F74" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G74" s="171"/>
+      <c r="H74" s="163"/>
+      <c r="I74" s="154"/>
+      <c r="J74" s="154"/>
+    </row>
+    <row r="75" spans="1:10" ht="15.75">
+      <c r="A75" s="165" t="s">
+        <v>479</v>
+      </c>
+      <c r="B75" s="166" t="s">
+        <v>480</v>
+      </c>
+      <c r="C75" s="167" t="s">
+        <v>158</v>
+      </c>
+      <c r="D75" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="E75" s="169" t="s">
+        <v>159</v>
+      </c>
+      <c r="F75" s="169" t="s">
+        <v>57</v>
+      </c>
+      <c r="G75" s="171"/>
+      <c r="H75" s="163"/>
+      <c r="I75" s="154"/>
+      <c r="J75" s="154"/>
+    </row>
+    <row r="76" spans="1:10" ht="15.75">
+      <c r="A76" s="165" t="s">
+        <v>476</v>
+      </c>
+      <c r="B76" s="166" t="s">
+        <v>293</v>
+      </c>
+      <c r="C76" s="167" t="s">
+        <v>48</v>
+      </c>
+      <c r="D76" s="167" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" s="169" t="s">
+        <v>49</v>
+      </c>
+      <c r="F76" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G76" s="171"/>
+      <c r="H76" s="163"/>
+      <c r="I76" s="154"/>
+      <c r="J76" s="154"/>
+    </row>
+    <row r="77" spans="1:10" ht="15.75">
+      <c r="A77" s="165" t="s">
+        <v>476</v>
+      </c>
+      <c r="B77" s="166" t="s">
+        <v>481</v>
+      </c>
+      <c r="C77" s="167" t="s">
+        <v>71</v>
+      </c>
+      <c r="D77" s="167" t="s">
+        <v>72</v>
+      </c>
+      <c r="E77" s="169" t="s">
+        <v>73</v>
+      </c>
+      <c r="F77" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G77" s="171"/>
+      <c r="H77" s="163"/>
+      <c r="I77" s="154"/>
+      <c r="J77" s="154"/>
+    </row>
+    <row r="78" spans="1:10" ht="15.75">
+      <c r="A78" s="165" t="s">
+        <v>476</v>
+      </c>
+      <c r="B78" s="166" t="s">
+        <v>482</v>
+      </c>
+      <c r="C78" s="167" t="s">
+        <v>161</v>
+      </c>
+      <c r="D78" s="167" t="s">
+        <v>162</v>
+      </c>
+      <c r="E78" s="169" t="s">
+        <v>163</v>
+      </c>
+      <c r="F78" s="169" t="s">
+        <v>164</v>
+      </c>
+      <c r="G78" s="171"/>
+      <c r="H78" s="163"/>
+      <c r="I78" s="154"/>
+      <c r="J78" s="154"/>
+    </row>
+    <row r="79" spans="1:10" ht="15.75">
+      <c r="A79" s="165" t="s">
+        <v>483</v>
+      </c>
+      <c r="B79" s="166" t="s">
+        <v>484</v>
+      </c>
+      <c r="C79" s="167" t="s">
+        <v>282</v>
+      </c>
+      <c r="D79" s="167" t="s">
+        <v>241</v>
+      </c>
+      <c r="E79" s="169" t="s">
+        <v>283</v>
+      </c>
+      <c r="F79" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G79" s="171"/>
+      <c r="H79" s="163"/>
+      <c r="I79" s="154"/>
+      <c r="J79" s="154"/>
+    </row>
+    <row r="80" spans="1:10" ht="15.75">
+      <c r="A80" s="165" t="s">
+        <v>483</v>
+      </c>
+      <c r="B80" s="166" t="s">
+        <v>63</v>
+      </c>
+      <c r="C80" s="167" t="s">
+        <v>149</v>
+      </c>
+      <c r="D80" s="167" t="s">
+        <v>21</v>
+      </c>
+      <c r="E80" s="169" t="s">
+        <v>150</v>
+      </c>
+      <c r="F80" s="169" t="s">
+        <v>151</v>
+      </c>
+      <c r="G80" s="171"/>
+      <c r="H80" s="163"/>
+      <c r="I80" s="154"/>
+      <c r="J80" s="154"/>
+    </row>
+    <row r="81" spans="1:10" ht="15.75">
+      <c r="A81" s="165" t="s">
+        <v>483</v>
+      </c>
+      <c r="B81" s="166" t="s">
+        <v>485</v>
+      </c>
+      <c r="C81" s="167" t="s">
+        <v>48</v>
+      </c>
+      <c r="D81" s="167" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" s="169" t="s">
+        <v>49</v>
+      </c>
+      <c r="F81" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G81" s="171"/>
+      <c r="H81" s="163"/>
+      <c r="I81" s="154"/>
+      <c r="J81" s="154"/>
+    </row>
+    <row r="82" spans="1:10" ht="15.75">
+      <c r="A82" s="165" t="s">
+        <v>483</v>
+      </c>
+      <c r="B82" s="166" t="s">
+        <v>486</v>
+      </c>
+      <c r="C82" s="167" t="s">
+        <v>197</v>
+      </c>
+      <c r="D82" s="167" t="s">
+        <v>198</v>
+      </c>
+      <c r="E82" s="169" t="s">
+        <v>199</v>
+      </c>
+      <c r="F82" s="169" t="s">
+        <v>200</v>
+      </c>
+      <c r="G82" s="171"/>
+      <c r="H82" s="163"/>
+      <c r="I82" s="154"/>
+      <c r="J82" s="154"/>
+    </row>
+    <row r="83" spans="1:10" ht="15.75">
+      <c r="A83" s="165" t="s">
+        <v>483</v>
+      </c>
+      <c r="B83" s="166" t="s">
+        <v>486</v>
+      </c>
+      <c r="C83" s="167" t="s">
+        <v>86</v>
+      </c>
+      <c r="D83" s="167" t="s">
+        <v>4</v>
+      </c>
+      <c r="E83" s="169" t="s">
+        <v>87</v>
+      </c>
+      <c r="F83" s="169" t="s">
+        <v>57</v>
+      </c>
+      <c r="G83" s="171"/>
+      <c r="H83" s="163"/>
+      <c r="I83" s="154"/>
+      <c r="J83" s="154"/>
+    </row>
+    <row r="84" spans="1:10" ht="45">
+      <c r="A84" s="165" t="s">
+        <v>483</v>
+      </c>
+      <c r="B84" s="166" t="s">
+        <v>205</v>
+      </c>
+      <c r="C84" s="167" t="s">
+        <v>117</v>
+      </c>
+      <c r="D84" s="167" t="s">
+        <v>118</v>
+      </c>
+      <c r="E84" s="169" t="s">
+        <v>119</v>
+      </c>
+      <c r="F84" s="169" t="s">
+        <v>74</v>
+      </c>
+      <c r="G84" s="176" t="s">
+        <v>499</v>
+      </c>
+      <c r="H84" s="163"/>
+      <c r="I84" s="154"/>
+      <c r="J84" s="154"/>
+    </row>
+    <row r="85" spans="1:10" ht="15.75">
+      <c r="A85" s="165" t="s">
+        <v>483</v>
+      </c>
+      <c r="B85" s="166" t="s">
+        <v>487</v>
+      </c>
+      <c r="C85" s="167" t="s">
+        <v>48</v>
+      </c>
+      <c r="D85" s="167" t="s">
+        <v>0</v>
+      </c>
+      <c r="E85" s="169" t="s">
+        <v>49</v>
+      </c>
+      <c r="F85" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G85" s="171"/>
+      <c r="H85" s="163"/>
+      <c r="I85" s="154"/>
+      <c r="J85" s="154"/>
+    </row>
+    <row r="86" spans="1:10" ht="15.75">
+      <c r="A86" s="165" t="s">
+        <v>483</v>
+      </c>
+      <c r="B86" s="166" t="s">
+        <v>488</v>
+      </c>
+      <c r="C86" s="167" t="s">
+        <v>197</v>
+      </c>
+      <c r="D86" s="167" t="s">
+        <v>198</v>
+      </c>
+      <c r="E86" s="169" t="s">
+        <v>199</v>
+      </c>
+      <c r="F86" s="169" t="s">
+        <v>200</v>
+      </c>
+      <c r="G86" s="171"/>
+      <c r="H86" s="163"/>
+      <c r="I86" s="154"/>
+      <c r="J86" s="154"/>
+    </row>
+    <row r="87" spans="1:10" ht="15.75">
+      <c r="A87" s="165" t="s">
+        <v>483</v>
+      </c>
+      <c r="B87" s="166" t="s">
+        <v>459</v>
+      </c>
+      <c r="C87" s="167" t="s">
+        <v>82</v>
+      </c>
+      <c r="D87" s="167" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" s="169" t="s">
+        <v>83</v>
+      </c>
+      <c r="F87" s="169" t="s">
+        <v>50</v>
+      </c>
+      <c r="G87" s="171"/>
+      <c r="H87" s="163"/>
+      <c r="I87" s="154"/>
+      <c r="J87" s="154"/>
+    </row>
+    <row r="88" spans="1:10" ht="15.75">
+      <c r="A88" s="165" t="s">
+        <v>483</v>
+      </c>
+      <c r="B88" s="166" t="s">
+        <v>489</v>
+      </c>
+      <c r="C88" s="167" t="s">
+        <v>158</v>
+      </c>
+      <c r="D88" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="E88" s="169" t="s">
+        <v>159</v>
+      </c>
+      <c r="F88" s="169">
+        <v>403</v>
+      </c>
+      <c r="G88" s="171"/>
+      <c r="H88" s="163"/>
+      <c r="I88" s="154"/>
+      <c r="J88" s="154"/>
+    </row>
+    <row r="89" spans="1:10" ht="15.75">
+      <c r="A89" s="165" t="s">
+        <v>483</v>
+      </c>
+      <c r="B89" s="166" t="s">
+        <v>409</v>
+      </c>
+      <c r="C89" s="167" t="s">
+        <v>158</v>
+      </c>
+      <c r="D89" s="167" t="s">
+        <v>33</v>
+      </c>
+      <c r="E89" s="169" t="s">
+        <v>159</v>
+      </c>
+      <c r="F89" s="169">
+        <v>403</v>
+      </c>
+      <c r="G89" s="171"/>
+      <c r="H89" s="163"/>
+      <c r="I89" s="154"/>
+      <c r="J89" s="154"/>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" s="154"/>
+      <c r="B90" s="154"/>
+      <c r="C90" s="154"/>
+      <c r="D90" s="154"/>
+      <c r="E90" s="154"/>
+      <c r="F90" s="154"/>
+      <c r="G90" s="154"/>
+      <c r="H90" s="154"/>
+      <c r="I90" s="154"/>
+      <c r="J90" s="154"/>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="154"/>
+      <c r="B91" s="154"/>
+      <c r="C91" s="154"/>
+      <c r="D91" s="154"/>
+      <c r="E91" s="154"/>
+      <c r="F91" s="154"/>
+      <c r="G91" s="154"/>
+      <c r="H91" s="154"/>
+      <c r="I91" s="154"/>
+      <c r="J91" s="154"/>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" s="154"/>
+      <c r="B92" s="154"/>
+      <c r="C92" s="154"/>
+      <c r="D92" s="154"/>
+      <c r="E92" s="154"/>
+      <c r="F92" s="154"/>
+      <c r="G92" s="154"/>
+      <c r="H92" s="154"/>
+      <c r="I92" s="154"/>
+      <c r="J92" s="154"/>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" s="154"/>
+      <c r="B93" s="154"/>
+      <c r="C93" s="154"/>
+      <c r="D93" s="154"/>
+      <c r="E93" s="154"/>
+      <c r="F93" s="154"/>
+      <c r="G93" s="154"/>
+      <c r="H93" s="154"/>
+      <c r="I93" s="154"/>
+      <c r="J93" s="154"/>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94" s="154"/>
+      <c r="B94" s="154"/>
+      <c r="C94" s="154"/>
+      <c r="D94" s="154"/>
+      <c r="E94" s="154"/>
+      <c r="F94" s="154"/>
+      <c r="G94" s="154"/>
+      <c r="H94" s="154"/>
+      <c r="I94" s="154"/>
+      <c r="J94" s="154"/>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" s="154"/>
+      <c r="B95" s="154"/>
+      <c r="C95" s="154"/>
+      <c r="D95" s="154"/>
+      <c r="E95" s="154"/>
+      <c r="F95" s="154"/>
+      <c r="G95" s="154"/>
+      <c r="H95" s="154"/>
+      <c r="I95" s="154"/>
+      <c r="J95" s="154"/>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96" s="154"/>
+      <c r="B96" s="154"/>
+      <c r="C96" s="154"/>
+      <c r="D96" s="154"/>
+      <c r="E96" s="154"/>
+      <c r="F96" s="154"/>
+      <c r="G96" s="154"/>
+      <c r="H96" s="154"/>
+      <c r="I96" s="154"/>
+      <c r="J96" s="154"/>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97" s="154"/>
+      <c r="B97" s="154"/>
+      <c r="C97" s="154"/>
+      <c r="D97" s="154"/>
+      <c r="E97" s="154"/>
+      <c r="F97" s="154"/>
+      <c r="G97" s="154"/>
+      <c r="H97" s="154"/>
+      <c r="I97" s="154"/>
+      <c r="J97" s="154"/>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" s="154"/>
+      <c r="B98" s="154"/>
+      <c r="C98" s="154"/>
+      <c r="D98" s="154"/>
+      <c r="E98" s="154"/>
+      <c r="F98" s="154"/>
+      <c r="G98" s="154"/>
+      <c r="H98" s="154"/>
+      <c r="I98" s="154"/>
+      <c r="J98" s="154"/>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" s="154"/>
+      <c r="B99" s="154"/>
+      <c r="C99" s="154"/>
+      <c r="D99" s="154"/>
+      <c r="E99" s="154"/>
+      <c r="F99" s="154"/>
+      <c r="G99" s="154"/>
+      <c r="H99" s="154"/>
+      <c r="I99" s="154"/>
+      <c r="J99" s="154"/>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" s="154"/>
+      <c r="B100" s="154"/>
+      <c r="C100" s="154"/>
+      <c r="D100" s="154"/>
+      <c r="E100" s="154"/>
+      <c r="F100" s="154"/>
+      <c r="G100" s="154"/>
+      <c r="H100" s="154"/>
+      <c r="I100" s="154"/>
+      <c r="J100" s="154"/>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="154"/>
+      <c r="B101" s="154"/>
+      <c r="C101" s="154"/>
+      <c r="D101" s="154"/>
+      <c r="E101" s="154"/>
+      <c r="F101" s="154"/>
+      <c r="G101" s="154"/>
+      <c r="H101" s="154"/>
+      <c r="I101" s="154"/>
+      <c r="J101" s="154"/>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" s="154"/>
+      <c r="B102" s="154"/>
+      <c r="C102" s="154"/>
+      <c r="D102" s="154"/>
+      <c r="E102" s="154"/>
+      <c r="F102" s="154"/>
+      <c r="G102" s="154"/>
+      <c r="H102" s="154"/>
+      <c r="I102" s="154"/>
+      <c r="J102" s="154"/>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103" s="154"/>
+      <c r="B103" s="154"/>
+      <c r="C103" s="154"/>
+      <c r="D103" s="154"/>
+      <c r="E103" s="154"/>
+      <c r="F103" s="154"/>
+      <c r="G103" s="154"/>
+      <c r="H103" s="154"/>
+      <c r="I103" s="154"/>
+      <c r="J103" s="154"/>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104" s="154"/>
+      <c r="B104" s="154"/>
+      <c r="C104" s="154"/>
+      <c r="D104" s="154"/>
+      <c r="E104" s="154"/>
+      <c r="F104" s="154"/>
+      <c r="G104" s="154"/>
+      <c r="H104" s="154"/>
+      <c r="I104" s="154"/>
+      <c r="J104" s="154"/>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="A105" s="154"/>
+      <c r="B105" s="154"/>
+      <c r="C105" s="154"/>
+      <c r="D105" s="154"/>
+      <c r="E105" s="154"/>
+      <c r="F105" s="154"/>
+      <c r="G105" s="154"/>
+      <c r="H105" s="154"/>
+      <c r="I105" s="154"/>
+      <c r="J105" s="154"/>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="A106" s="154"/>
+      <c r="B106" s="154"/>
+      <c r="C106" s="154"/>
+      <c r="D106" s="154"/>
+      <c r="E106" s="154"/>
+      <c r="F106" s="154"/>
+      <c r="G106" s="154"/>
+      <c r="H106" s="154"/>
+      <c r="I106" s="154"/>
+      <c r="J106" s="154"/>
+    </row>
+    <row r="107" spans="1:10">
+      <c r="A107" s="154"/>
+      <c r="B107" s="154"/>
+      <c r="C107" s="154"/>
+      <c r="D107" s="154"/>
+      <c r="E107" s="154"/>
+      <c r="F107" s="154"/>
+      <c r="G107" s="154"/>
+      <c r="H107" s="154"/>
+      <c r="I107" s="154"/>
+      <c r="J107" s="154"/>
+    </row>
+    <row r="108" spans="1:10">
+      <c r="A108" s="154"/>
+      <c r="B108" s="154"/>
+      <c r="C108" s="154"/>
+      <c r="D108" s="154"/>
+      <c r="E108" s="154"/>
+      <c r="F108" s="154"/>
+      <c r="G108" s="154"/>
+      <c r="H108" s="154"/>
+      <c r="I108" s="154"/>
+      <c r="J108" s="154"/>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109" s="154"/>
+      <c r="B109" s="154"/>
+      <c r="C109" s="154"/>
+      <c r="D109" s="154"/>
+      <c r="E109" s="154"/>
+      <c r="F109" s="154"/>
+      <c r="G109" s="154"/>
+      <c r="H109" s="154"/>
+      <c r="I109" s="154"/>
+      <c r="J109" s="154"/>
+    </row>
+    <row r="110" spans="1:10">
+      <c r="A110" s="154"/>
+      <c r="B110" s="154"/>
+      <c r="C110" s="154"/>
+      <c r="D110" s="154"/>
+      <c r="E110" s="154"/>
+      <c r="F110" s="154"/>
+      <c r="G110" s="154"/>
+      <c r="H110" s="154"/>
+      <c r="I110" s="154"/>
+      <c r="J110" s="154"/>
+    </row>
+    <row r="111" spans="1:10">
+      <c r="A111" s="154"/>
+      <c r="B111" s="154"/>
+      <c r="C111" s="154"/>
+      <c r="D111" s="154"/>
+      <c r="E111" s="154"/>
+      <c r="F111" s="154"/>
+      <c r="G111" s="154"/>
+      <c r="H111" s="154"/>
+      <c r="I111" s="154"/>
+      <c r="J111" s="154"/>
+    </row>
+    <row r="112" spans="1:10">
+      <c r="A112" s="154"/>
+      <c r="B112" s="154"/>
+      <c r="C112" s="154"/>
+      <c r="D112" s="154"/>
+      <c r="E112" s="154"/>
+      <c r="F112" s="154"/>
+      <c r="G112" s="154"/>
+      <c r="H112" s="154"/>
+      <c r="I112" s="154"/>
+      <c r="J112" s="154"/>
+    </row>
+    <row r="113" spans="1:10">
+      <c r="A113" s="154"/>
+      <c r="B113" s="154"/>
+      <c r="C113" s="154"/>
+      <c r="D113" s="154"/>
+      <c r="E113" s="154"/>
+      <c r="F113" s="154"/>
+      <c r="G113" s="154"/>
+      <c r="H113" s="154"/>
+      <c r="I113" s="154"/>
+      <c r="J113" s="154"/>
+    </row>
+    <row r="114" spans="1:10">
+      <c r="A114" s="154"/>
+      <c r="B114" s="154"/>
+      <c r="C114" s="154"/>
+      <c r="D114" s="154"/>
+      <c r="E114" s="154"/>
+      <c r="F114" s="154"/>
+      <c r="G114" s="154"/>
+      <c r="H114" s="154"/>
+      <c r="I114" s="154"/>
+      <c r="J114" s="154"/>
+    </row>
+    <row r="115" spans="1:10">
+      <c r="A115" s="154"/>
+      <c r="B115" s="154"/>
+      <c r="C115" s="154"/>
+      <c r="D115" s="154"/>
+      <c r="E115" s="154"/>
+      <c r="F115" s="154"/>
+      <c r="G115" s="154"/>
+      <c r="H115" s="154"/>
+      <c r="I115" s="154"/>
+      <c r="J115" s="154"/>
+    </row>
+    <row r="116" spans="1:10">
+      <c r="A116" s="154"/>
+      <c r="B116" s="154"/>
+      <c r="C116" s="154"/>
+      <c r="D116" s="154"/>
+      <c r="E116" s="154"/>
+      <c r="F116" s="154"/>
+      <c r="G116" s="154"/>
+      <c r="H116" s="154"/>
+      <c r="I116" s="154"/>
+      <c r="J116" s="154"/>
+    </row>
+    <row r="117" spans="1:10">
+      <c r="A117" s="154"/>
+      <c r="B117" s="154"/>
+      <c r="C117" s="154"/>
+      <c r="D117" s="154"/>
+      <c r="E117" s="154"/>
+      <c r="F117" s="154"/>
+      <c r="G117" s="154"/>
+      <c r="H117" s="154"/>
+      <c r="I117" s="154"/>
+      <c r="J117" s="154"/>
+    </row>
+    <row r="118" spans="1:10">
+      <c r="A118" s="154"/>
+      <c r="B118" s="154"/>
+      <c r="C118" s="154"/>
+      <c r="D118" s="154"/>
+      <c r="E118" s="154"/>
+      <c r="F118" s="154"/>
+      <c r="G118" s="154"/>
+      <c r="H118" s="154"/>
+      <c r="I118" s="154"/>
+      <c r="J118" s="154"/>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119" s="154"/>
+      <c r="B119" s="154"/>
+      <c r="C119" s="154"/>
+      <c r="D119" s="154"/>
+      <c r="E119" s="154"/>
+      <c r="F119" s="154"/>
+      <c r="G119" s="154"/>
+      <c r="H119" s="154"/>
+      <c r="I119" s="154"/>
+      <c r="J119" s="154"/>
+    </row>
+    <row r="120" spans="1:10">
+      <c r="A120" s="154"/>
+      <c r="B120" s="154"/>
+      <c r="C120" s="154"/>
+      <c r="D120" s="154"/>
+      <c r="E120" s="154"/>
+      <c r="F120" s="154"/>
+      <c r="G120" s="154"/>
+      <c r="H120" s="154"/>
+      <c r="I120" s="154"/>
+      <c r="J120" s="154"/>
+    </row>
+    <row r="121" spans="1:10">
+      <c r="A121" s="154"/>
+      <c r="B121" s="154"/>
+      <c r="C121" s="154"/>
+      <c r="D121" s="154"/>
+      <c r="E121" s="154"/>
+      <c r="F121" s="154"/>
+      <c r="G121" s="154"/>
+      <c r="H121" s="154"/>
+      <c r="I121" s="154"/>
+      <c r="J121" s="154"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -28079,7 +31704,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AB248"/>
   <sheetViews>
-    <sheetView topLeftCell="J22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -33665,8 +37290,8 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:AC130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -33779,8 +37404,8 @@
         <v>0</v>
       </c>
       <c r="L2" s="5">
-        <f>COUNTIF(D:D,D2)/41</f>
-        <v>0.46341463414634149</v>
+        <f>COUNTIF(D:D,D2)/113</f>
+        <v>0.16814159292035399</v>
       </c>
       <c r="M2" s="46">
         <f>COUNTIF(D:D,D2)</f>
@@ -33850,7 +37475,7 @@
         <v>38</v>
       </c>
       <c r="L3" s="5">
-        <f>COUNTIF(D:D,)/41</f>
+        <f>COUNTIF(D:D,)/113</f>
         <v>0</v>
       </c>
       <c r="M3" s="123">
@@ -33921,8 +37546,8 @@
         <v>1</v>
       </c>
       <c r="L4" s="5">
-        <f>COUNTIF(D:D,D110)/41</f>
-        <v>2.4390243902439025E-2</v>
+        <f>COUNTIF(D:D,D110)/113</f>
+        <v>8.8495575221238937E-3</v>
       </c>
       <c r="M4" s="123">
         <f>COUNTIF(D:D,D110)</f>
@@ -33992,8 +37617,8 @@
         <v>11</v>
       </c>
       <c r="L5" s="5">
-        <f>COUNTIF(D:D,D52)/41</f>
-        <v>7.3170731707317069E-2</v>
+        <f>COUNTIF(D:D,D52)/113</f>
+        <v>2.6548672566371681E-2</v>
       </c>
       <c r="M5" s="123">
         <f>COUNTIF(D:D,D52)</f>
@@ -34063,8 +37688,8 @@
         <v>2</v>
       </c>
       <c r="L6" s="5">
-        <f>COUNTIF(D:D,D93)/41</f>
-        <v>2.4390243902439025E-2</v>
+        <f>COUNTIF(D:D,D93)/113</f>
+        <v>8.8495575221238937E-3</v>
       </c>
       <c r="M6" s="123">
         <f>COUNTIF(D:D,D93)</f>
@@ -34134,8 +37759,8 @@
         <v>3</v>
       </c>
       <c r="L7" s="5">
-        <f>COUNTIF(D:D,D10)/41</f>
-        <v>4.878048780487805E-2</v>
+        <f>COUNTIF(D:D,D10)/113</f>
+        <v>1.7699115044247787E-2</v>
       </c>
       <c r="M7" s="123">
         <f>COUNTIF(D:D,D10)</f>
@@ -34170,8 +37795,8 @@
         <v>4</v>
       </c>
       <c r="L8" s="5">
-        <f>COUNTIF(D:D,D7)/41</f>
-        <v>0.21951219512195122</v>
+        <f>COUNTIF(D:D,D7)/113</f>
+        <v>7.9646017699115043E-2</v>
       </c>
       <c r="M8" s="123">
         <f>COUNTIF(D:D,D7)</f>
@@ -34206,8 +37831,8 @@
         <v>5</v>
       </c>
       <c r="L9" s="5">
-        <f>COUNTIF(D:D,D28)/41</f>
-        <v>4.878048780487805E-2</v>
+        <f>COUNTIF(D:D,D28)/113</f>
+        <v>1.7699115044247787E-2</v>
       </c>
       <c r="M9" s="123">
         <f>COUNTIF(D:D,D20)</f>
@@ -34242,11 +37867,11 @@
         <v>6</v>
       </c>
       <c r="L10" s="5">
-        <f t="shared" ref="L3:L37" si="0">COUNTIF(D:D,D10)/41</f>
-        <v>4.878048780487805E-2</v>
+        <f>COUNTIF(D:D,D10)/113</f>
+        <v>1.7699115044247787E-2</v>
       </c>
       <c r="M10" s="123">
-        <f t="shared" ref="M3:M37" si="1">COUNTIF(D:D,D10)</f>
+        <f t="shared" ref="M3:M37" si="0">COUNTIF(D:D,D10)</f>
         <v>2</v>
       </c>
     </row>
@@ -34278,8 +37903,8 @@
         <v>7</v>
       </c>
       <c r="L11" s="5">
-        <f>COUNTIF(D:D,D61)/41</f>
-        <v>2.4390243902439025E-2</v>
+        <f>COUNTIF(D:D,D61)/113</f>
+        <v>8.8495575221238937E-3</v>
       </c>
       <c r="M11" s="123">
         <f>COUNTIF(D:D,D61)</f>
@@ -34314,8 +37939,8 @@
         <v>8</v>
       </c>
       <c r="L12" s="5">
-        <f>COUNTIF(D:D,D42)/41</f>
-        <v>0.14634146341463414</v>
+        <f>COUNTIF(D:D,D42)/113</f>
+        <v>5.3097345132743362E-2</v>
       </c>
       <c r="M12" s="123">
         <f>COUNTIF(D:D,D42)</f>
@@ -34350,8 +37975,8 @@
         <v>9</v>
       </c>
       <c r="L13" s="5">
-        <f>COUNTIF(D:D,D6)/41</f>
-        <v>0.21951219512195122</v>
+        <f>COUNTIF(D:D,D6)/113</f>
+        <v>7.9646017699115043E-2</v>
       </c>
       <c r="M13" s="123">
         <f>COUNTIF(D:D,D6)</f>
@@ -34386,8 +38011,8 @@
         <v>10</v>
       </c>
       <c r="L14" s="5">
-        <f>COUNTIF(D:D,D67)/41</f>
-        <v>7.3170731707317069E-2</v>
+        <f>COUNTIF(D:D,D67)/113</f>
+        <v>2.6548672566371681E-2</v>
       </c>
       <c r="M14" s="123">
         <f>COUNTIF(D:D,D67)</f>
@@ -34422,8 +38047,8 @@
         <v>12</v>
       </c>
       <c r="L15" s="5">
-        <f>COUNTIF(D:D,D17)/41</f>
-        <v>2.4390243902439025E-2</v>
+        <f>COUNTIF(D:D,D17)/113</f>
+        <v>8.8495575221238937E-3</v>
       </c>
       <c r="M15" s="123">
         <f>COUNTIF(D:D,D17)</f>
@@ -34458,7 +38083,7 @@
         <v>13</v>
       </c>
       <c r="L16" s="5">
-        <f>COUNTIF(D:D,)/41</f>
+        <f>COUNTIF(D:D,)/113</f>
         <v>0</v>
       </c>
       <c r="M16" s="123">
@@ -34494,7 +38119,7 @@
         <v>14</v>
       </c>
       <c r="L17" s="5">
-        <f>COUNTIF(D:D,)/41</f>
+        <f>COUNTIF(D:D,)/113</f>
         <v>0</v>
       </c>
       <c r="M17" s="123">
@@ -34530,7 +38155,7 @@
         <v>15</v>
       </c>
       <c r="L18" s="5">
-        <f>COUNTIF(D:D,)/41</f>
+        <f>COUNTIF(D:D,)/113</f>
         <v>0</v>
       </c>
       <c r="M18" s="123">
@@ -34566,8 +38191,8 @@
         <v>16</v>
       </c>
       <c r="L19" s="5">
-        <f>COUNTIF(D:D,D105)/41</f>
-        <v>2.4390243902439025E-2</v>
+        <f>COUNTIF(D:D,D105)/113</f>
+        <v>8.8495575221238937E-3</v>
       </c>
       <c r="M19" s="123">
         <f>COUNTIF(D:D,D105)</f>
@@ -34602,8 +38227,8 @@
         <v>17</v>
       </c>
       <c r="L20" s="5">
-        <f>COUNTIF(D:D,D21)/41</f>
-        <v>9.7560975609756101E-2</v>
+        <f>COUNTIF(D:D,D21)/113</f>
+        <v>3.5398230088495575E-2</v>
       </c>
       <c r="M20" s="123">
         <f>COUNTIF(D:D,D21)</f>
@@ -34638,8 +38263,8 @@
         <v>18</v>
       </c>
       <c r="L21" s="5">
-        <f>COUNTIF(D:D,D9)/41</f>
-        <v>0.12195121951219512</v>
+        <f>COUNTIF(D:D,D9)/113</f>
+        <v>4.4247787610619468E-2</v>
       </c>
       <c r="M21" s="123">
         <f>COUNTIF(D:D,D9)</f>
@@ -34674,8 +38299,8 @@
         <v>19</v>
       </c>
       <c r="L22" s="5">
-        <f>COUNTIF(D:D,D109)/41</f>
-        <v>2.4390243902439025E-2</v>
+        <f>COUNTIF(D:D,D109)/113</f>
+        <v>8.8495575221238937E-3</v>
       </c>
       <c r="M22" s="123">
         <f>COUNTIF(D:D,D109)</f>
@@ -34710,7 +38335,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="5">
-        <f>COUNTIF(D:D,)/41</f>
+        <f>COUNTIF(D:D,)/113</f>
         <v>0</v>
       </c>
       <c r="M23" s="123">
@@ -34746,7 +38371,7 @@
         <v>21</v>
       </c>
       <c r="L24" s="5">
-        <f>COUNTIF(D:D,)/41</f>
+        <f>COUNTIF(D:D,)/113</f>
         <v>0</v>
       </c>
       <c r="M24" s="123">
@@ -34782,8 +38407,8 @@
         <v>22</v>
       </c>
       <c r="L25" s="5">
-        <f>COUNTIF(D:D,D18)/41</f>
-        <v>2.4390243902439025E-2</v>
+        <f>COUNTIF(D:D,D18)/113</f>
+        <v>8.8495575221238937E-3</v>
       </c>
       <c r="M25" s="123">
         <f>COUNTIF(D:D,D18)</f>
@@ -34818,8 +38443,8 @@
         <v>23</v>
       </c>
       <c r="L26" s="5">
-        <f>COUNTIF(D:D,D35)/41</f>
-        <v>2.4390243902439025E-2</v>
+        <f>COUNTIF(D:D,D35)/113</f>
+        <v>8.8495575221238937E-3</v>
       </c>
       <c r="M26" s="123">
         <f>COUNTIF(D:D,D35)</f>
@@ -34854,8 +38479,8 @@
         <v>24</v>
       </c>
       <c r="L27" s="5">
-        <f>COUNTIF(D:D,D39)/41</f>
-        <v>0.14634146341463414</v>
+        <f>COUNTIF(D:D,D39)/113</f>
+        <v>5.3097345132743362E-2</v>
       </c>
       <c r="M27" s="123">
         <f>COUNTIF(D:D,D39)</f>
@@ -34890,8 +38515,8 @@
         <v>25</v>
       </c>
       <c r="L28" s="5">
-        <f>COUNTIF(D:D,D55)/41</f>
-        <v>2.4390243902439025E-2</v>
+        <f>COUNTIF(D:D,D55)/113</f>
+        <v>8.8495575221238937E-3</v>
       </c>
       <c r="M28" s="123">
         <f>COUNTIF(D:D,D55)</f>
@@ -34926,8 +38551,8 @@
         <v>26</v>
       </c>
       <c r="L29" s="5">
-        <f>COUNTIF(D:D,D38)/41</f>
-        <v>0.14634146341463414</v>
+        <f>COUNTIF(D:D,D38)/113</f>
+        <v>5.3097345132743362E-2</v>
       </c>
       <c r="M29" s="123">
         <f>COUNTIF(D:D,D38)</f>
@@ -34962,8 +38587,8 @@
         <v>27</v>
       </c>
       <c r="L30" s="5">
-        <f>COUNTIF(D:D,D11)/41</f>
-        <v>9.7560975609756101E-2</v>
+        <f>COUNTIF(D:D,D11)/113</f>
+        <v>3.5398230088495575E-2</v>
       </c>
       <c r="M30" s="123">
         <f>COUNTIF(D:D,D11)</f>
@@ -34998,8 +38623,8 @@
         <v>28</v>
       </c>
       <c r="L31" s="5">
-        <f>COUNTIF(D:D,D111)/41</f>
-        <v>0.1951219512195122</v>
+        <f>COUNTIF(D:D,D111)/113</f>
+        <v>7.0796460176991149E-2</v>
       </c>
       <c r="M31" s="123">
         <f>COUNTIF(D:D,D111)</f>
@@ -35034,8 +38659,8 @@
         <v>29</v>
       </c>
       <c r="L32" s="5">
-        <f>COUNTIF(D:D,D31)/41</f>
-        <v>9.7560975609756101E-2</v>
+        <f>COUNTIF(D:D,D31)/113</f>
+        <v>3.5398230088495575E-2</v>
       </c>
       <c r="M32" s="123">
         <f>COUNTIF(D:D,D31)</f>
@@ -35070,8 +38695,8 @@
         <v>30</v>
       </c>
       <c r="L33" s="5">
-        <f>COUNTIF(D:D,D37)/41</f>
-        <v>7.3170731707317069E-2</v>
+        <f>COUNTIF(D:D,D37)/113</f>
+        <v>2.6548672566371681E-2</v>
       </c>
       <c r="M33" s="123">
         <f>COUNTIF(D:D,D37)</f>
@@ -35106,7 +38731,7 @@
         <v>31</v>
       </c>
       <c r="L34" s="5">
-        <f>COUNTIF(D:D,)/41</f>
+        <f>COUNTIF(D:D,)/113</f>
         <v>0</v>
       </c>
       <c r="M34" s="123">
@@ -35142,7 +38767,7 @@
         <v>32</v>
       </c>
       <c r="L35" s="5">
-        <f>COUNTIF(D:D,)/41</f>
+        <f>COUNTIF(D:D,)/113</f>
         <v>0</v>
       </c>
       <c r="M35" s="123">
@@ -35178,8 +38803,8 @@
         <v>33</v>
       </c>
       <c r="L36" s="5">
-        <f>COUNTIF(D:D,D95)/41</f>
-        <v>4.878048780487805E-2</v>
+        <f>COUNTIF(D:D,D95)/113</f>
+        <v>1.7699115044247787E-2</v>
       </c>
       <c r="M36" s="123">
         <f>COUNTIF(D:D,D95)</f>
@@ -35214,7 +38839,7 @@
         <v>34</v>
       </c>
       <c r="L37" s="5">
-        <f>COUNTIF(D:D,)/41</f>
+        <f>COUNTIF(D:D,)/113</f>
         <v>0</v>
       </c>
       <c r="M37" s="123">

</xml_diff>